<commit_message>
added MixUCB with MetaChoice
</commit_message>
<xml_diff>
--- a/MixUCB_compare.xlsx
+++ b/MixUCB_compare.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,20 +463,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>lin</t>
+          <t>mixI</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6745604419758923</v>
+        <v>0.6777390380663068</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6745604419758923</v>
+        <v>0.6025394045490597</v>
       </c>
     </row>
     <row r="3">
@@ -486,16 +486,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="C3" t="n">
-        <v>204</v>
+        <v>140</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7999366321572099</v>
+        <v>0.3571030328815977</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5924357593044886</v>
+        <v>0.2828485349226024</v>
       </c>
     </row>
     <row r="4">
@@ -505,35 +505,35 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>122</v>
+        <v>64</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5585349757505164</v>
+        <v>0.7353630522180974</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4304655193005528</v>
+        <v>0.7244889849610094</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>mixI</t>
+          <t>mixII</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C5" t="n">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1861957525562919</v>
+        <v>0.2677827191672575</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1484857218000705</v>
+        <v>0.256166505513746</v>
       </c>
     </row>
     <row r="6">
@@ -543,16 +543,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="C6" t="n">
-        <v>115</v>
+        <v>55</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4263582249033749</v>
+        <v>0.6663259101981938</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3503791427847489</v>
+        <v>0.632052519543884</v>
       </c>
     </row>
     <row r="7">
@@ -562,282 +562,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1128763686320173</v>
+        <v>0.5829420827845576</v>
       </c>
       <c r="E7" t="n">
-        <v>0.09202639985047875</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>mixII</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>36</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.7690397250970981</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.7276187482197175</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>mixIII</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C9" t="n">
-        <v>102</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.6834525311984639</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.6680808684645807</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>mixIII</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="C10" t="n">
-        <v>52</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.7142077855234581</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.7075697032660294</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>mixIII</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="n">
-        <v>33</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.7780061003961642</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.7712317856167525</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>lin</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.6727014370065468</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.6727014370065468</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>mixI</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C13" t="n">
-        <v>191</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.6897592225076291</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.2661227141473293</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>mixI</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="C14" t="n">
-        <v>100</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.6437260260710488</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.4616063353252408</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>mixI</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="n">
-        <v>62</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.6299668708888976</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.5154837080223356</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>mixII</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C16" t="n">
-        <v>128</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.6131778140753104</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.3314221645078719</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>mixII</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="C17" t="n">
-        <v>63</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.7472466469740195</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.5835583820302213</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>mixII</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="n">
-        <v>33</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.4218735586574875</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.3815939327539103</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>mixIII</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C19" t="n">
-        <v>109</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.7409670748693153</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.7255834950849719</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>mixIII</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="C20" t="n">
-        <v>55</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0.7897035110139815</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.7921831587273158</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>mixIII</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" t="n">
-        <v>35</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.796345686173467</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.7942632248471423</v>
+        <v>0.5765014363451367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added "compare_params_NOA.py" and fixed problems
</commit_message>
<xml_diff>
--- a/MixUCB_compare.xlsx
+++ b/MixUCB_compare.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>mode</t>
+          <t>feedback_type</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -446,17 +446,32 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>expert_type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>queries</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>avg_auto_reward</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>avg_total_reward</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>cum_auto_rewards_per_time</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>cum_queries_per_time</t>
         </is>
       </c>
     </row>
@@ -469,14 +484,29 @@
       <c r="B2" t="n">
         <v>0.5</v>
       </c>
-      <c r="C2" t="n">
-        <v>200</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>compare</t>
+        </is>
       </c>
       <c r="D2" t="n">
-        <v>0.6777390380663068</v>
+        <v>193</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6025394045490597</v>
+        <v>0.6223834013452407</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.3665924867434461</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7831388714872995), np.float64(0.7546276404200656), np.float64(0.8153135356196316), np.float64(0.8153135356196316), np.float64(0.8153135356196316), np.float64(0.8153135356196316), np.float64(0.8153135356196316), np.float64(0.8153135356196316), np.float64(0.8153135356196316), np.float64(0.8153135356196316), np.float64(0.8153135356196316), np.float64(0.8153135356196316), np.float64(0.8153135356196316), np.float64(0.5865509552783013), np.float64(0.5865509552783011), np.float64(0.5865509552783011), np.float64(0.5865509552783011), np.float64(0.620900418911803), np.float64(0.620900418911803), np.float64(0.6136166811256287), np.float64(0.6136166811256287), np.float64(0.6136166811256287), np.float64(0.6136166811256287), np.float64(0.6136166811256287), np.float64(0.6136166811256287), np.float64(0.6136166811256287), np.float64(0.6136166811256287), np.float64(0.6026109262455187), np.float64(0.6026109262455187), np.float64(0.6026109262455187), np.float64(0.6026109262455187), np.float64(0.6026109262455187), np.float64(0.6026109262455187), np.float64(0.6512702926912947), np.float64(0.6512702926912947), np.float64(0.6512702926912947), np.float64(0.6512702926912947), np.float64(0.6512702926912947), np.float64(0.6512702926912947), np.float64(0.6512702926912947), np.float64(0.6512702926912947), np.float64(0.6288413265897477), np.float64(0.6288413265897477), np.float64(0.4706122219606238), np.float64(0.49413025764125573), np.float64(0.4870674777898505), np.float64(0.4870674777898505), np.float64(0.4870674777898505), np.float64(0.4870674777898505), np.float64(0.4870674777898505), np.float64(0.4870674777898505), np.float64(0.5038977563461294), np.float64(0.5038977563461294), np.float64(0.5038977563461294), np.float64(0.5038977563461293), np.float64(0.5038977563461293), np.float64(0.5038977563461293), np.float64(0.5038977563461293), np.float64(0.5318695815438466), np.float64(0.5318695815438466), np.float64(0.5630620839373601), np.float64(0.5741732054180938), np.float64(0.5741732054180939), np.float64(0.5741732054180939), np.float64(0.5741732054180939), np.float64(0.5741732054180939), np.float64(0.5741732054180939), np.float64(0.5951364250743286), np.float64(0.6062606185197966), np.float64(0.6062606185197966), np.float64(0.6062606185197965), np.float64(0.613549955560711), np.float64(0.6226542358624243), np.float64(0.6226542358624243), np.float64(0.6226542358624243), np.float64(0.6366657421043234), np.float64(0.6366657421043234), np.float64(0.646329733769673), np.float64(0.646329733769673), np.float64(0.661685678732554), np.float64(0.6755166778403213), np.float64(0.6569329077505657), np.float64(0.6569329077505657), np.float64(0.6569329077505657), np.float64(0.6646479979988558), np.float64(0.6646479979988558), np.float64(0.6646479979988558), np.float64(0.6646479979988558), np.float64(0.6646479979988558), np.float64(0.6721365260806911), np.float64(0.6833330068324032), np.float64(0.6818761774065382), np.float64(0.6818761774065382), np.float64(0.6818761774065382), np.float64(0.6818761774065382), np.float64(0.6430290048151963), np.float64(0.6500340086518089), np.float64(0.6609237100605648), np.float64(0.6609237100605648), np.float64(0.6638897972591576), np.float64(0.6638897972591576), np.float64(0.6638897972591576), np.float64(0.6732329690199109), np.float64(0.6722942297133686), np.float64(0.6722942297133686), np.float64(0.6722942297133686), np.float64(0.6807303413807412), np.float64(0.6807303413807412), np.float64(0.6807303413807412), np.float64(0.6807303413807412), np.float64(0.6807303413807413), np.float64(0.6807303413807413), np.float64(0.6450618628115853), np.float64(0.6450618628115853), np.float64(0.6450618628115853), np.float64(0.6492481758187213), np.float64(0.6492481758187213), np.float64(0.6520158685648955), np.float64(0.6461540519634781), np.float64(0.6497573920310857), np.float64(0.6497573920310857), np.float64(0.6497573920310857), np.float64(0.6497573920310857), np.float64(0.6455121611760943), np.float64(0.6455121611760943), np.float64(0.6455121611760943), np.float64(0.6455121611760946), np.float64(0.6525660043170135), np.float64(0.6511101309177225), np.float64(0.6552331804565156), np.float64(0.6474088066394696), np.float64(0.6474088066394696), np.float64(0.6548601212896402), np.float64(0.6489689182074035), np.float64(0.6553749056771419), np.float64(0.6553749056771419), np.float64(0.6306837034120101), np.float64(0.6306837034120101), np.float64(0.6306837034120101), np.float64(0.6306837034120101), np.float64(0.6286855879697151), np.float64(0.6298159425841038), np.float64(0.6298159425841038), np.float64(0.6367210266863652), np.float64(0.632843660656728), np.float64(0.6337682678152537), np.float64(0.6393596370164872), np.float64(0.6393596370164872), np.float64(0.6393596370164872), np.float64(0.62395680577423), np.float64(0.6288489122413725), np.float64(0.6288489122413725), np.float64(0.6288489122413725), np.float64(0.6288489122413725), np.float64(0.6099604141003508), np.float64(0.6099604141003508), np.float64(0.6099604141003508), np.float64(0.6124678956785456), np.float64(0.6124678956785456), np.float64(0.6157064808215025), np.float64(0.6206647649167203), np.float64(0.6206647649167203), np.float64(0.6206647649167203), np.float64(0.6253323090117645), np.float64(0.6291202367673221), np.float64(0.6291202367673221), np.float64(0.6343627844851953), np.float64(0.6343627844851953), np.float64(0.6343627844851953), np.float64(0.6387140959293546), np.float64(0.6293038431277163), np.float64(0.6346151763509055), np.float64(0.6346151763509055), np.float64(0.6226839933693584), np.float64(0.6221727245007052), np.float64(0.627158515843169), np.float64(0.627158515843169), np.float64(0.627158515843169), np.float64(0.627158515843169), np.float64(0.627158515843169), np.float64(0.627158515843169), np.float64(0.627158515843169), np.float64(0.627158515843169), np.float64(0.6164022207201239), np.float64(0.6191868069479227), np.float64(0.6195438512464112), np.float64(0.6195438512464112), np.float64(0.6222432378655853), np.float64(0.6222432378655853), np.float64(0.6241933245702842), np.float64(0.6241933245702842), np.float64(0.6241933245702842), np.float64(0.6241933245702842), np.float64(0.6285175579893464), np.float64(0.6278772771168258), np.float64(0.6278772771168258), np.float64(0.6278772771168258), np.float64(0.632545983203708), np.float64(0.632545983203708), np.float64(0.632545983203708), np.float64(0.6365574167300272), np.float64(0.6365574167300272), np.float64(0.6365574167300272), np.float64(0.6409942167909786), np.float64(0.6409942167909786), np.float64(0.6441181349069165), np.float64(0.6441181349069166), np.float64(0.6441181349069166), np.float64(0.6393344610388343), np.float64(0.6393344610388343), np.float64(0.6347948802488508), np.float64(0.6347948802488508), np.float64(0.6347948802488508), np.float64(0.62069458111848), np.float64(0.6206945811184799), np.float64(0.6206945811184799), np.float64(0.6206945811184799), np.float64(0.6206945811184799), np.float64(0.6161841343882334), np.float64(0.6201721469997099), np.float64(0.6234333032109584), np.float64(0.6103295742129442), np.float64(0.6139082821212398), np.float64(0.6137703118973943), np.float64(0.6137703118973943), np.float64(0.6137703118973943), np.float64(0.6178538105324921), np.float64(0.6178538105324921), np.float64(0.6186234012322078), np.float64(0.6183154619062271), np.float64(0.6216372577627474), np.float64(0.6223900272306456), np.float64(0.6223900272306456), np.float64(0.6240626997748497), np.float64(0.6240626997748497), np.float64(0.6240626997748497), np.float64(0.6252669683219003), np.float64(0.6286340624308826), np.float64(0.6285956825933553), np.float64(0.6285956825933553), np.float64(0.6285956825933553), np.float64(0.6289756844881899), np.float64(0.6289756844881899), np.float64(0.6289756844881899), np.float64(0.6325452801153598), np.float64(0.6333472345140241), np.float64(0.6312218344247225), np.float64(0.6301944548957116), np.float64(0.6254277775646412), np.float64(0.6254277775646412)]</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 49, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 59, 60, 61, 62, 62, 63, 63, 64, 65, 66, 67, 68, 69, 70, 70, 71, 72, 73, 74, 75, 75, 76, 77, 78, 79, 80, 81, 82, 82, 83, 83, 83, 83, 84, 85, 86, 87, 88, 88, 89, 90, 91, 92, 93, 94, 94, 95, 95, 95, 96, 97, 98, 99, 100, 100, 100, 101, 102, 102, 102, 103, 104, 104, 105, 105, 106, 106, 106, 106, 107, 108, 108, 109, 110, 111, 112, 112, 112, 112, 113, 114, 115, 115, 115, 115, 116, 116, 117, 118, 118, 118, 119, 120, 120, 121, 122, 123, 124, 125, 125, 126, 127, 127, 128, 128, 128, 128, 129, 130, 131, 131, 132, 133, 134, 134, 134, 134, 134, 135, 135, 135, 135, 136, 136, 137, 138, 139, 139, 139, 140, 140, 140, 140, 140, 141, 142, 142, 142, 143, 144, 145, 145, 146, 147, 147, 148, 148, 148, 149, 150, 150, 150, 151, 151, 152, 153, 153, 153, 153, 154, 154, 154, 154, 155, 156, 157, 158, 159, 160, 161, 161, 161, 161, 162, 162, 163, 163, 164, 165, 166, 166, 166, 167, 168, 168, 169, 170, 170, 171, 172, 172, 173, 173, 174, 175, 175, 176, 176, 177, 178, 178, 179, 180, 181, 182, 182, 182, 182, 182, 182, 182, 183, 184, 184, 185, 185, 185, 185, 185, 186, 186, 187, 188, 188, 188, 188, 189, 190, 190, 191, 192, 192, 192, 192, 192, 192, 193]</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -488,14 +518,29 @@
       <c r="B3" t="n">
         <v>0.75</v>
       </c>
-      <c r="C3" t="n">
-        <v>140</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>compare</t>
+        </is>
       </c>
       <c r="D3" t="n">
-        <v>0.3571030328815977</v>
+        <v>116</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2828485349226024</v>
+        <v>0.4035875147295997</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.286246546450096</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(-0.35130852003943147), np.float64(-0.35130852003943147), np.float64(-0.35130852003943147), np.float64(-0.35130852003943147), np.float64(-0.35130852003943147), np.float64(-0.35130852003943147), np.float64(-0.35130852003943147), np.float64(-0.46194748974132266), np.float64(-0.46194748974132266), np.float64(-0.46194748974132266), np.float64(-0.46194748974132266), np.float64(-0.46194748974132266), np.float64(-0.46194748974132266), np.float64(-0.46194748974132266), np.float64(-0.5348720775302143), np.float64(-0.5348720775302143), np.float64(-0.5348720775302143), np.float64(-0.5348720775302143), np.float64(-0.42595368203187517), np.float64(-0.26977777083546084), np.float64(-0.26977777083546084), np.float64(-0.26977777083546084), np.float64(-0.26977777083546084), np.float64(-0.20535251338120133), np.float64(-0.07503449321703319), np.float64(-0.1504048988445998), np.float64(-0.1504048988445998), np.float64(-0.1504048988445998), np.float64(-0.11635698117886578), np.float64(-0.16392355588902835), np.float64(-0.16392355588902835), np.float64(-0.16392355588902835), np.float64(-0.16392355588902835), np.float64(-0.16392355588902835), np.float64(-0.08748991538043455), np.float64(-0.08748991538043455), np.float64(-0.048135055236828504), np.float64(0.0009678190955239457), np.float64(0.0009678190955239457), np.float64(0.0009678190955239457), np.float64(0.0009678190955239457), np.float64(0.0009678190955239457), np.float64(0.0009678190955239457), np.float64(0.0009678190955239457), np.float64(0.03057817607145814), np.float64(0.03057817607145814), np.float64(0.04986129421947579), np.float64(0.04986129421947579), np.float64(-0.005026688614439459), np.float64(-0.005026688614439459), np.float64(-0.005026688614439445), np.float64(0.015855163187531794), np.float64(0.015855163187531794), np.float64(0.015855163187531794), np.float64(0.015855163187531794), np.float64(-0.03997951830034629), np.float64(-0.03997951830034629), np.float64(0.004769889038303232), np.float64(-0.01138559044031624), np.float64(-0.01138559044031624), np.float64(-0.01138559044031624), np.float64(-0.0023850197146310145), np.float64(-0.0023850197146310145), np.float64(-0.0023850197146310145), np.float64(-0.04216358965592592), np.float64(0.002041490626552789), np.float64(0.0020414906265527936), np.float64(0.023185810511337845), np.float64(0.06040708390701784), np.float64(0.06040708390701784), np.float64(0.06040708390701784), np.float64(0.06040708390701784), np.float64(0.07324556285517889), np.float64(0.07324556285517889), np.float64(0.07324556285517889), np.float64(0.10665499074995619), np.float64(0.13855908279592422), np.float64(0.13855908279592422), np.float64(0.13855908279592422), np.float64(0.16823882732697368), np.float64(0.13585905220429276), np.float64(0.15877223951445546), np.float64(0.15877223951445546), np.float64(0.16157214740969206), np.float64(0.18646791938167095), np.float64(0.18646791938167095), np.float64(0.20913566546647472), np.float64(0.20913566546647472), np.float64(0.22951245166701298), np.float64(0.22951245166701298), np.float64(0.25017791172966447), np.float64(0.26580040281420214), np.float64(0.26580040281420214), np.float64(0.26580040281420214), np.float64(0.26580040281420214), np.float64(0.28480088424091526), np.float64(0.28480088424091526), np.float64(0.2961442576573273), np.float64(0.290804813735565), np.float64(0.29080481373556494), np.float64(0.29080481373556494), np.float64(0.29080481373556494), np.float64(0.305750789426257), np.float64(0.2912825701835691), np.float64(0.3057060776880059), np.float64(0.3057060776880059), np.float64(0.29979491347125536), np.float64(0.29979491347125536), np.float64(0.31268323898325867), np.float64(0.31690144318944563), np.float64(0.31690144318944563), np.float64(0.32406067793086357), np.float64(0.332372102133077), np.float64(0.34400639461629945), np.float64(0.35694301735164985), np.float64(0.34800101512860543), np.float64(0.360105478448005), np.float64(0.36734302055441503), np.float64(0.36734302055441503), np.float64(0.3790542083423495), np.float64(0.37501070351574206), np.float64(0.38438753675427634), np.float64(0.3951622223411094), np.float64(0.3951622223411094), np.float64(0.405537818407235), np.float64(0.41472454450202756), np.float64(0.4035504785790666), np.float64(0.4035504785790666), np.float64(0.4035504785790666), np.float64(0.401965924597668), np.float64(0.401965924597668), np.float64(0.4062443179135344), np.float64(0.4113106266262235), np.float64(0.40477458799790367), np.float64(0.4090648858521441), np.float64(0.40607485332622567), np.float64(0.4127438255850052), np.float64(0.41956034227502553), np.float64(0.4087734357612582), np.float64(0.40403957335613355), np.float64(0.40403957335613355), np.float64(0.4113928061583642), np.float64(0.41953872903284317), np.float64(0.42704360868566493), np.float64(0.4344039234659311), np.float64(0.4404864182685698), np.float64(0.44304277862889074), np.float64(0.44606921804157085), np.float64(0.4466748907429717), np.float64(0.44803720831639704), np.float64(0.4409565930666847), np.float64(0.43822052471314055), np.float64(0.43822052471314055), np.float64(0.4223935393521122), np.float64(0.42651311211819537), np.float64(0.42651311211819537), np.float64(0.4213519175700761), np.float64(0.4213519175700761), np.float64(0.41684834479881866), np.float64(0.4225673205381406), np.float64(0.4285749591819028), np.float64(0.4285749591819028), np.float64(0.43445237756526695), np.float64(0.42971633068041903), np.float64(0.42508389926301526), np.float64(0.4308949918944889), np.float64(0.4342632284634491), np.float64(0.43964722379982174), np.float64(0.44131294125418985), np.float64(0.42904596915908244), np.float64(0.42189916167444563), np.float64(0.4072656469874005), np.float64(0.4072656469874005), np.float64(0.4089026604037647), np.float64(0.40493174131261434), np.float64(0.39991329237062095), np.float64(0.4029883616889807), np.float64(0.405132997038712), np.float64(0.40513299703871186), np.float64(0.40985913304725546), np.float64(0.4064739142508723), np.float64(0.4064739142508723), np.float64(0.41145649757949043), np.float64(0.4167335512598061), np.float64(0.4134208748885982), np.float64(0.418641690834682), np.float64(0.41864169083468206), np.float64(0.41191724115069706), np.float64(0.4063782237814735), np.float64(0.40697866322432913), np.float64(0.40713570704718816), np.float64(0.41237868482398315), np.float64(0.40010784818300454), np.float64(0.395232868279523), np.float64(0.395232868279523), np.float64(0.3949872355071683), np.float64(0.3944834932719574), np.float64(0.3963260972049904), np.float64(0.4004980573558568), np.float64(0.40521888031901093), np.float64(0.40521888031901093), np.float64(0.39959277262145615), np.float64(0.40420271032432264), np.float64(0.40001607989366544), np.float64(0.4020637131335422), np.float64(0.3973649341618218), np.float64(0.39788710818912676), np.float64(0.40220958386769284), np.float64(0.4053582096151457), np.float64(0.4076515930804878), np.float64(0.40886828094332756), np.float64(0.40886828094332756), np.float64(0.4129465866152036), np.float64(0.4129465866152036), np.float64(0.4166734695161628), np.float64(0.4151206946595701), np.float64(0.4054956349119342), np.float64(0.4070256572176283), np.float64(0.4070256572176284), np.float64(0.41118918625333667), np.float64(0.414697653973032), np.float64(0.4174536780268349), np.float64(0.41542762612098133), np.float64(0.4191851389696681), np.float64(0.42183213253887847), np.float64(0.42183213253887847), np.float64(0.4231865154148733), np.float64(0.42483510973739447), np.float64(0.4284635729593347), np.float64(0.43240363564303635), np.float64(0.4281147762799031), np.float64(0.42962793765549784), np.float64(0.43228063878659856), np.float64(0.43424486511970406), np.float64(0.42653200243105793), np.float64(0.4279253384984045), np.float64(0.42518117404283945), np.float64(0.42139190760614653), np.float64(0.4248192407078465), np.float64(0.4275004417867159), np.float64(0.4237434605749894), np.float64(0.42647613891207065), np.float64(0.4224546716410187), np.float64(0.4242091304148893), np.float64(0.4158022616622956), np.float64(0.4117845048585041), np.float64(0.4153429106943469), np.float64(0.4115309845191524), np.float64(0.4107446810864258), np.float64(0.4141724795722769), np.float64(0.41154961097950915), np.float64(0.4106116584609929), np.float64(0.4106116584609929), np.float64(0.4127856531259733), np.float64(0.4132071648326535), np.float64(0.4057560766153126), np.float64(0.40530297555694506), np.float64(0.4076468609891587), np.float64(0.4109947432158722), np.float64(0.4102096024857035), np.float64(0.41357173726934043), np.float64(0.4150192811179739), np.float64(0.4072435050240219), np.float64(0.40542660647525997), np.float64(0.40743865373884447), np.float64(0.41019263413875723), np.float64(0.4029298749014856), np.float64(0.39864868203305925), np.float64(0.4017624755132658), np.float64(0.4017624755132658)]</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 29, 30, 31, 32, 33, 34, 35, 35, 36, 37, 38, 39, 40, 41, 41, 42, 43, 44, 44, 44, 45, 46, 47, 47, 47, 47, 48, 49, 49, 49, 50, 51, 52, 53, 53, 54, 54, 54, 55, 56, 57, 58, 59, 60, 60, 61, 61, 62, 62, 63, 64, 64, 65, 66, 67, 67, 68, 68, 68, 69, 70, 70, 71, 72, 72, 72, 73, 73, 73, 74, 75, 76, 76, 77, 78, 78, 78, 79, 80, 80, 80, 80, 81, 81, 81, 82, 82, 83, 83, 84, 84, 84, 85, 86, 87, 87, 88, 88, 88, 89, 90, 91, 91, 91, 91, 92, 92, 93, 93, 93, 94, 94, 94, 94, 94, 94, 94, 94, 95, 95, 95, 95, 95, 96, 96, 96, 96, 97, 98, 98, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 100, 100, 100, 100, 100, 100, 100, 100, 100, 100, 100, 100, 101, 101, 101, 102, 102, 103, 103, 103, 103, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 105, 105, 105, 105, 105, 105, 106, 106, 106, 107, 107, 107, 107, 107, 108, 108, 108, 108, 108, 108, 108, 108, 109, 109, 109, 109, 109, 109, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 111, 111, 112, 112, 112, 112, 112, 113, 113, 113, 113, 113, 113, 113, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 115, 115, 115, 115, 115, 115, 115, 115, 115, 115, 115, 115, 115, 115, 115, 115, 115, 116]</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -507,14 +552,29 @@
       <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" t="n">
-        <v>64</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>compare</t>
+        </is>
       </c>
       <c r="D4" t="n">
-        <v>0.7353630522180974</v>
+        <v>63</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7244889849610094</v>
+        <v>0.6840368771007134</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.5484060564575992</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(-0.9515263840404017), np.float64(-0.9515263840404017), np.float64(-0.9515263840404017), np.float64(-0.9515263840404017), np.float64(-0.9515263840404017), np.float64(-0.967310049106181), np.float64(-0.967310049106181), np.float64(-0.967310049106181), np.float64(-0.967310049106181), np.float64(-0.967310049106181), np.float64(-0.967310049106181), np.float64(-0.967310049106181), np.float64(-0.967310049106181), np.float64(-0.967310049106181), np.float64(-0.967310049106181), np.float64(-0.9718898071466263), np.float64(-0.8477529818148306), np.float64(-0.7915761142952118), np.float64(-0.7915761142952118), np.float64(-0.7915761142952118), np.float64(-0.7915761142952118), np.float64(-0.5737902972560098), np.float64(-0.5737902972560098), np.float64(-0.3750401555266828), np.float64(-0.3750401555266828), np.float64(-0.3750401555266828), np.float64(-0.3750401555266828), np.float64(-0.3750401555266828), np.float64(-0.21356396569396308), np.float64(-0.21356396569396313), np.float64(-0.21356396569396313), np.float64(-0.21356396569396313), np.float64(-0.21356396569396313), np.float64(-0.0927271178167872), np.float64(-0.0927271178167872), np.float64(-0.0927271178167872), np.float64(0.016515795215280783), np.float64(0.10444387470081012), np.float64(0.12712620431038665), np.float64(0.16440929194380383), np.float64(0.2027120563152443), np.float64(0.24758414646836557), np.float64(0.24758414646836557), np.float64(0.2686610313624564), np.float64(0.2686610313624564), np.float64(0.2686610313624564), np.float64(0.2686610313624564), np.float64(0.2800638718379476), np.float64(0.2800638718379476), np.float64(0.2800638718379476), np.float64(0.3095224235667802), np.float64(0.3013819982398632), np.float64(0.3363089492124097), np.float64(0.33630894921240967), np.float64(0.361448773075369), np.float64(0.3881392418593515), np.float64(0.4143922660421625), np.float64(0.4387650045278893), np.float64(0.46121216825326283), np.float64(0.4493428514797475), np.float64(0.44916250424249093), np.float64(0.4491625042424908), np.float64(0.45605100436667717), np.float64(0.45605100436667717), np.float64(0.46110962815736223), np.float64(0.4583526911445158), np.float64(0.47510119485207875), np.float64(0.48287885556554505), np.float64(0.48957119515375186), np.float64(0.501001336329832), np.float64(0.5104051013492444), np.float64(0.5118604975836948), np.float64(0.5118604975836948), np.float64(0.5175982988985987), np.float64(0.5175982988985987), np.float64(0.5273468015734042), np.float64(0.5254077931937404), np.float64(0.5332556061439107), np.float64(0.5419331136453787), np.float64(0.552391775639105), np.float64(0.5529009156717254), np.float64(0.5529009156717254), np.float64(0.5539066633360309), np.float64(0.5611264084034762), np.float64(0.5594601685013711), np.float64(0.565181512775867), np.float64(0.5694980994530282), np.float64(0.5646988992262516), np.float64(0.573402725398774), np.float64(0.5799874590783738), np.float64(0.5799874590783738), np.float64(0.5880055398453985), np.float64(0.5823789355111106), np.float64(0.5851130131106304), np.float64(0.5799323842543027), np.float64(0.5873817878708307), np.float64(0.5925796928066851), np.float64(0.5885334101978803), np.float64(0.5954419943236835), np.float64(0.600663203162626), np.float64(0.5930663806946284), np.float64(0.5940730648831437), np.float64(0.5984191748030385), np.float64(0.6029139825546974), np.float64(0.6078342254828), np.float64(0.6136374458640524), np.float64(0.6085477594015081), np.float64(0.6046344359816224), np.float64(0.6046344359816224), np.float64(0.6019511449948667), np.float64(0.599807495886145), np.float64(0.5943317280155422), np.float64(0.5989344840439386), np.float64(0.6042303908683868), np.float64(0.6081957735584449), np.float64(0.6106681450776902), np.float64(0.6058597512469293), np.float64(0.6088980879083905), np.float64(0.6099108188846278), np.float64(0.6123750723649283), np.float64(0.6154712495267665), np.float64(0.6199103928653003), np.float64(0.6242260783906292), np.float64(0.6264910733853082), np.float64(0.6308049248804136), np.float64(0.6284323159763826), np.float64(0.6245222347402686), np.float64(0.6285486300941621), np.float64(0.6327608958671656), np.float64(0.6276040157305613), np.float64(0.6259129492584944), np.float64(0.6300237632786876), np.float64(0.6272733698688527), np.float64(0.6284182969767355), np.float64(0.6273958343361761), np.float64(0.6291250900916905), np.float64(0.630679980479294), np.float64(0.6324453639138595), np.float64(0.6342087286483904), np.float64(0.6378281156009792), np.float64(0.641264631766132), np.float64(0.6432089213929091), np.float64(0.6455695514934994), np.float64(0.6417959503486718), np.float64(0.642213787526617), np.float64(0.6417206024510874), np.float64(0.6434225628686859), np.float64(0.6466906369998409), np.float64(0.6466906369998409), np.float64(0.6437561376511894), np.float64(0.6443502432603109), np.float64(0.6443502432603109), np.float64(0.6462445651883794), np.float64(0.6471529108165374), np.float64(0.6471529108165374), np.float64(0.6469279078486456), np.float64(0.6473611459624793), np.float64(0.647861731839477), np.float64(0.6488705453377196), np.float64(0.6468330521626805), np.float64(0.6418784630248631), np.float64(0.6389662302609483), np.float64(0.6412960019716445), np.float64(0.6380362227815738), np.float64(0.63508053030493), np.float64(0.6354565656195045), np.float64(0.6382338435875645), np.float64(0.6372092757391004), np.float64(0.6390930377262541), np.float64(0.6369213635664865), np.float64(0.6396188242284323), np.float64(0.6397297730433893), np.float64(0.6422789871073095), np.float64(0.6432837338492675), np.float64(0.6391967722876181), np.float64(0.6415705788583916), np.float64(0.644135724362479), np.float64(0.6392486325912143), np.float64(0.6357322015216861), np.float64(0.6384104159871137), np.float64(0.6398051390180418), np.float64(0.6395831971115866), np.float64(0.6421625306460154), np.float64(0.6435116762450926), np.float64(0.6441684300843158), np.float64(0.642760477694671), np.float64(0.6450004393129197), np.float64(0.645615860158191), np.float64(0.6465390424004819), np.float64(0.6468486840971979), np.float64(0.6440551603885806), np.float64(0.6411447914908147), np.float64(0.6416168935560492), np.float64(0.6423571810039067), np.float64(0.6441730676594586), np.float64(0.6440448506269805), np.float64(0.6450742438094054), np.float64(0.646734348372964), np.float64(0.6490113366212903), np.float64(0.6490113366212903), np.float64(0.6505287100538611), np.float64(0.6504096695633207), np.float64(0.6513092080161912), np.float64(0.6530247066925237), np.float64(0.6551924719389568), np.float64(0.6529937909443998), np.float64(0.6545862235794218), np.float64(0.6554176379438938), np.float64(0.6575138557389099), np.float64(0.6578738498311636), np.float64(0.6576992782251576), np.float64(0.6591798639821115), np.float64(0.6604630229502169), np.float64(0.6601404335427771), np.float64(0.6614354806193514), np.float64(0.6624517973293607), np.float64(0.6597026604472248), np.float64(0.6601843578673394), np.float64(0.660661655133105), np.float64(0.6617689821980689), np.float64(0.6635598747872095), np.float64(0.6651179927724379), np.float64(0.6664346199749225), np.float64(0.6682978179203546), np.float64(0.6646009817507395), np.float64(0.6644841500484987), np.float64(0.6655473901921539), np.float64(0.66326024782034), np.float64(0.6608340327129134), np.float64(0.660417636763315), np.float64(0.661492043845698), np.float64(0.6600402095857253), np.float64(0.6592218725463623), np.float64(0.6576882330109856), np.float64(0.658986189624884), np.float64(0.6586786452957857), np.float64(0.6603281403691066), np.float64(0.6585080730798151), np.float64(0.6591465648317374), np.float64(0.6607371034632059), np.float64(0.6588412110844203), np.float64(0.6592270519738654), np.float64(0.6599810620510408), np.float64(0.6616795502273302), np.float64(0.6612237457860983), np.float64(0.662643228821768), np.float64(0.6620978712184473), np.float64(0.6631757460332641), np.float64(0.6644830124810192), np.float64(0.6654424961620323), np.float64(0.6668518368366937), np.float64(0.6649287296837817), np.float64(0.6636059030773658), np.float64(0.6619703928494045), np.float64(0.6635170728709389), np.float64(0.6626187112728018), np.float64(0.6641730408404192), np.float64(0.6639464978732612), np.float64(0.6615486004924332), np.float64(0.6629078468253925), np.float64(0.6644081061195151), np.float64(0.6659360092198281), np.float64(0.6670049231263209), np.float64(0.6685096328031003), np.float64(0.6696547049136572), np.float64(0.6700991541718353), np.float64(0.6707422840044079), np.float64(0.6721287964932608), np.float64(0.6733831029525827), np.float64(0.6744589178392724), np.float64(0.6733412440053583), np.float64(0.674714117070108), np.float64(0.6754419950772202), np.float64(0.6766477491970581), np.float64(0.6780431853735078), np.float64(0.6794103458526435), np.float64(0.6802303988350203), np.float64(0.6808217714476533), np.float64(0.6821262787030754), np.float64(0.6834013017816164), np.float64(0.683748483134938)]</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 18, 19, 20, 21, 22, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 31, 31, 31, 32, 33, 34, 34, 35, 35, 36, 37, 38, 39, 39, 40, 41, 42, 43, 43, 44, 45, 45, 45, 45, 45, 45, 45, 46, 46, 47, 48, 49, 49, 50, 51, 51, 51, 51, 52, 52, 52, 52, 52, 52, 52, 52, 53, 53, 54, 54, 54, 54, 54, 54, 54, 54, 54, 55, 55, 56, 56, 56, 56, 56, 56, 56, 57, 57, 57, 57, 57, 57, 57, 57, 57, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 60, 60, 60, 61, 61, 61, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63]</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -526,14 +586,29 @@
       <c r="B5" t="n">
         <v>0.5</v>
       </c>
-      <c r="C5" t="n">
-        <v>128</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>compare</t>
+        </is>
       </c>
       <c r="D5" t="n">
-        <v>0.2677827191672575</v>
+        <v>122</v>
       </c>
       <c r="E5" t="n">
-        <v>0.256166505513746</v>
+        <v>0.7833617663573624</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.5990325620402617</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.9829289343267616), np.float64(0.9725689466532621), np.float64(0.9725689466532621), np.float64(0.9725689466532621), np.float64(0.9725689466532621), np.float64(0.9725689466532621), np.float64(0.9725689466532621), np.float64(0.893389294916534), np.float64(0.9125010376615678), np.float64(0.9125010376615678), np.float64(0.751381306699056), np.float64(0.751381306699056), np.float64(0.751381306699056), np.float64(0.751381306699056), np.float64(0.751381306699056), np.float64(0.751381306699056), np.float64(0.751381306699056), np.float64(0.7926549758052367), np.float64(0.7926549758052367), np.float64(0.7926549758052367), np.float64(0.7926549758052367), np.float64(0.8205922171956767), np.float64(0.7370906276335485), np.float64(0.7265865976349372), np.float64(0.7265865976349372), np.float64(0.7265865976349372), np.float64(0.7265865976349372), np.float64(0.7390981411697763), np.float64(0.7000594218091291), np.float64(0.7000594218091291), np.float64(0.700059421809129), np.float64(0.6619288094616189), np.float64(0.6619288094616189), np.float64(0.6806412089006272), np.float64(0.6806412089006272), np.float64(0.6756688190560741), np.float64(0.6756688190560741), np.float64(0.6756688190560741), np.float64(0.6756688190560741), np.float64(0.6756688190560741), np.float64(0.6962495028907353), np.float64(0.6962495028907353), np.float64(0.7068011534999212), np.float64(0.6957152347214468), np.float64(0.6977633356522754), np.float64(0.6977633356522754), np.float64(0.7114624176418366), np.float64(0.7248835453373641), np.float64(0.72997789443565), np.float64(0.712856802386975), np.float64(0.712856802386975), np.float64(0.693906270830589), np.float64(0.693906270830589), np.float64(0.693906270830589), np.float64(0.6939062708305891), np.float64(0.7015270893414475), np.float64(0.7015270893414475), np.float64(0.6961865428296263), np.float64(0.7006905010745892), np.float64(0.7099423359923899), np.float64(0.7174510738592625), np.float64(0.7174510738592625), np.float64(0.7261680372197742), np.float64(0.7261680372197742), np.float64(0.7261680372197742), np.float64(0.7261680372197742), np.float64(0.734820883982305), np.float64(0.734820883982305), np.float64(0.7383266103721934), np.float64(0.7464059102763918), np.float64(0.7464059102763918), np.float64(0.7464059102763918), np.float64(0.7352440837785691), np.float64(0.7429787006674788), np.float64(0.7429787006674788), np.float64(0.7450911605597581), np.float64(0.7450911605597581), np.float64(0.7512461057987053), np.float64(0.7512461057987053), np.float64(0.7512461057987053), np.float64(0.7576324699345232), np.float64(0.7583283830721582), np.float64(0.756724199469146), np.float64(0.756724199469146), np.float64(0.756724199469146), np.float64(0.7581438340908624), np.float64(0.7581438340908624), np.float64(0.7581438340908624), np.float64(0.7634937783906093), np.float64(0.7634937783906093), np.float64(0.7662362328862551), np.float64(0.7662362328862551), np.float64(0.7601883287671461), np.float64(0.7614464724257882), np.float64(0.7614464724257884), np.float64(0.7614464724257884), np.float64(0.7621446420129876), np.float64(0.7627201882278107), np.float64(0.7565944557553889), np.float64(0.7551843201647562), np.float64(0.7551843201647562), np.float64(0.7551843201647562), np.float64(0.755184320164756), np.float64(0.7509080172000651), np.float64(0.7509080172000651), np.float64(0.7509080172000651), np.float64(0.7509080172000651), np.float64(0.7509080172000651), np.float64(0.751812023773082), np.float64(0.751812023773082), np.float64(0.7564829964214396), np.float64(0.7564829964214396), np.float64(0.7598250097392423), np.float64(0.7641006256163821), np.float64(0.7641006256163821), np.float64(0.7645896255928201), np.float64(0.7591900098221687), np.float64(0.7599362580612505), np.float64(0.7627786178387005), np.float64(0.7627786178387005), np.float64(0.7627786178387005), np.float64(0.7653842554450654), np.float64(0.7693543088750129), np.float64(0.7693543088750129), np.float64(0.765136741788448), np.float64(0.7683894513305071), np.float64(0.7683894513305072), np.float64(0.7683894513305072), np.float64(0.7720334962291779), np.float64(0.7677995056582845), np.float64(0.7702827667394402), np.float64(0.7663034139382662), np.float64(0.7650048849785118), np.float64(0.7650048849785118), np.float64(0.7650048849785119), np.float64(0.7683718894997883), np.float64(0.7683718894997883), np.float64(0.7683718894997883), np.float64(0.7683718894997883), np.float64(0.7687412422502049), np.float64(0.7707050158777141), np.float64(0.7688546606298069), np.float64(0.7688546606298069), np.float64(0.7720977047446063), np.float64(0.7750727221552329), np.float64(0.7750727221552329), np.float64(0.7750727221552329), np.float64(0.7697331386439362), np.float64(0.7690833227089077), np.float64(0.772149017207896), np.float64(0.7750191310732925), np.float64(0.7774896303254833), np.float64(0.7794412494348367), np.float64(0.781240558031634), np.float64(0.781240558031634), np.float64(0.7789428110662877), np.float64(0.7789428110662877), np.float64(0.7788552851851633), np.float64(0.7767135890736616), np.float64(0.7767135890736616), np.float64(0.7741947166879956), np.float64(0.7762716907362446), np.float64(0.775745356870854), np.float64(0.7738186297436591), np.float64(0.7738186297436591), np.float64(0.7733546676967941), np.float64(0.7759082637424544), np.float64(0.7780746100234462), np.float64(0.7801512234583237), np.float64(0.7823367938514738), np.float64(0.7846974294110803), np.float64(0.7859470827554746), np.float64(0.7829463435690005), np.float64(0.7829463435690005), np.float64(0.7844363128643459), np.float64(0.7858766685461892), np.float64(0.7858766685461892), np.float64(0.7869548351605622), np.float64(0.7888739026005384), np.float64(0.7888451436628916), np.float64(0.7831734921731092), np.float64(0.7849849945353614), np.float64(0.7849849945353613), np.float64(0.7849849945353613), np.float64(0.7868015784634186), np.float64(0.7848335683754473), np.float64(0.7867934944672973), np.float64(0.7883862005178931), np.float64(0.7844076343171249), np.float64(0.7837220439571742), np.float64(0.7837352915063541), np.float64(0.7813952016552388), np.float64(0.7826139811042563), np.float64(0.7826139811042563), np.float64(0.7839771863144576), np.float64(0.7846693774296025), np.float64(0.7846693774296025), np.float64(0.7863917541354859), np.float64(0.7878234783765342), np.float64(0.7879673942018999), np.float64(0.7878236467918887), np.float64(0.7878236467918887), np.float64(0.7874760879675037), np.float64(0.7869686337979378), np.float64(0.7865153486761729), np.float64(0.7855267055225963), np.float64(0.7865150222357989), np.float64(0.7880489373103138), np.float64(0.7841147639998755), np.float64(0.7799459090528051), np.float64(0.7809732623674245), np.float64(0.7813593215465735), np.float64(0.7827997088836959), np.float64(0.7827997088836959), np.float64(0.7843841264763936), np.float64(0.7851110251910897), np.float64(0.7823945837735509), np.float64(0.7823945837735509), np.float64(0.7823945837735509), np.float64(0.7823945837735509), np.float64(0.783994563851741), np.float64(0.7811995889603613), np.float64(0.7811995889603613), np.float64(0.7817344515099905), np.float64(0.7798318594801832), np.float64(0.7808763699625241), np.float64(0.7808763699625241), np.float64(0.7824875727602231), np.float64(0.7824875727602231), np.float64(0.7838969516373829), np.float64(0.7811569222138737), np.float64(0.7784424087747487), np.float64(0.779790853221019), np.float64(0.7780517272428525), np.float64(0.7790862371116677), np.float64(0.7792725475764078), np.float64(0.7799699166756119), np.float64(0.7809864204596795), np.float64(0.781682687074421), np.float64(0.7812622015452798), np.float64(0.7827019602585337), np.float64(0.783865159849739), np.float64(0.7846426472848997), np.float64(0.7860681556705889), np.float64(0.7863619655463174), np.float64(0.7863619655463174), np.float64(0.7877575339495888), np.float64(0.7888657238849296), np.float64(0.7902253081462471), np.float64(0.7888420833383936), np.float64(0.7886279141638354), np.float64(0.78887830020841), np.float64(0.78887830020841), np.float64(0.7893833543380286), np.float64(0.7906726654661529), np.float64(0.791707648331618), np.float64(0.7923401462577717), np.float64(0.7934762889673761), np.float64(0.7939338084642548), np.float64(0.7949470359149189), np.float64(0.7939840347766572), np.float64(0.7934260096649415), np.float64(0.7910744887818796), np.float64(0.7893082204295115), np.float64(0.7885995652948038), np.float64(0.7885995652948038), np.float64(0.7857922546549356), np.float64(0.7869724185707995), np.float64(0.787400582590221), np.float64(0.787400582590221), np.float64(0.7848047412283586), np.float64(0.7860177440777738), np.float64(0.7840288908741422), np.float64(0.7824039536935226)]</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 25, 25, 26, 27, 28, 29, 30, 30, 30, 31, 31, 32, 33, 34, 35, 36, 37, 37, 38, 39, 40, 40, 40, 40, 41, 42, 43, 43, 43, 44, 45, 45, 46, 46, 47, 47, 48, 49, 50, 51, 51, 52, 52, 52, 52, 53, 53, 53, 53, 53, 54, 54, 55, 56, 57, 57, 58, 58, 58, 58, 58, 59, 59, 60, 61, 62, 62, 63, 63, 63, 64, 65, 65, 65, 66, 66, 67, 67, 68, 69, 69, 69, 69, 70, 71, 71, 72, 73, 73, 74, 74, 75, 75, 75, 76, 77, 77, 77, 77, 77, 78, 79, 80, 80, 81, 82, 83, 84, 84, 85, 85, 86, 86, 86, 87, 87, 87, 87, 87, 88, 89, 89, 89, 90, 90, 90, 91, 92, 92, 92, 92, 92, 92, 93, 94, 94, 95, 96, 97, 97, 97, 97, 98, 98, 98, 99, 100, 100, 100, 100, 100, 100, 100, 100, 101, 101, 102, 102, 102, 103, 103, 103, 103, 103, 104, 104, 104, 104, 104, 104, 104, 104, 104, 105, 105, 105, 106, 106, 106, 106, 106, 106, 107, 108, 108, 108, 108, 108, 108, 108, 108, 108, 108, 109, 109, 109, 110, 110, 110, 110, 110, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 112, 112, 112, 112, 113, 114, 115, 115, 115, 116, 116, 116, 116, 117, 117, 118, 118, 118, 118, 118, 118, 118, 118, 118, 118, 118, 118, 118, 118, 118, 118, 118, 119, 119, 119, 119, 119, 119, 119, 120, 120, 120, 120, 120, 120, 120, 120, 120, 120, 120, 120, 120, 121, 121, 121, 121, 122, 122, 122, 122, 122]</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -545,14 +620,29 @@
       <c r="B6" t="n">
         <v>0.75</v>
       </c>
-      <c r="C6" t="n">
-        <v>55</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>compare</t>
+        </is>
       </c>
       <c r="D6" t="n">
-        <v>0.6663259101981938</v>
+        <v>52</v>
       </c>
       <c r="E6" t="n">
-        <v>0.632052519543884</v>
+        <v>0.5995652541864896</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5292610913274454</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.5840261534095798), np.float64(0.5840261534095798), np.float64(0.5840261534095798), np.float64(0.6374411260045559), np.float64(0.6374411260045559), np.float64(0.6374411260045559), np.float64(0.6374411260045559), np.float64(0.6888608209593649), np.float64(0.6888608209593649), np.float64(0.6888608209593649), np.float64(0.6888608209593649), np.float64(0.5666525933316318), np.float64(0.5666525933316318), np.float64(0.5666525933316318), np.float64(0.6318559658125148), np.float64(0.6318559658125148), np.float64(0.5277576346765188), np.float64(0.5277576346765188), np.float64(0.4680737940424115), np.float64(0.4680737940424115), np.float64(0.4680737940424115), np.float64(0.35742063572050525), np.float64(0.39820140672289794), np.float64(0.44266715918580035), np.float64(0.44704126166707775), np.float64(0.44704126166707775), np.float64(0.44704126166707775), np.float64(0.44704126166707775), np.float64(0.49312029168861926), np.float64(0.49312029168861926), np.float64(0.49221756578697806), np.float64(0.5284875437235806), np.float64(0.5409772949267483), np.float64(0.5582599161638488), np.float64(0.5465355872394607), np.float64(0.5465355872394607), np.float64(0.5465355872394607), np.float64(0.5465355872394607), np.float64(0.5716090508167561), np.float64(0.588811476665079), np.float64(0.588811476665079), np.float64(0.588811476665079), np.float64(0.6069877213575725), np.float64(0.6250423558189028), np.float64(0.6250423558189028), np.float64(0.6250423558189028), np.float64(0.6026116081381447), np.float64(0.6198782101805149), np.float64(0.6156898026158119), np.float64(0.6156898026158119), np.float64(0.6187370911671882), np.float64(0.6034963420517239), np.float64(0.614704972270554), np.float64(0.6272339854571969), np.float64(0.6272339854571969), np.float64(0.6208997484855948), np.float64(0.6208997484855948), np.float64(0.6208997484855948), np.float64(0.6117537301961551), np.float64(0.6241138323978778), np.float64(0.6330282765178933), np.float64(0.6391854606164262), np.float64(0.6391854606164262), np.float64(0.6391854606164262), np.float64(0.6444124066716168), np.float64(0.6440136369992867), np.float64(0.6440136369992867), np.float64(0.6530167841298359), np.float64(0.6350517511054351), np.float64(0.6446480254360651), np.float64(0.6529713109062132), np.float64(0.6608120201957179), np.float64(0.6560634595203457), np.float64(0.6560634595203457), np.float64(0.6313014189960493), np.float64(0.6313014189960493), np.float64(0.629723885490048), np.float64(0.636448893844801), np.float64(0.6440365782036345), np.float64(0.6288767596539518), np.float64(0.6122073862593658), np.float64(0.5965520565846842), np.float64(0.6026491065279097), np.float64(0.6098742663749601), np.float64(0.6098742663749601), np.float64(0.6174952100038482), np.float64(0.60138769878253), np.float64(0.5973133515614594), np.float64(0.5860461730047246), np.float64(0.5894580361935822), np.float64(0.5879980419982649), np.float64(0.570721737621033), np.float64(0.5580302282464672), np.float64(0.56551214953134), np.float64(0.5645126213729195), np.float64(0.5645126213729194), np.float64(0.5645126213729194), np.float64(0.5645126213729194), np.float64(0.5497591528450344), np.float64(0.5427059763085913), np.float64(0.546707471869155), np.float64(0.553502841993213), np.float64(0.5573705670885178), np.float64(0.5459156520683904), np.float64(0.5333767193297004), np.float64(0.5381175067212314), np.float64(0.5314623832125543), np.float64(0.5366731221872303), np.float64(0.5431865367251693), np.float64(0.5477914618123111), np.float64(0.5394420059839656), np.float64(0.5433032789906245), np.float64(0.5493849789129738), np.float64(0.5493849789129738), np.float64(0.5498552783976939), np.float64(0.5457392592695973), np.float64(0.550339891141494), np.float64(0.550339891141494), np.float64(0.5501511602460968), np.float64(0.5557643345178962), np.float64(0.5557643345178962), np.float64(0.5602617967705267), np.float64(0.5577507340949402), np.float64(0.5554697870402894), np.float64(0.5605225746404996), np.float64(0.5647019415695997), np.float64(0.5696618553268263), np.float64(0.5741370607951599), np.float64(0.5759780900816899), np.float64(0.5736262095391244), np.float64(0.5736262095391244), np.float64(0.5772404175509938), np.float64(0.5714248054099377), np.float64(0.5645126446867009), np.float64(0.5691763394662357), np.float64(0.5680717831757587), np.float64(0.5692633353029204), np.float64(0.5703037019420957), np.float64(0.5743928502354108), np.float64(0.5656159583681368), np.float64(0.565545374194361), np.float64(0.5577683106474773), np.float64(0.5577683106474773), np.float64(0.5534047823583073), np.float64(0.5480234348360742), np.float64(0.5466468310501736), np.float64(0.5509956468821041), np.float64(0.5534067162631559), np.float64(0.5530702191469232), np.float64(0.5479586387187616), np.float64(0.5521291058859968), np.float64(0.5559981181924922), np.float64(0.5552402168381401), np.float64(0.5488745023573257), np.float64(0.5502094776232174), np.float64(0.5530198657124866), np.float64(0.5559523424459397), np.float64(0.5471172220425473), np.float64(0.5426710658233901), np.float64(0.5465728789604184), np.float64(0.549800294924421), np.float64(0.5528900226405805), np.float64(0.5502290028154858), np.float64(0.5530890187728679), np.float64(0.5563010486655948), np.float64(0.5598634986542448), np.float64(0.5631504449227263), np.float64(0.5666136460419899), np.float64(0.565303309631645), np.float64(0.568712237587223), np.float64(0.5710451967808206), np.float64(0.5725336561534942), np.float64(0.5758115673298478), np.float64(0.5789248851816147), np.float64(0.5744726115452149), np.float64(0.5718072220623454), np.float64(0.5749883436942176), np.float64(0.5700729211251436), np.float64(0.573224383185164), np.float64(0.5749530871831934), np.float64(0.5779909404077889), np.float64(0.581003078070626), np.float64(0.583750123140326), np.float64(0.5867000575259381), np.float64(0.5895322702542989), np.float64(0.5923984672831675), np.float64(0.5862423391986606), np.float64(0.5795962522481611), np.float64(0.5778728958017415), np.float64(0.5742097349173148), np.float64(0.5761330004450413), np.float64(0.5789252225935954), np.float64(0.5804383582740459), np.float64(0.5809799003634476), np.float64(0.5834140152401147), np.float64(0.5858310348415521), np.float64(0.5884609031458115), np.float64(0.5910133912598542), np.float64(0.5907476963027206), np.float64(0.5869650001636569), np.float64(0.5894429397808978), np.float64(0.5903291586333043), np.float64(0.5927950158197728), np.float64(0.5951601980800311), np.float64(0.5941011261340583), np.float64(0.5879698863741856), np.float64(0.5852435390194206), np.float64(0.5875701235781718), np.float64(0.5898295722962532), np.float64(0.5922630133917303), np.float64(0.5914458862022277), np.float64(0.5937224888527858), np.float64(0.5903175785570054), np.float64(0.5927034761833899), np.float64(0.594733277104926), np.float64(0.5931220177508456), np.float64(0.5945374043969357), np.float64(0.5945374043969357), np.float64(0.59288352697276), np.float64(0.5922163201752617), np.float64(0.5944954811808675), np.float64(0.5940636463931311), np.float64(0.5960621767459222), np.float64(0.5971857563249651), np.float64(0.5970171779162344), np.float64(0.5989516579833396), np.float64(0.5971701273042669), np.float64(0.5923359018728573), np.float64(0.5931327021348878), np.float64(0.5945872435182732), np.float64(0.5967371103959347), np.float64(0.5982873078091606), np.float64(0.6000662825975912), np.float64(0.5964252000270537), np.float64(0.5978048169897608), np.float64(0.5960394534259891), np.float64(0.5958562688145709), np.float64(0.5910496718094725), np.float64(0.5931244792401256), np.float64(0.5946386596197355), np.float64(0.5966330809671715), np.float64(0.598667025139433), np.float64(0.6006216302342281), np.float64(0.6020959256156777), np.float64(0.6038502892560632), np.float64(0.6051584788166926), np.float64(0.6039327595994682), np.float64(0.6000081937547042), np.float64(0.6016844303892491), np.float64(0.6002380504319879), np.float64(0.6020718764392179), np.float64(0.6036015466745119), np.float64(0.602763091520183), np.float64(0.6043545820184502), np.float64(0.6045757466744626), np.float64(0.6060077313908221), np.float64(0.6025173882884542), np.float64(0.6043677994372675), np.float64(0.6017495873403604), np.float64(0.6031531641500437), np.float64(0.6044315305125538), np.float64(0.6024353212098212), np.float64(0.6023851030834334), np.float64(0.6007076883756329), np.float64(0.5976835128385214), np.float64(0.5978632797495701), np.float64(0.5950174863740627), np.float64(0.5950819083647332), np.float64(0.5967531349519974), np.float64(0.5972411942875597), np.float64(0.5981732179152263), np.float64(0.5985788418016568), np.float64(0.5994449160225314), np.float64(0.6010617137937415), np.float64(0.6024474913378289), np.float64(0.6030242206017745), np.float64(0.6010919681117058), np.float64(0.5999908862271309), np.float64(0.5966121844183704), np.float64(0.59828477573775), np.float64(0.5944497275545159), np.float64(0.5961376583630504), np.float64(0.5953510013439856), np.float64(0.5970316954411687), np.float64(0.5986606883003607), np.float64(0.5952813869657505), np.float64(0.5969373893313944), np.float64(0.594513814914272), np.float64(0.5960844474270416), np.float64(0.5977154474294556), np.float64(0.5990903753191043)]</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 8, 9, 10, 10, 11, 12, 13, 13, 14, 15, 16, 16, 17, 18, 18, 19, 19, 20, 20, 21, 22, 22, 22, 22, 22, 23, 24, 25, 25, 26, 26, 26, 26, 26, 26, 27, 28, 29, 29, 29, 30, 31, 31, 31, 32, 33, 33, 33, 33, 34, 34, 34, 34, 34, 35, 35, 36, 37, 37, 37, 37, 37, 38, 39, 39, 39, 40, 40, 40, 40, 40, 40, 40, 41, 41, 42, 42, 42, 42, 42, 42, 42, 42, 42, 43, 43, 43, 43, 43, 43, 43, 43, 43, 43, 43, 44, 45, 46, 46, 46, 46, 46, 46, 46, 46, 46, 46, 46, 46, 46, 46, 46, 46, 47, 47, 47, 47, 48, 48, 48, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 50, 50, 50, 50, 50, 50, 50, 50, 50, 50, 50, 50, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52]</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -564,14 +654,845 @@
       <c r="B7" t="n">
         <v>1</v>
       </c>
-      <c r="C7" t="n">
-        <v>30</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>compare</t>
+        </is>
       </c>
       <c r="D7" t="n">
-        <v>0.5829420827845576</v>
+        <v>38</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5765014363451367</v>
+        <v>0.4199230215768699</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.3835319941475508</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(-0.9224535490554655), np.float64(-0.1728077467104685), np.float64(-0.1728077467104685), np.float64(-0.1728077467104685), np.float64(-0.1728077467104685), np.float64(0.14024387933199925), np.float64(0.14024387933199925), np.float64(0.21961130454395844), np.float64(0.21961130454395844), np.float64(0.21961130454395844), np.float64(0.21961130454395844), np.float64(0.21961130454395844), np.float64(0.21961130454395844), np.float64(0.21961130454395844), np.float64(0.21961130454395844), np.float64(0.2876708481136519), np.float64(0.16580013922641965), np.float64(0.16580013922641965), np.float64(0.16580013922641965), np.float64(0.2809633041796106), np.float64(0.2809633041796106), np.float64(0.25451655181908683), np.float64(0.25451655181908683), np.float64(0.28493554127697124), np.float64(0.28493554127697124), np.float64(0.28493554127697124), np.float64(0.32111662325734164), np.float64(0.32111662325734164), np.float64(0.38144775360057), np.float64(0.3116650553211567), np.float64(0.3168475537392977), np.float64(0.25947528516281204), np.float64(0.30844536700977054), np.float64(0.30844536700977054), np.float64(0.2712844618511739), np.float64(0.2449467110754961), np.float64(0.28653981986187055), np.float64(0.3167240739371087), np.float64(0.3337507695872057), np.float64(0.3653483390095823), np.float64(0.3653483390095823), np.float64(0.3653483390095823), np.float64(0.3542604675746107), np.float64(0.369673852625911), np.float64(0.3831046721477453), np.float64(0.4019215298395887), np.float64(0.3612857743183371), np.float64(0.3612857743183371), np.float64(0.3612857743183371), np.float64(0.3612857743183371), np.float64(0.3505728011296237), np.float64(0.31935516505660494), np.float64(0.31935516505660494), np.float64(0.3421765558866219), np.float64(0.3421765558866219), np.float64(0.3632234258906987), np.float64(0.3632234258906987), np.float64(0.3632234258906987), np.float64(0.37881809136699973), np.float64(0.37881809136699973), np.float64(0.3839250761093175), np.float64(0.3839250761093175), np.float64(0.38816615781086156), np.float64(0.3903955780596224), np.float64(0.40697127171357833), np.float64(0.4226860029569617), np.float64(0.38843280352320536), np.float64(0.4024841043837415), np.float64(0.4024841043837415), np.float64(0.4151898428410955), np.float64(0.4127605134871944), np.float64(0.4019160443516949), np.float64(0.37257516107739713), np.float64(0.3839966464071959), np.float64(0.38668395093475194), np.float64(0.3932198889847673), np.float64(0.40611310060192635), np.float64(0.4182256797593527), np.float64(0.41951645024452544), np.float64(0.42388380142633125), np.float64(0.43532728950818034), np.float64(0.44226513728436484), np.float64(0.4374281620701505), np.float64(0.4183006232401587), np.float64(0.40943820339293474), np.float64(0.4159498879374432), np.float64(0.39438600258569995), np.float64(0.4003350674556196), np.float64(0.40307165046268817), np.float64(0.40807917727252063), np.float64(0.39798557942398477), np.float64(0.4030059546782082), np.float64(0.40897864985873267), np.float64(0.41643208486005406), np.float64(0.40543164119854885), np.float64(0.4033446152886231), np.float64(0.40189541125230044), np.float64(0.40815790370773253), np.float64(0.4081579037077326), np.float64(0.41512089290897275), np.float64(0.4234793632757245), np.float64(0.4292995110100411), np.float64(0.4132869443161876), np.float64(0.4195956253027797), np.float64(0.42751725196421314), np.float64(0.42072582532247416), np.float64(0.41041311194383384), np.float64(0.41812893275485763), np.float64(0.4252387444622687), np.float64(0.4324500357171051), np.float64(0.4231317267704445), np.float64(0.4250154419910605), np.float64(0.424351263283963), np.float64(0.4248580161423241), np.float64(0.41864923116895686), np.float64(0.42052059345393494), np.float64(0.42703706285176857), np.float64(0.42174815225049733), np.float64(0.4282417259458203), np.float64(0.414427764577489), np.float64(0.41366565390384585), np.float64(0.4156545073260603), np.float64(0.41333611773626944), np.float64(0.39912794466068113), np.float64(0.38778014263297644), np.float64(0.39228466305275883), np.float64(0.3946796190808451), np.float64(0.3827834638369751), np.float64(0.3743279250105581), np.float64(0.37663976088365636), np.float64(0.3804275869957885), np.float64(0.3804275869957885), np.float64(0.37847716828581646), np.float64(0.38395539532428713), np.float64(0.38940113409696964), np.float64(0.3853374505758972), np.float64(0.3740242036101937), np.float64(0.36212962291897294), np.float64(0.3631459955515239), np.float64(0.3593734495415642), np.float64(0.36465303237200064), np.float64(0.37025929094085336), np.float64(0.3662706404541255), np.float64(0.3650961803228099), np.float64(0.3696539604978955), np.float64(0.374910910749647), np.float64(0.374967756834238), np.float64(0.3803011941399086), np.float64(0.38141260369645463), np.float64(0.3755571205022112), np.float64(0.3763440735009463), np.float64(0.3786310355168343), np.float64(0.3738131239209494), np.float64(0.37677746156186126), np.float64(0.3704807012176633), np.float64(0.37548929198762526), np.float64(0.37335030540621916), np.float64(0.3773003229301063), np.float64(0.37378861350590264), np.float64(0.37843911853960355), np.float64(0.3775467896470335), np.float64(0.3765642630311975), np.float64(0.38098998780584625), np.float64(0.3856868592051356), np.float64(0.3862537160415799), np.float64(0.3809993737628359), np.float64(0.3832508154609212), np.float64(0.3811402489114457), np.float64(0.3856900859165271), np.float64(0.37934502210656157), np.float64(0.37538915769199493), np.float64(0.37928050049533213), np.float64(0.3738447980106136), np.float64(0.371296756248546), np.float64(0.37288054258598846), np.float64(0.3772298416666616), np.float64(0.3815451791902411), np.float64(0.38254311907075184), np.float64(0.38618533452231313), np.float64(0.3896026302074846), np.float64(0.39329515671724485), np.float64(0.39164821725312116), np.float64(0.3935358248180584), np.float64(0.39660585043665364), np.float64(0.3926877203405167), np.float64(0.3964997127808589), np.float64(0.38909417092359416), np.float64(0.3930259274987415), np.float64(0.39495817085334106), np.float64(0.3987064029290858), np.float64(0.4024561462460296), np.float64(0.4007419934085654), np.float64(0.4034630275810013), np.float64(0.40182528375333687), np.float64(0.4053497117314263), np.float64(0.4085425005053126), np.float64(0.4038463416984864), np.float64(0.40727119652013893), np.float64(0.40842509306600777), np.float64(0.41188893769864), np.float64(0.41278039862358834), np.float64(0.40825686459806604), np.float64(0.4113860028104043), np.float64(0.4113520695632201), np.float64(0.4051077045469564), np.float64(0.39796762261394547), np.float64(0.39220599775147524), np.float64(0.3953929023197505), np.float64(0.39239255180043736), np.float64(0.3958012644382628), np.float64(0.3961148305509994), np.float64(0.3991855087706998), np.float64(0.4010500371065016), np.float64(0.4024908156256439), np.float64(0.40328911980181853), np.float64(0.40146418234360864), np.float64(0.40471485373644056), np.float64(0.40723149698969313), np.float64(0.4042342640121084), np.float64(0.40325729722753645), np.float64(0.40575896501715153), np.float64(0.40575301690471205), np.float64(0.40710421275194275), np.float64(0.4102030665712577), np.float64(0.41318604851447843), np.float64(0.41220174369230456), np.float64(0.4124478010742216), np.float64(0.4149298404876543), np.float64(0.4108912433639155), np.float64(0.41362342708161337), np.float64(0.40893348699838705), np.float64(0.41185142363890914), np.float64(0.41202462087521696), np.float64(0.4115045225022152), np.float64(0.41242985260120674), np.float64(0.41249283285704436), np.float64(0.4151076700239331), np.float64(0.4126486724921453), np.float64(0.414615152942039), np.float64(0.41384890079225106), np.float64(0.4157387981168039), np.float64(0.4185341157530724), np.float64(0.42129336760062425), np.float64(0.41897549693203606), np.float64(0.4216629068531727), np.float64(0.4197581034309294), np.float64(0.4138307905711944), np.float64(0.41298458617856265), np.float64(0.415134172472846), np.float64(0.4113071893853363), np.float64(0.4140067924231331), np.float64(0.4118116037230484), np.float64(0.41337449347143723), np.float64(0.4082807668984776), np.float64(0.4064212215948315), np.float64(0.408743154858684), np.float64(0.41028344474688255), np.float64(0.41180618357049437), np.float64(0.4141268497976905), np.float64(0.41075723498774347), np.float64(0.41332396761963325), np.float64(0.4156315612120263), np.float64(0.41312460877269014), np.float64(0.41299072666926406), np.float64(0.4139091842974648), np.float64(0.4163982251531247), np.float64(0.411709256048065), np.float64(0.40626157082093206), np.float64(0.4085498412557224), np.float64(0.4110453385933227), np.float64(0.4061582307207049), np.float64(0.40687024408503464), np.float64(0.40212222832784467), np.float64(0.4040154078620885), np.float64(0.4064626955877284), np.float64(0.4080257599064648), np.float64(0.40939383811459107), np.float64(0.4062518188506217), np.float64(0.4038218244949653), np.float64(0.40619481998768375), np.float64(0.4074143086599635), np.float64(0.4095781797804328), np.float64(0.40978725688418904), np.float64(0.41045834972605), np.float64(0.4127867181776634), np.float64(0.41452888053442966), np.float64(0.41494608950268264), np.float64(0.41679843752026147), np.float64(0.4172198380345966), np.float64(0.4185123509089543), np.float64(0.4196596172634679), np.float64(0.4179331383550481), np.float64(0.41747542826616046), np.float64(0.4194892040690967)]</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 5, 5, 6, 7, 8, 8, 9, 9, 10, 11, 12, 13, 14, 15, 16, 16, 16, 17, 18, 18, 19, 19, 20, 20, 21, 22, 22, 23, 23, 23, 23, 23, 23, 24, 24, 24, 24, 24, 24, 24, 25, 26, 26, 26, 26, 26, 26, 27, 28, 29, 29, 29, 30, 30, 31, 31, 32, 33, 33, 34, 34, 35, 35, 35, 35, 35, 35, 35, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 36, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38]</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>mixI</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>demonstrate</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>189</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.5746613786481621</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.2569021029706754</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(-0.6115375297996689), np.float64(-0.6115375297996689), np.float64(-0.6115375297996689), np.float64(-0.6115375297996689), np.float64(-0.6115375297996689), np.float64(-0.6115375297996689), np.float64(-0.6115375297996689), np.float64(-0.6115375297996689), np.float64(-0.6115375297996689), np.float64(-0.6115375297996689), np.float64(-0.6115375297996689), np.float64(-0.6115375297996689), np.float64(-0.6115375297996689), np.float64(-0.7798922205030727), np.float64(-0.7798922205030727), np.float64(-0.7798922205030727), np.float64(-0.7798922205030727), np.float64(-0.7798922205030727), np.float64(-0.7798922205030727), np.float64(-0.7798922205030727), np.float64(-0.7798922205030727), np.float64(-0.7798922205030727), np.float64(-0.7798922205030727), np.float64(-0.7798922205030727), np.float64(-0.7798922205030727), np.float64(-0.639727342985423), np.float64(-0.639727342985423), np.float64(-0.639727342985423), np.float64(-0.639727342985423), np.float64(-0.6397273429854231), np.float64(-0.6397273429854231), np.float64(-0.6397273429854231), np.float64(-0.2977134174569345), np.float64(-0.2977134174569345), np.float64(-0.2977134174569345), np.float64(-0.11883969172638478), np.float64(-0.11883969172638478), np.float64(-0.21206262918302554), np.float64(-0.21206262918302554), np.float64(-0.21206262918302554), np.float64(-0.21206262918302554), np.float64(-0.21206262918302554), np.float64(-0.286820956496766), np.float64(-0.286820956496766), np.float64(-0.286820956496766), np.float64(-0.2868209564967659), np.float64(-0.2868209564967659), np.float64(-0.22569294784029248), np.float64(-0.22569294784029248), np.float64(-0.22569294784029248), np.float64(-0.22569294784029248), np.float64(-0.30106090849434697), np.float64(-0.30106090849434697), np.float64(-0.2339070092961882), np.float64(-0.2339070092961882), np.float64(-0.2339070092961882), np.float64(-0.2339070092961882), np.float64(-0.2339070092961882), np.float64(-0.2339070092961882), np.float64(-0.29373700773310596), np.float64(-0.29373700773310596), np.float64(-0.29373700773310596), np.float64(-0.29373700773310596), np.float64(-0.3217048608517659), np.float64(-0.3217048608517659), np.float64(-0.3217048608517659), np.float64(-0.3217048608517659), np.float64(-0.3217048608517659), np.float64(-0.3217048608517659), np.float64(-0.3217048608517659), np.float64(-0.3217048608517659), np.float64(-0.3217048608517659), np.float64(-0.3655831172812523), np.float64(-0.3655831172812523), np.float64(-0.3655831172812523), np.float64(-0.3655831172812523), np.float64(-0.3655831172812523), np.float64(-0.36558311728125226), np.float64(-0.27189559055041623), np.float64(-0.27189559055041623), np.float64(-0.18775165762221063), np.float64(-0.18775165762221063), np.float64(-0.12372106769252764), np.float64(-0.07443999024066184), np.float64(-0.07443999024066184), np.float64(-0.07443999024066186), np.float64(-0.04982228394493795), np.float64(-0.04982228394493795), np.float64(-0.04982228394493795), np.float64(-0.04982228394493795), np.float64(-0.04982228394493795), np.float64(-0.04982228394493795), np.float64(-0.038903520484099466), np.float64(-0.03890352048409947), np.float64(-0.03890352048409947), np.float64(-0.03890352048409947), np.float64(-0.01334737552926113), np.float64(-0.01334737552926113), np.float64(0.01598340903611286), np.float64(0.01598340903611286), np.float64(0.01598340903611286), np.float64(0.055601421354879395), np.float64(0.055601421354879395), np.float64(0.08299289921066942), np.float64(0.08299289921066942), np.float64(0.11997454414097468), np.float64(0.11997454414097468), np.float64(0.11997454414097468), np.float64(0.11997454414097468), np.float64(0.11997454414097469), np.float64(0.11997454414097469), np.float64(0.15513922694574567), np.float64(0.18646020935923335), np.float64(0.18646020935923335), np.float64(0.18646020935923335), np.float64(0.1950604439856814), np.float64(0.1950604439856814), np.float64(0.1950604439856814), np.float64(0.1950604439856814), np.float64(0.1950604439856814), np.float64(0.1950604439856814), np.float64(0.1950604439856814), np.float64(0.1950604439856814), np.float64(0.1950604439856814), np.float64(0.1950604439856814), np.float64(0.22377032025068602), np.float64(0.22193213378086382), np.float64(0.22193213378086382), np.float64(0.22193213378086382), np.float64(0.22193213378086382), np.float64(0.22193213378086382), np.float64(0.22193213378086382), np.float64(0.2328503622889542), np.float64(0.2328503622889542), np.float64(0.2328503622889542), np.float64(0.2328503622889542), np.float64(0.23110687232779845), np.float64(0.23110687232779845), np.float64(0.24957103079827905), np.float64(0.24957103079827905), np.float64(0.24957103079827905), np.float64(0.2720248604657616), np.float64(0.2861676347910784), np.float64(0.2861676347910784), np.float64(0.2861676347910784), np.float64(0.2861676347910784), np.float64(0.2861676347910784), np.float64(0.2861676347910784), np.float64(0.2861676347910784), np.float64(0.2906841303276343), np.float64(0.2906841303276343), np.float64(0.2906841303276343), np.float64(0.2906841303276343), np.float64(0.2906841303276343), np.float64(0.2906841303276343), np.float64(0.2906841303276343), np.float64(0.292909564403885), np.float64(0.3090762088196092), np.float64(0.3185891879611545), np.float64(0.3346544031758762), np.float64(0.3346544031758762), np.float64(0.3346544031758762), np.float64(0.329722409331327), np.float64(0.329722409331327), np.float64(0.329722409331327), np.float64(0.329722409331327), np.float64(0.33729921996747), np.float64(0.3466178377153581), np.float64(0.3466178377153581), np.float64(0.3516522085791572), np.float64(0.3662785057345324), np.float64(0.3662785057345324), np.float64(0.3662785057345324), np.float64(0.36627850573453247), np.float64(0.36627850573453247), np.float64(0.36627850573453247), np.float64(0.37757484778353123), np.float64(0.37549309441622997), np.float64(0.38760359959089535), np.float64(0.39684269416467766), np.float64(0.39684269416467766), np.float64(0.4081457946472151), np.float64(0.41848187149056015), np.float64(0.41848187149056015), np.float64(0.41848187149056015), np.float64(0.42467737636285524), np.float64(0.42148461838242923), np.float64(0.42148461838242923), np.float64(0.4321790939634198), np.float64(0.4321790939634198), np.float64(0.4321790939634198), np.float64(0.4321790939634198), np.float64(0.4426805380756751), np.float64(0.4426805380756751), np.float64(0.4395186018427286), np.float64(0.44794559724265764), np.float64(0.4386251741417038), np.float64(0.4386251741417039), np.float64(0.4386251741417039), np.float64(0.43482404761459786), np.float64(0.44397778450572173), np.float64(0.44397778450572173), np.float64(0.4532446587832692), np.float64(0.4589891562275367), np.float64(0.4589891562275367), np.float64(0.45898915622753667), np.float64(0.46193238864389874), np.float64(0.469543967365574), np.float64(0.469543967365574), np.float64(0.469543967365574), np.float64(0.47738865460602853), np.float64(0.4771690723390286), np.float64(0.4771690723390286), np.float64(0.47716907233902867), np.float64(0.4808019825962371), np.float64(0.48776805418100133), np.float64(0.48556037366080884), np.float64(0.492683641690003), np.float64(0.49918183326744736), np.float64(0.48939692511795563), np.float64(0.48939692511795563), np.float64(0.49609846143397746), np.float64(0.49609846143397746), np.float64(0.5000334063318085), np.float64(0.5016254030312485), np.float64(0.5016254030312485), np.float64(0.5081685558222211), np.float64(0.5081685558222211), np.float64(0.5144821344728889), np.float64(0.5151695843571089), np.float64(0.5186060120060014), np.float64(0.5186060120060014), np.float64(0.5241191316441003), np.float64(0.5299601129493066), np.float64(0.5268587208178327), np.float64(0.5321104260004517), np.float64(0.5321104260004517), np.float64(0.5321104260004516), np.float64(0.5321104260004514), np.float64(0.5321104260004514), np.float64(0.5321104260004514), np.float64(0.5321104260004514), np.float64(0.5321104260004514), np.float64(0.5321104260004514), np.float64(0.537462159568813), np.float64(0.537462159568813), np.float64(0.5361204937229529), np.float64(0.5361204937229529), np.float64(0.5361204937229529), np.float64(0.5391647216004698), np.float64(0.5444658382692471), np.float64(0.5420659645733792), np.float64(0.5420659645733792), np.float64(0.542228120929117), np.float64(0.5452981572927653), np.float64(0.5406371027576256), np.float64(0.5456591548963482), np.float64(0.5457338161951819), np.float64(0.5457338161951819), np.float64(0.5441969010003598), np.float64(0.5441969010003598), np.float64(0.5445378203722192), np.float64(0.5489902369596613), np.float64(0.5536731829949487), np.float64(0.5581641895158977), np.float64(0.5581641895158977), np.float64(0.5571996585394695), np.float64(0.5604479828484217), np.float64(0.5635169663436915), np.float64(0.5650477691625951), np.float64(0.5641062071971945), np.float64(0.560940597596654), np.float64(0.5575400644230974), np.float64(0.5596779823174242), np.float64(0.5625953512703011), np.float64(0.5665645004467664), np.float64(0.5704796541341189), np.float64(0.5704796541341189), np.float64(0.5710024417027488), np.float64(0.5709781898544388), np.float64(0.5709781898544388)]</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 41, 42, 43, 44, 45, 46, 47, 47, 48, 49, 49, 50, 50, 51, 52, 53, 54, 54, 55, 56, 57, 58, 58, 59, 60, 61, 61, 62, 62, 63, 64, 65, 66, 67, 67, 68, 69, 70, 70, 71, 72, 73, 74, 75, 76, 77, 78, 78, 79, 80, 81, 82, 83, 83, 84, 84, 85, 85, 85, 86, 87, 87, 88, 89, 90, 91, 92, 92, 93, 94, 95, 95, 96, 96, 97, 98, 98, 99, 99, 100, 100, 101, 102, 103, 104, 105, 105, 105, 106, 107, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 116, 116, 117, 118, 119, 120, 121, 121, 122, 123, 124, 124, 125, 125, 126, 127, 127, 127, 128, 129, 130, 131, 132, 133, 133, 134, 135, 136, 137, 138, 139, 139, 139, 139, 139, 140, 141, 141, 142, 143, 144, 144, 144, 145, 145, 145, 146, 147, 148, 149, 150, 150, 150, 150, 150, 151, 151, 151, 152, 153, 153, 153, 154, 154, 155, 156, 157, 157, 158, 158, 158, 158, 159, 160, 160, 160, 161, 161, 161, 162, 163, 163, 163, 164, 165, 165, 165, 166, 167, 167, 167, 167, 167, 167, 167, 168, 168, 169, 169, 169, 170, 170, 171, 171, 171, 171, 172, 172, 172, 172, 172, 173, 174, 175, 176, 177, 178, 179, 180, 180, 181, 181, 182, 183, 183, 183, 183, 184, 184, 184, 184, 184, 184, 185, 185, 186, 186, 186, 186, 186, 187, 187, 187, 187, 187, 187, 187, 187, 187, 187, 187, 187, 188, 188, 188, 189]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>mixI</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>demonstrate</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>94</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.5587695169942337</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.4325596861040458</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.6014149586414785), np.float64(0.6014149586414785), np.float64(0.6014149586414785), np.float64(0.6014149586414785), np.float64(0.6014149586414785), np.float64(0.6014149586414785), np.float64(0.6014149586414785), np.float64(0.6014149586414785), np.float64(0.6014149586414785), np.float64(0.7386162045580933), np.float64(0.7462888539037031), np.float64(0.7462888539037031), np.float64(0.7462888539037031), np.float64(0.7462888539037031), np.float64(0.7462888539037031), np.float64(0.7462888539037031), np.float64(0.7462888539037031), np.float64(0.7462888539037031), np.float64(0.797858637144466), np.float64(0.797858637144466), np.float64(0.7814138524601242), np.float64(0.7965157017494917), np.float64(0.7965157017494917), np.float64(0.7710289026384473), np.float64(0.7710289026384473), np.float64(0.7623273059480574), np.float64(0.7623273059480574), np.float64(0.7623273059480575), np.float64(0.7623273059480575), np.float64(0.7623273059480575), np.float64(0.7623273059480575), np.float64(0.7623273059480575), np.float64(0.7623273059480575), np.float64(0.7623273059480575), np.float64(0.7654512351643743), np.float64(0.7654512351643744), np.float64(0.7654512351643744), np.float64(0.7166574306760469), np.float64(0.7042462963317836), np.float64(0.7042462963317836), np.float64(0.7207281620854423), np.float64(0.7207281620854423), np.float64(0.732892928393833), np.float64(0.732892928393833), np.float64(0.7517246798690725), np.float64(0.7517246798690725), np.float64(0.7301435924706393), np.float64(0.7301435924706393), np.float64(0.7201637336270011), np.float64(0.7366246895204911), np.float64(0.7366246895204911), np.float64(0.7321981666454596), np.float64(0.7321981666454596), np.float64(0.7321981666454596), np.float64(0.723472243557844), np.float64(0.723472243557844), np.float64(0.723472243557844), np.float64(0.7306481576482832), np.float64(0.7306481576482832), np.float64(0.7306481576482832), np.float64(0.7393994347054738), np.float64(0.7512436713889891), np.float64(0.7512436713889891), np.float64(0.7512436713889891), np.float64(0.7616738200573734), np.float64(0.7361505921039608), np.float64(0.7361505921039608), np.float64(0.7377767529356154), np.float64(0.7377767529356154), np.float64(0.739405982658474), np.float64(0.739405982658474), np.float64(0.7298663011039934), np.float64(0.7071748804218172), np.float64(0.7071748804218172), np.float64(0.7071748804218172), np.float64(0.7071748804218172), np.float64(0.6999779836603172), np.float64(0.6999779836603172), np.float64(0.7096912875759872), np.float64(0.7058127485068961), np.float64(0.7045515071178712), np.float64(0.7045515071178712), np.float64(0.7107535311759673), np.float64(0.7107535311759672), np.float64(0.6968741023854911), np.float64(0.6968741023854911), np.float64(0.6968741023854911), np.float64(0.6968741023854911), np.float64(0.705340102641191), np.float64(0.705340102641191), np.float64(0.705340102641191), np.float64(0.7131295249760639), np.float64(0.7131295249760639), np.float64(0.7131295249760639), np.float64(0.7204220170568505), np.float64(0.7204220170568505), np.float64(0.7204220170568505), np.float64(0.7204220170568505), np.float64(0.7161253485569045), np.float64(0.7221326332470505), np.float64(0.7053347704285361), np.float64(0.7125183234716639), np.float64(0.7148880742289263), np.float64(0.6925575597911515), np.float64(0.6925575597911515), np.float64(0.6799221029548352), np.float64(0.6793103730820491), np.float64(0.6733403944890867), np.float64(0.6487181691215579), np.float64(0.6417750936754708), np.float64(0.6414268734922705), np.float64(0.6414268734922705), np.float64(0.6430776930672124), np.float64(0.6430776930672124), np.float64(0.6495077693966569), np.float64(0.6558874408380272), np.float64(0.6558874408380272), np.float64(0.6623696227544876), np.float64(0.6666197535906474), np.float64(0.6673144494134956), np.float64(0.6676373753221331), np.float64(0.657098917038078), np.float64(0.6624184299696538), np.float64(0.6624184299696538), np.float64(0.6624184299696538), np.float64(0.6675795406729035), np.float64(0.669073250623502), np.float64(0.6642616281364742), np.float64(0.6496014570845943), np.float64(0.6551630126153563), np.float64(0.6522318136873301), np.float64(0.6401214313117902), np.float64(0.6416614673302761), np.float64(0.6409910450279022), np.float64(0.6409420712017466), np.float64(0.6422123612590015), np.float64(0.632498754867824), np.float64(0.6291751111027274), np.float64(0.6291751111027274), np.float64(0.6234091650955031), np.float64(0.6219206158463702), np.float64(0.6237570449006593), np.float64(0.6271391308010426), np.float64(0.6320292703914138), np.float64(0.6320292703914138), np.float64(0.6254014181030235), np.float64(0.6300466777377586), np.float64(0.6300466777377586), np.float64(0.6176010572663108), np.float64(0.6218487964800531), np.float64(0.6105529450167991), np.float64(0.6099912620666332), np.float64(0.6088943990554018), np.float64(0.6088943990554018), np.float64(0.6132492533939966), np.float64(0.6132492533939966), np.float64(0.6111255457026379), np.float64(0.6079699088141406), np.float64(0.608503758493999), np.float64(0.6100689044473436), np.float64(0.6100689044473436), np.float64(0.6134160699421318), np.float64(0.6156012735463653), np.float64(0.6192189626816772), np.float64(0.6201194674521012), np.float64(0.6233869175530565), np.float64(0.6270543572055716), np.float64(0.6304960800680571), np.float64(0.633549930139915), np.float64(0.6341411512399486), np.float64(0.6369425882370722), np.float64(0.6382238068287401), np.float64(0.6348445638083381), np.float64(0.6384096039295285), np.float64(0.6409154248609137), np.float64(0.6383187630363948), np.float64(0.6417576780475223), np.float64(0.6417576780475223), np.float64(0.6350955758711256), np.float64(0.6357111296934992), np.float64(0.6386373899857872), np.float64(0.6386373899857872), np.float64(0.6297687604562102), np.float64(0.633154636460806), np.float64(0.6356987980645037), np.float64(0.6361703057542015), np.float64(0.627841991385644), np.float64(0.6275306408605732), np.float64(0.6191855578107096), np.float64(0.6166852812549672), np.float64(0.61485349074026), np.float64(0.6101502462584152), np.float64(0.6118783951909368), np.float64(0.6139683965555722), np.float64(0.6146555240394456), np.float64(0.6146781367426729), np.float64(0.6165079219678417), np.float64(0.6175498592742207), np.float64(0.6168891081768754), np.float64(0.6154481617334572), np.float64(0.6184889208829822), np.float64(0.6183893089200659), np.float64(0.6103967530919118), np.float64(0.6103967530919118), np.float64(0.6030547126238918), np.float64(0.5983126596937212), np.float64(0.5936392533409353), np.float64(0.5902778435783866), np.float64(0.5903987519039704), np.float64(0.5860900735915221), np.float64(0.5889265011255196), np.float64(0.5881667551036858), np.float64(0.584778297582188), np.float64(0.5852254092259344), np.float64(0.5791057284181026), np.float64(0.5801672802576162), np.float64(0.5799810361905852), np.float64(0.5824319235742569), np.float64(0.577443155694673), np.float64(0.5791955290668054), np.float64(0.5819120887855802), np.float64(0.5829997836027364), np.float64(0.5832518810004861), np.float64(0.5858887537354288), np.float64(0.5866381247250356), np.float64(0.5866018871391936), np.float64(0.5866018871391936), np.float64(0.5891427819144204), np.float64(0.5849989905401357), np.float64(0.5792304360378723), np.float64(0.5769757235271804), np.float64(0.5794084012879169), np.float64(0.5800950480518079), np.float64(0.5782867611686646), np.float64(0.5782867611686646), np.float64(0.5744321773945953), np.float64(0.5766306423232015), np.float64(0.5746233146387631), np.float64(0.5746233146387631), np.float64(0.5687976360344497), np.float64(0.5638281506211091), np.float64(0.5647714428720956), np.float64(0.5608469654521573), np.float64(0.5595756283753984), np.float64(0.5612355752453669), np.float64(0.5609906468257353), np.float64(0.5615715191486472), np.float64(0.5620205318191495), np.float64(0.5576751930205099), np.float64(0.5576751930205099), np.float64(0.560251155225787), np.float64(0.562546455388446), np.float64(0.562546455388446), np.float64(0.5631588197672238), np.float64(0.5642276364374841), np.float64(0.5667160308151886), np.float64(0.5685935869872677), np.float64(0.5700211151957068), np.float64(0.5699314860249843), np.float64(0.5723251919997653), np.float64(0.5737896526570762), np.float64(0.574970589664822), np.float64(0.5751273278822463), np.float64(0.5735895520791402), np.float64(0.5734165728172149), np.float64(0.5734165728172149), np.float64(0.575311351065621), np.float64(0.5723673451722996), np.float64(0.5742104282211258), np.float64(0.5747049497420671), np.float64(0.5748474712456815), np.float64(0.575952265720969), np.float64(0.5781273440064466), np.float64(0.5801155011867402), np.float64(0.5801502856538896), np.float64(0.5820336971287522), np.float64(0.5763958821355019), np.float64(0.571521190943976), np.float64(0.5712821030014548), np.float64(0.5730295605071298), np.float64(0.5695058253620574), np.float64(0.5673700057861194), np.float64(0.5630061984315302), np.float64(0.5586369268882228), np.float64(0.5605430465657196), np.float64(0.5625678100702838), np.float64(0.5599133940932312)]</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 12, 13, 14, 15, 16, 17, 18, 19, 20, 20, 20, 21, 22, 23, 24, 25, 26, 27, 27, 28, 28, 28, 29, 29, 30, 30, 31, 32, 33, 34, 35, 36, 37, 38, 38, 39, 40, 40, 40, 41, 41, 42, 42, 43, 43, 44, 44, 45, 45, 45, 46, 46, 47, 48, 48, 49, 50, 50, 51, 52, 52, 52, 53, 54, 54, 54, 55, 55, 56, 56, 57, 57, 57, 58, 59, 60, 60, 61, 61, 61, 61, 62, 62, 63, 63, 64, 65, 66, 66, 67, 68, 68, 69, 70, 70, 71, 72, 73, 73, 73, 73, 73, 73, 73, 74, 74, 74, 74, 74, 74, 74, 75, 75, 76, 76, 76, 77, 77, 77, 77, 77, 77, 77, 78, 79, 79, 79, 79, 79, 79, 79, 79, 79, 79, 79, 79, 79, 79, 80, 80, 80, 80, 80, 80, 81, 81, 81, 82, 82, 82, 82, 82, 82, 83, 83, 84, 84, 84, 84, 84, 85, 85, 85, 85, 85, 85, 85, 85, 85, 85, 85, 85, 85, 85, 85, 85, 85, 86, 86, 86, 86, 87, 87, 87, 87, 87, 87, 87, 87, 87, 87, 87, 87, 87, 87, 87, 87, 87, 87, 87, 87, 87, 87, 88, 88, 88, 88, 88, 88, 88, 88, 88, 88, 88, 88, 88, 88, 88, 88, 88, 88, 88, 88, 88, 88, 88, 89, 89, 89, 89, 89, 89, 89, 89, 90, 90, 90, 90, 91, 91, 91, 91, 91, 91, 91, 91, 91, 91, 91, 92, 92, 92, 93, 93, 93, 93, 93, 93, 93, 93, 93, 93, 93, 93, 93, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94]</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>mixI</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>demonstrate</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>83</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.7157374000496006</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.5514742912162703</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.8818633763175747), np.float64(0.8818633763175747), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.43129771334639616), np.float64(0.47811958333009885), np.float64(0.47811958333009885), np.float64(0.47811958333009885), np.float64(0.47811958333009885), np.float64(0.47811958333009885), np.float64(0.47811958333009885), np.float64(0.47811958333009885), np.float64(0.47811958333009885), np.float64(0.47811958333009885), np.float64(0.47811958333009885), np.float64(0.47811958333009885), np.float64(0.47811958333009885), np.float64(0.47811958333009885), np.float64(0.39702527737220844), np.float64(0.5060629708475088), np.float64(0.5060629708475088), np.float64(0.5459941490670756), np.float64(0.5465533037968241), np.float64(0.5465533037968241), np.float64(0.584655353853321), np.float64(0.5864624866353133), np.float64(0.6278133340952242), np.float64(0.6278133340952242), np.float64(0.6278133340952242), np.float64(0.6278133340952242), np.float64(0.6278133340952242), np.float64(0.6278133340952242), np.float64(0.6616354075074399), np.float64(0.6616354075074399), np.float64(0.6499373227888213), np.float64(0.6442812343136455), np.float64(0.6442812343136455), np.float64(0.6466877833575903), np.float64(0.6466877833575903), np.float64(0.6632301048983592), np.float64(0.668310000170231), np.float64(0.668310000170231), np.float64(0.6426778591645478), np.float64(0.652845036267235), np.float64(0.652845036267235), np.float64(0.6695345525430995), np.float64(0.6695345525430995), np.float64(0.6695345525430995), np.float64(0.6695345525430995), np.float64(0.6858969177421564), np.float64(0.6966751674090493), np.float64(0.7046599474235727), np.float64(0.686277290583599), np.float64(0.6859960688162293), np.float64(0.6859960688162293), np.float64(0.6939820324370914), np.float64(0.6948389272466907), np.float64(0.7017596689280986), np.float64(0.6816832349650132), np.float64(0.6874260396792735), np.float64(0.6766194384721516), np.float64(0.6860361069231362), np.float64(0.6860361069231362), np.float64(0.6734296791342421), np.float64(0.682034788689753), np.float64(0.6893446232725784), np.float64(0.68136315295922), np.float64(0.6899759094593803), np.float64(0.6899759094593803), np.float64(0.6871451791464264), np.float64(0.6824298717010007), np.float64(0.6869145538272229), np.float64(0.6869145538272229), np.float64(0.6790252382818848), np.float64(0.6721255603003258), np.float64(0.6721255603003258), np.float64(0.6721255603003258), np.float64(0.6792195481651194), np.float64(0.6856578378132273), np.float64(0.6860626811387581), np.float64(0.6860626811387581), np.float64(0.6818452987046091), np.float64(0.6885537242823749), np.float64(0.6846452662475006), np.float64(0.6805223931477578), np.float64(0.6775206793118714), np.float64(0.6809350437591096), np.float64(0.6699137880094792), np.float64(0.6756933292112103), np.float64(0.6700395672315099), np.float64(0.6708138033200791), np.float64(0.6755688934723607), np.float64(0.6755688934723607), np.float64(0.6785662029876012), np.float64(0.6770568149325517), np.float64(0.6733288496439718), np.float64(0.678627449710412), np.float64(0.678627449710412), np.float64(0.6750164535149212), np.float64(0.6703574463970479), np.float64(0.6717702663245089), np.float64(0.6683649959240444), np.float64(0.6683649959240444), np.float64(0.6700948719260705), np.float64(0.6748045842936352), np.float64(0.6715022053350543), np.float64(0.6750891684850062), np.float64(0.6693409769517311), np.float64(0.6693409769517311), np.float64(0.6740817303054375), np.float64(0.6739462718155943), np.float64(0.6765279033419913), np.float64(0.6801345950052955), np.float64(0.6827262313300042), np.float64(0.6850751250494472), np.float64(0.689121905901661), np.float64(0.6907246655392585), np.float64(0.688591883039435), np.float64(0.6838778585795279), np.float64(0.6823104795236254), np.float64(0.6823104795236254), np.float64(0.6840875526514172), np.float64(0.6798191816183659), np.float64(0.6806191280164027), np.float64(0.683621165062759), np.float64(0.6862216398419256), np.float64(0.6825073532838376), np.float64(0.6861976713760451), np.float64(0.6861976713760451), np.float64(0.684130926973379), np.float64(0.6877141280396653), np.float64(0.6905847113484928), np.float64(0.6922787437922124), np.float64(0.6886475142574854), np.float64(0.6886475142574854), np.float64(0.6868852432636426), np.float64(0.6879802068723019), np.float64(0.6912973200026771), np.float64(0.6912973200026771), np.float64(0.6944480927377765), np.float64(0.6953006680173575), np.float64(0.6971671105612194), np.float64(0.6935085003651579), np.float64(0.6915838802408797), np.float64(0.6915806403754127), np.float64(0.6920796634178654), np.float64(0.6920796634178652), np.float64(0.6946644542251156), np.float64(0.6951776798034786), np.float64(0.6957327737865202), np.float64(0.696955160933452), np.float64(0.6997935942833596), np.float64(0.6967891289974845), np.float64(0.6960075905134303), np.float64(0.6981591708069018), np.float64(0.6964600318259621), np.float64(0.6981013127080747), np.float64(0.6963697220989327), np.float64(0.6986956779092387), np.float64(0.6999506578305559), np.float64(0.7017605154813503), np.float64(0.7020166912041261), np.float64(0.7039561530207324), np.float64(0.7048313108020071), np.float64(0.7071657618172701), np.float64(0.7051893462486893), np.float64(0.7035501752874633), np.float64(0.7049561596859151), np.float64(0.7054267221074975), np.float64(0.7072133579303607), np.float64(0.707781544093106), np.float64(0.7078274883435081), np.float64(0.7100809526908443), np.float64(0.7123433825250867), np.float64(0.7089777445184999), np.float64(0.7058120686171448), np.float64(0.7079591377574566), np.float64(0.709923299635595), np.float64(0.7105706414581422), np.float64(0.712002214150171), np.float64(0.7092293848031795), np.float64(0.7113369176397766), np.float64(0.7094824477342392), np.float64(0.7082123859837551), np.float64(0.7066128707952075), np.float64(0.7076813248572336), np.float64(0.7069464511956958), np.float64(0.7089819784097626), np.float64(0.7108533056796865), np.float64(0.7113946975785655), np.float64(0.7091633101337961), np.float64(0.7102790317701754), np.float64(0.7081821941466196), np.float64(0.7088838669223492), np.float64(0.7107036603113854), np.float64(0.7124072705793058), np.float64(0.7142510163929122), np.float64(0.7158151522813953), np.float64(0.7168534772972617), np.float64(0.7167074406571801), np.float64(0.7177605293422488), np.float64(0.7193335667498509), np.float64(0.7208170236496902), np.float64(0.7204397297340607), np.float64(0.7221595082618054), np.float64(0.723543406660667), np.float64(0.7250868050372927), np.float64(0.7259916619765948), np.float64(0.7243715131121639), np.float64(0.7216038277310369), np.float64(0.7214996234912495), np.float64(0.7221603554845922), np.float64(0.7219630966346884), np.float64(0.7232141858476654), np.float64(0.7247772646414332), np.float64(0.7255824185018839), np.float64(0.7251753677355814), np.float64(0.7244975813255691), np.float64(0.7233522700966305), np.float64(0.7248591896791974), np.float64(0.7264313868030023), np.float64(0.7279664154864256), np.float64(0.7248808369002864), np.float64(0.7254506821662953), np.float64(0.7230589738263018), np.float64(0.721548613740474), np.float64(0.7204947683374398), np.float64(0.7202710545364158), np.float64(0.7189203120413161), np.float64(0.7184991593363865), np.float64(0.7176890902616078), np.float64(0.7178665668966948), np.float64(0.7150290642820687), np.float64(0.7165338242856678), np.float64(0.7167430702166232), np.float64(0.7181343256305629), np.float64(0.7195680665925303), np.float64(0.7202091144942834), np.float64(0.7213737624971585), np.float64(0.7226509771536127), np.float64(0.72219930953581), np.float64(0.7194158444255332), np.float64(0.7178118667116662), np.float64(0.7191955076441), np.float64(0.7169994835230739), np.float64(0.715983763243359), np.float64(0.7155525991421219), np.float64(0.7168248002948365), np.float64(0.7153935435268867), np.float64(0.7140251410047944), np.float64(0.7145926635776654), np.float64(0.713977852194759), np.float64(0.7151112274418429), np.float64(0.7155515869016725), np.float64(0.7144548356161884), np.float64(0.7152477060212353), np.float64(0.7141448486657472), np.float64(0.7152961919091575), np.float64(0.7161621011519024), np.float64(0.7151367400359531), np.float64(0.7146466011389603), np.float64(0.7151273792740966)]</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 20, 21, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 52, 52, 53, 53, 53, 54, 54, 54, 54, 55, 56, 57, 58, 59, 59, 60, 60, 60, 61, 61, 62, 62, 62, 63, 63, 63, 64, 64, 65, 66, 67, 67, 67, 67, 67, 67, 68, 68, 68, 68, 68, 68, 68, 68, 69, 69, 69, 69, 69, 69, 70, 70, 70, 70, 71, 71, 71, 72, 73, 73, 73, 73, 74, 74, 74, 74, 74, 74, 74, 74, 74, 74, 74, 74, 75, 75, 75, 75, 75, 76, 76, 76, 76, 76, 77, 77, 77, 77, 77, 77, 78, 78, 78, 78, 78, 78, 78, 78, 78, 78, 78, 78, 79, 79, 79, 79, 79, 79, 79, 79, 80, 80, 80, 80, 80, 80, 81, 81, 81, 81, 82, 82, 82, 82, 82, 82, 82, 82, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83]</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>mixII</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>demonstrate</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>117</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.5309169928842959</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.3304756548716187</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.697157296646986), np.float64(0.697157296646986), np.float64(0.697157296646986), np.float64(0.697157296646986), np.float64(0.8390828663545677), np.float64(0.8390828663545677), np.float64(0.8390828663545677), np.float64(0.8390828663545677), np.float64(0.8390828663545677), np.float64(0.8390828663545677), np.float64(0.8390828663545677), np.float64(0.7861166479445569), np.float64(0.7861166479445569), np.float64(0.7861166479445569), np.float64(0.7861166479445569), np.float64(0.8293193350602835), np.float64(0.8293193350602835), np.float64(0.8293193350602835), np.float64(0.8293193350602835), np.float64(0.8293193350602835), np.float64(0.7414788058228095), np.float64(0.7414788058228095), np.float64(0.7414788058228095), np.float64(0.7845656714610169), np.float64(0.8133540405568135), np.float64(0.8133540405568135), np.float64(0.8133540405568135), np.float64(0.8133540405568135), np.float64(0.8176496433491883), np.float64(0.8176496433491884), np.float64(0.8176496433491884), np.float64(0.7343226137849702), np.float64(0.7343226137849702), np.float64(0.7343226137849702), np.float64(0.7343226137849702), np.float64(0.7343226137849702), np.float64(0.7607031560830564), np.float64(0.7607031560830564), np.float64(0.7607031560830564), np.float64(0.6583014931896328), np.float64(0.6583014931896328), np.float64(0.6583014931896328), np.float64(0.6538104091575568), np.float64(0.6538104091575568), np.float64(0.6328529721021667), np.float64(0.659057369922948), np.float64(0.6541513552815632), np.float64(0.6541513552815632), np.float64(0.6541513552815632), np.float64(0.6732591480299558), np.float64(0.6039549607140268), np.float64(0.6039549607140268), np.float64(0.6039549607140268), np.float64(0.6039549607140268), np.float64(0.5502504413351619), np.float64(0.5502504413351619), np.float64(0.5502504413351619), np.float64(0.5707181256398608), np.float64(0.5658882006175864), np.float64(0.5658882006175864), np.float64(0.5658882006175864), np.float64(0.5658882006175864), np.float64(0.5658882006175864), np.float64(0.5658882006175864), np.float64(0.5727204799863614), np.float64(0.5727204799863614), np.float64(0.5427099542080129), np.float64(0.5427099542080129), np.float64(0.5427099542080129), np.float64(0.5168834988546497), np.float64(0.5257993404252608), np.float64(0.5445047585903044), np.float64(0.5445047585903044), np.float64(0.5445047585903044), np.float64(0.5561444910856316), np.float64(0.5654205586673444), np.float64(0.580844103478504), np.float64(0.580844103478504), np.float64(0.580844103478504), np.float64(0.5771916139007474), np.float64(0.5827837075346725), np.float64(0.5899343827636251), np.float64(0.5883569673986755), np.float64(0.5883569673986755), np.float64(0.6006829103698514), np.float64(0.6006829103698516), np.float64(0.5883372769366939), np.float64(0.5944426255281947), np.float64(0.604410804010541), np.float64(0.6135664709048708), np.float64(0.6088647294019012), np.float64(0.6174829804418112), np.float64(0.625003258723004), np.float64(0.6250032587230041), np.float64(0.6250032587230041), np.float64(0.6241769738445561), np.float64(0.6254990369284115), np.float64(0.6254990369284115), np.float64(0.6254990369284115), np.float64(0.6254990369284115), np.float64(0.6254990369284115), np.float64(0.6072518326378347), np.float64(0.6001878921132643), np.float64(0.6089627907748841), np.float64(0.6165862551879036), np.float64(0.6165862551879036), np.float64(0.6165862551879036), np.float64(0.6185532634334043), np.float64(0.6225794369179054), np.float64(0.6186170800342833), np.float64(0.6186170800342833), np.float64(0.6112523179871219), np.float64(0.6112523179871219), np.float64(0.5935161128004821), np.float64(0.6000281132124619), np.float64(0.6000281132124619), np.float64(0.5893379448607036), np.float64(0.5964462755800725), np.float64(0.5994030333619306), np.float64(0.5994030333619306), np.float64(0.5994030333619306), np.float64(0.5994030333619306), np.float64(0.5994030333619306), np.float64(0.5994030333619306), np.float64(0.5983294151643215), np.float64(0.6012034987968121), np.float64(0.5915345352643916), np.float64(0.5847474519661223), np.float64(0.5860896288525907), np.float64(0.5727400850721402), np.float64(0.5796221437451641), np.float64(0.5799659943933123), np.float64(0.5861772244390002), np.float64(0.5891881771241535), np.float64(0.5879955250296655), np.float64(0.5879955250296655), np.float64(0.5879955250296655), np.float64(0.5885057877276394), np.float64(0.5919805328912626), np.float64(0.5919805328912626), np.float64(0.5916747734203112), np.float64(0.5937125259149316), np.float64(0.5993401972649635), np.float64(0.5956731531294426), np.float64(0.5956731531294426), np.float64(0.5956731531294426), np.float64(0.5872937687265694), np.float64(0.5872937687265694), np.float64(0.5928322147717013), np.float64(0.5905302275328378), np.float64(0.5933872272191993), np.float64(0.5876498371753697), np.float64(0.5876498371753697), np.float64(0.5876498371753697), np.float64(0.5862321442460251), np.float64(0.5862321442460251), np.float64(0.5835386777920689), np.float64(0.5829422483295282), np.float64(0.5829422483295282), np.float64(0.5880907837290924), np.float64(0.5880907837290924), np.float64(0.5880907837290924), np.float64(0.5900566369089607), np.float64(0.594979917747278), np.float64(0.594979917747278), np.float64(0.5983740067456599), np.float64(0.6029563155677105), np.float64(0.6015926246346518), np.float64(0.6015926246346518), np.float64(0.6015926246346518), np.float64(0.5886492464941214), np.float64(0.5882338447113392), np.float64(0.5882338447113392), np.float64(0.5923389031147189), np.float64(0.5930037790205632), np.float64(0.5872486008066189), np.float64(0.587219601997386), np.float64(0.587219601997386), np.float64(0.587219601997386), np.float64(0.5860344710967966), np.float64(0.5830046320410341), np.float64(0.5797972438246097), np.float64(0.5797972438246097), np.float64(0.5831824633379177), np.float64(0.5831824633379177), np.float64(0.586253668503244), np.float64(0.5778834546518836), np.float64(0.5750889111607895), np.float64(0.5674868866296543), np.float64(0.5710553240840204), np.float64(0.5608130765425855), np.float64(0.557989277190807), np.float64(0.5613956402237009), np.float64(0.5623934329283206), np.float64(0.5522275560825955), np.float64(0.5563773878936422), np.float64(0.548184738704822), np.float64(0.548184738704822), np.float64(0.548184738704822), np.float64(0.548184738704822), np.float64(0.5422229407298583), np.float64(0.5401219593977263), np.float64(0.5313702329193188), np.float64(0.5321943953904087), np.float64(0.5351866123012926), np.float64(0.526235122696343), np.float64(0.5295494949924529), np.float64(0.5318265602361776), np.float64(0.5326143956647841), np.float64(0.5326143956647841), np.float64(0.5258853081914519), np.float64(0.5258853081914519), np.float64(0.5298487993842687), np.float64(0.5211737482044003), np.float64(0.5218400224251805), np.float64(0.5152886663780124), np.float64(0.5127207812530306), np.float64(0.5151518955646083), np.float64(0.5156753402025257), np.float64(0.5126032120587523), np.float64(0.5155972298705047), np.float64(0.5191453262296366), np.float64(0.5214049428266639), np.float64(0.5214049428266639), np.float64(0.5214049428266639), np.float64(0.5149436778011318), np.float64(0.5149436778011318), np.float64(0.5182254088855331), np.float64(0.5215352183374983), np.float64(0.5215352183374983), np.float64(0.5234302412285637), np.float64(0.5234302412285637), np.float64(0.5235359138585368), np.float64(0.5267374250289298), np.float64(0.5301395509529134), np.float64(0.5322039322506866), np.float64(0.5340113003657473), np.float64(0.5357906586534363), np.float64(0.5390641427245669), np.float64(0.5405671814830562), np.float64(0.5437481285952965), np.float64(0.5437481285952965), np.float64(0.5437481285952965), np.float64(0.5376045429034363), np.float64(0.5387905833564981), np.float64(0.5418626425212496), np.float64(0.5360520514706135), np.float64(0.538377564767504), np.float64(0.538507016670025), np.float64(0.5411493723645531), np.float64(0.5392023168772617), np.float64(0.5374635386909143), np.float64(0.5313257921689684), np.float64(0.525200732952242), np.float64(0.5252893662368626), np.float64(0.527522200636398), np.float64(0.5283712772026578), np.float64(0.5281697915017601), np.float64(0.5310487839186169), np.float64(0.5302701705719955), np.float64(0.5302701705719955), np.float64(0.527285249225171), np.float64(0.5236423784155043), np.float64(0.5255326672464973), np.float64(0.5273259022454373), np.float64(0.5245445997162985), np.float64(0.526685493533235), np.float64(0.5242857904475052), np.float64(0.5203558995887382), np.float64(0.5203558995887382), np.float64(0.5218597246847616), np.float64(0.5218597246847616), np.float64(0.5239958892528275), np.float64(0.5240826119495126), np.float64(0.5263566191038638), np.float64(0.5219773064552677), np.float64(0.5240861175608831), np.float64(0.5240861175608831), np.float64(0.5193056224994473), np.float64(0.5181677744827257), np.float64(0.5195408462437279), np.float64(0.5221835354969524), np.float64(0.5221835354969524), np.float64(0.5221835354969524), np.float64(0.5218056618528087), np.float64(0.5223202673720796), np.float64(0.5237709070606597), np.float64(0.5258928103629441), np.float64(0.5284600742091382)]</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 10, 11, 12, 13, 13, 14, 15, 16, 17, 18, 19, 19, 20, 21, 22, 22, 23, 24, 25, 26, 26, 27, 28, 28, 28, 29, 30, 31, 31, 32, 33, 33, 34, 35, 36, 37, 37, 38, 39, 39, 40, 41, 41, 42, 42, 42, 42, 43, 44, 44, 44, 45, 46, 47, 47, 48, 49, 49, 49, 50, 51, 52, 53, 54, 54, 55, 55, 56, 57, 57, 57, 57, 58, 59, 59, 59, 59, 60, 61, 61, 61, 61, 61, 62, 62, 63, 63, 63, 63, 63, 63, 63, 63, 64, 65, 65, 65, 66, 67, 68, 69, 69, 69, 69, 69, 70, 71, 71, 71, 71, 72, 72, 73, 73, 73, 74, 74, 74, 74, 75, 76, 77, 78, 79, 79, 79, 79, 79, 79, 79, 79, 79, 79, 79, 79, 80, 81, 81, 81, 82, 82, 82, 82, 82, 83, 84, 84, 85, 85, 85, 85, 85, 86, 87, 87, 88, 88, 88, 89, 89, 90, 91, 91, 91, 92, 92, 92, 92, 93, 94, 94, 94, 95, 95, 95, 95, 95, 96, 97, 97, 97, 97, 98, 98, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 100, 101, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 103, 103, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 105, 106, 106, 107, 107, 107, 108, 108, 109, 109, 109, 109, 109, 109, 109, 109, 109, 109, 110, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 112, 112, 112, 112, 112, 112, 112, 112, 112, 113, 113, 114, 114, 114, 114, 114, 114, 115, 115, 115, 115, 115, 116, 117, 117, 117, 117, 117, 117]</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>mixII</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>demonstrate</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>59</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.8055038588242686</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.6462832829745134</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.5027797486203515), np.float64(0.5027797486203515), np.float64(0.5027797486203515), np.float64(0.5027797486203515), np.float64(0.5018719830663811), np.float64(0.6452612901800795), np.float64(0.6452612901800795), np.float64(0.6452612901800795), np.float64(0.7314149616355747), np.float64(0.7314149616355747), np.float64(0.7314149616355747), np.float64(0.7314149616355747), np.float64(0.7647575580031915), np.float64(0.7647575580031915), np.float64(0.7647575580031915), np.float64(0.7133795932128804), np.float64(0.7133795932128804), np.float64(0.7133795932128804), np.float64(0.7133795932128805), np.float64(0.7133795932128805), np.float64(0.697034273047139), np.float64(0.7337419899492881), np.float64(0.7337419899492881), np.float64(0.7337419899492881), np.float64(0.7118380166583944), np.float64(0.7118380166583944), np.float64(0.7118380166583944), np.float64(0.7118380166583944), np.float64(0.7118380166583944), np.float64(0.7118380166583944), np.float64(0.7118380166583944), np.float64(0.7118380166583944), np.float64(0.705621704054605), np.float64(0.705621704054605), np.float64(0.6977774264556106), np.float64(0.6977774264556106), np.float64(0.707410905884529), np.float64(0.707410905884529), np.float64(0.707410905884529), np.float64(0.7283222255932669), np.float64(0.7283222255932669), np.float64(0.7283222255932669), np.float64(0.7403518544516051), np.float64(0.7286961910160012), np.float64(0.7286961910160012), np.float64(0.7286961910160012), np.float64(0.7286961910160012), np.float64(0.7286961910160012), np.float64(0.7442803847331696), np.float64(0.7354099201958637), np.float64(0.7384599462582057), np.float64(0.7326400741743366), np.float64(0.7371875882037088), np.float64(0.7270710352796587), np.float64(0.7249372635591068), np.float64(0.7367610345987193), np.float64(0.7367610345987193), np.float64(0.7367610345987193), np.float64(0.7422124845608747), np.float64(0.7422124845608747), np.float64(0.7315612189989572), np.float64(0.7181746881620567), np.float64(0.7181746881620567), np.float64(0.7274038181366881), np.float64(0.7274038181366881), np.float64(0.7274038181366881), np.float64(0.7316689450327644), np.float64(0.7316689450327644), np.float64(0.7316689450327644), np.float64(0.7336952244456356), np.float64(0.7294521558759214), np.float64(0.7368912393446814), np.float64(0.7403983204695229), np.float64(0.745275479581044), np.float64(0.7452754795810439), np.float64(0.7452754795810439), np.float64(0.7496803169836175), np.float64(0.7562864812586493), np.float64(0.7628295917027665), np.float64(0.7680202432082364), np.float64(0.7736580159119958), np.float64(0.7718209338326747), np.float64(0.7729173616641504), np.float64(0.7729173616641504), np.float64(0.7784000389709913), np.float64(0.7832026673217508), np.float64(0.7822381556158874), np.float64(0.7822381556158874), np.float64(0.777467290015117), np.float64(0.7816356201559139), np.float64(0.7805207466828763), np.float64(0.784015784901809), np.float64(0.7879585597085872), np.float64(0.7879585597085872), np.float64(0.7921657384259916), np.float64(0.7921657384259916), np.float64(0.7925862875941518), np.float64(0.7919718005402994), np.float64(0.7926398809368005), np.float64(0.7902643198342258), np.float64(0.7904946209250786), np.float64(0.7915529890371164), np.float64(0.7898594181801549), np.float64(0.7898594181801549), np.float64(0.7929364725987613), np.float64(0.7885916979266085), np.float64(0.7914670374987904), np.float64(0.7942155344104633), np.float64(0.7966631098705668), np.float64(0.7970222726993188), np.float64(0.7991233944798034), np.float64(0.7977866422573497), np.float64(0.7990932017814295), np.float64(0.8017750570386644), np.float64(0.8017750570386645), np.float64(0.8024721693153294), np.float64(0.8051298560923437), np.float64(0.8053718269435867), np.float64(0.8028535590477581), np.float64(0.8032433367581173), np.float64(0.8056172050785704), np.float64(0.8059459546233044), np.float64(0.8047308409321388), np.float64(0.8044729925329905), np.float64(0.8048945703625625), np.float64(0.8048945703625625), np.float64(0.8017290365139381), np.float64(0.8017290365139381), np.float64(0.7972720657983813), np.float64(0.7972720657983813), np.float64(0.798071426018132), np.float64(0.7945250325087596), np.float64(0.7958698420522298), np.float64(0.7965785821404361), np.float64(0.7980642236156771), np.float64(0.7969363630960987), np.float64(0.7953201372053824), np.float64(0.7975738351511396), np.float64(0.79988817820159), np.float64(0.7973004711850608), np.float64(0.7961192070313566), np.float64(0.7961192070313566), np.float64(0.7983543282196783), np.float64(0.7995345321143392), np.float64(0.8013628619614565), np.float64(0.8034266691363522), np.float64(0.8012209314575893), np.float64(0.8002874496188239), np.float64(0.7965629508137501), np.float64(0.797615189462827), np.float64(0.7996502255646768), np.float64(0.8005808337018523), np.float64(0.8007892540862416), np.float64(0.8004885630770695), np.float64(0.8019884104637134), np.float64(0.8031231806134793), np.float64(0.7997105824757151), np.float64(0.8003939132177663), np.float64(0.8022050365340057), np.float64(0.7997316462471105), np.float64(0.801572245769269), np.float64(0.8017537944030708), np.float64(0.8035174557075583), np.float64(0.8032621443559316), np.float64(0.8047374157788406), np.float64(0.806298625665254), np.float64(0.8071289683306219), np.float64(0.8067565972814167), np.float64(0.8062077128332785), np.float64(0.8070701410603857), np.float64(0.8079979182293253), np.float64(0.8088526706731254), np.float64(0.8068967585883607), np.float64(0.8080892557454628), np.float64(0.8095500214275769), np.float64(0.8108746147332684), np.float64(0.8118070547117199), np.float64(0.812546240381096), np.float64(0.8139393608782034), np.float64(0.8149849905812843), np.float64(0.8156230673657846), np.float64(0.8136455184157513), np.float64(0.8105881291960243), np.float64(0.8093363412942702), np.float64(0.8092445632111054), np.float64(0.81067301684811), np.float64(0.8095742764262225), np.float64(0.8107134346202695), np.float64(0.8114794041845793), np.float64(0.8127505718987494), np.float64(0.8141073270535947), np.float64(0.81386694342035), np.float64(0.8151261689305652), np.float64(0.8139187587519634), np.float64(0.8123797221707271), np.float64(0.8136676921946076), np.float64(0.8142278161018566), np.float64(0.8149683028468933), np.float64(0.8159633151257722), np.float64(0.8159633151257722), np.float64(0.8134610301620918), np.float64(0.8133270019973959), np.float64(0.813025239534669), np.float64(0.810897447728312), np.float64(0.8108778613436979), np.float64(0.8121035722257057), np.float64(0.8098385398472946), np.float64(0.8104729999548203), np.float64(0.8098138560795367), np.float64(0.8095141039868922), np.float64(0.8102388588959338), np.float64(0.8091689018393696), np.float64(0.8091791249340113), np.float64(0.810209990726795), np.float64(0.8089601021692466), np.float64(0.8095987403811438), np.float64(0.8107600635034687), np.float64(0.8086381660296527), np.float64(0.8089596146057226), np.float64(0.8092169043897138), np.float64(0.8094070351091877), np.float64(0.8099038312599496), np.float64(0.8092215172723748), np.float64(0.8083874335588966), np.float64(0.8086816583843335), np.float64(0.8078064771074434), np.float64(0.8066151535208118), np.float64(0.8068297485552351), np.float64(0.8076056243317153), np.float64(0.8079813239382034), np.float64(0.807742349106039), np.float64(0.8071010229812973), np.float64(0.8081674794170779), np.float64(0.8079582007055385), np.float64(0.8088169710840505), np.float64(0.8077362049422641), np.float64(0.8079702434297217), np.float64(0.8063282180877404), np.float64(0.8073523631506139), np.float64(0.8083869773364442), np.float64(0.8081540492728202), np.float64(0.8091313369523138), np.float64(0.808126660796496), np.float64(0.8073523724354704), np.float64(0.807964400620948), np.float64(0.8080320664606354), np.float64(0.8071668256830111), np.float64(0.8073052948569676), np.float64(0.8066394807465844), np.float64(0.8074084758112486), np.float64(0.8076498485489462), np.float64(0.8069307141548201), np.float64(0.8072247200964784), np.float64(0.8074114006774624), np.float64(0.8071815678133462), np.float64(0.8074896411996851), np.float64(0.8069601940505642), np.float64(0.8065295463568917), np.float64(0.8072424273109993), np.float64(0.8079941315790073), np.float64(0.80806275859581), np.float64(0.8073073522244253), np.float64(0.8072097333313467), np.float64(0.8080043833661367), np.float64(0.8072997776665838), np.float64(0.8070766264550783), np.float64(0.8068603886445092), np.float64(0.8074670387360248), np.float64(0.8080923978687462), np.float64(0.8072014266464612), np.float64(0.8066418092722284), np.float64(0.8069800506087614), np.float64(0.8068667488593384), np.float64(0.8076961822287102), np.float64(0.8073703858894771), np.float64(0.8078649106527293), np.float64(0.8074956917533408), np.float64(0.8070573097281878), np.float64(0.8069610904824993), np.float64(0.8072193559480924), np.float64(0.8071503881298885), np.float64(0.8053802885216478), np.float64(0.8062049463346811), np.float64(0.8063323819341973), np.float64(0.805999014273228), np.float64(0.8067944981332006), np.float64(0.8065546704787051), np.float64(0.8052758100178521), np.float64(0.805990630482795), np.float64(0.8058846024381836), np.float64(0.805442074436826), np.float64(0.8057993469586391), np.float64(0.8059750665366375), np.float64(0.8064741682429751)]</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 5, 6, 7, 8, 8, 8, 9, 10, 10, 11, 12, 13, 13, 14, 15, 15, 16, 17, 18, 19, 19, 19, 20, 21, 21, 22, 23, 24, 25, 26, 27, 28, 28, 29, 29, 30, 30, 31, 32, 32, 33, 34, 34, 34, 35, 36, 37, 38, 38, 38, 38, 38, 38, 38, 38, 38, 39, 40, 40, 41, 41, 41, 42, 42, 43, 44, 44, 45, 46, 46, 46, 46, 46, 46, 47, 48, 48, 48, 48, 48, 48, 48, 48, 49, 49, 49, 49, 50, 50, 50, 50, 50, 50, 51, 51, 52, 52, 52, 52, 52, 52, 52, 52, 53, 53, 53, 53, 53, 53, 53, 53, 53, 53, 53, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 55, 55, 56, 56, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59, 59]</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>mixII</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>demonstrate</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>40</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.7530789555362994</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.6661847330971298</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.9652289501360899), np.float64(0.9652289501360899), np.float64(0.9745118519945839), np.float64(0.9745118519945839), np.float64(0.9745118519945839), np.float64(0.9745118519945839), np.float64(0.9745118519945839), np.float64(0.9745118519945839), np.float64(0.9745118519945839), np.float64(0.9745118519945839), np.float64(0.9516971921809988), np.float64(0.9516971921809988), np.float64(0.9516971921809988), np.float64(0.9516971921809988), np.float64(0.9516971921809988), np.float64(0.9516971921809988), np.float64(0.9516971921809988), np.float64(0.8266032256128973), np.float64(0.8609032993153735), np.float64(0.8816666095528864), np.float64(0.858397902585306), np.float64(0.858397902585306), np.float64(0.8254514466262552), np.float64(0.8254514466262552), np.float64(0.8381795741429449), np.float64(0.8512816344642612), np.float64(0.8027272194529226), np.float64(0.816999426491996), np.float64(0.7822195812230723), np.float64(0.7822195812230723), np.float64(0.7828005978509781), np.float64(0.7828005978509781), np.float64(0.7931050999781284), np.float64(0.7931050999781284), np.float64(0.7931050999781284), np.float64(0.7834353009042275), np.float64(0.7834353009042275), np.float64(0.7817081629735488), np.float64(0.7817081629735488), np.float64(0.7817081629735488), np.float64(0.7866440020324943), np.float64(0.7866440020324944), np.float64(0.7827177409509557), np.float64(0.7917436392583966), np.float64(0.7955626832652686), np.float64(0.7952772146887747), np.float64(0.7952772146887747), np.float64(0.7952772146887747), np.float64(0.8029511436524612), np.float64(0.8029511436524612), np.float64(0.8104390352684939), np.float64(0.8104390352684939), np.float64(0.8130527538722201), np.float64(0.8162495319779681), np.float64(0.8076122929947479), np.float64(0.8142249130806528), np.float64(0.8055877185524334), np.float64(0.8000368701060598), np.float64(0.8010321554984217), np.float64(0.8004283528840301), np.float64(0.8044591521609964), np.float64(0.8100720854145802), np.float64(0.8152248975286164), np.float64(0.8141609499657702), np.float64(0.7966553173066676), np.float64(0.8019881967749501), np.float64(0.8066364976305359), np.float64(0.7988704245190456), np.float64(0.7953854105079695), np.float64(0.7980409227150376), np.float64(0.7952936595743041), np.float64(0.7996375943050927), np.float64(0.7996375943050927), np.float64(0.7996375943050928), np.float64(0.793141612967041), np.float64(0.7971304172540171), np.float64(0.7959559843935288), np.float64(0.7943875185521437), np.float64(0.7949073258203404), np.float64(0.7980212797252382), np.float64(0.7986470730514866), np.float64(0.7986470730514866), np.float64(0.8023628964991285), np.float64(0.791888683051672), np.float64(0.7938769263560924), np.float64(0.7952681248315058), np.float64(0.7949992787332644), np.float64(0.7944234553185034), np.float64(0.7974885793299926), np.float64(0.7919437308932147), np.float64(0.7951224007149714), np.float64(0.7942069575054894), np.float64(0.7975233008625752), np.float64(0.7994692094568934), np.float64(0.7957043747574775), np.float64(0.7957043747574775), np.float64(0.7987267065754726), np.float64(0.8012036341488463), np.float64(0.803836357083602), np.float64(0.7971501015007452), np.float64(0.7972054532124875), np.float64(0.7998906691343384), np.float64(0.8025201283359649), np.float64(0.8052622134770577), np.float64(0.807871566284238), np.float64(0.807751091920369), np.float64(0.8079221402778856), np.float64(0.8051521374039211), np.float64(0.8041843801958379), np.float64(0.8064342371918822), np.float64(0.8077093810795831), np.float64(0.8098107330085247), np.float64(0.8100478245873916), np.float64(0.809821253936501), np.float64(0.81067174857263), np.float64(0.8048763121355273), np.float64(0.8019940771284033), np.float64(0.801355874006115), np.float64(0.8035956070622297), np.float64(0.800687061548545), np.float64(0.8011902244940494), np.float64(0.8001392804335306), np.float64(0.8015454018908098), np.float64(0.8034806457546241), np.float64(0.8034806457546241), np.float64(0.8055445355237401), np.float64(0.8074621734779012), np.float64(0.8093725140852993), np.float64(0.8082673894339064), np.float64(0.8096206019431129), np.float64(0.8075458516693272), np.float64(0.7997053770073), np.float64(0.7982308988239478), np.float64(0.7985679256780839), np.float64(0.7975619589909092), np.float64(0.7967840162270624), np.float64(0.7977111533046395), np.float64(0.7994895496907733), np.float64(0.7960628743526283), np.float64(0.7949399568733696), np.float64(0.795535310475332), np.float64(0.7874681549451497), np.float64(0.789061866224945), np.float64(0.7909395282451981), np.float64(0.7924670967050977), np.float64(0.7933860746386082), np.float64(0.7944175636165354), np.float64(0.7938868736537102), np.float64(0.7956485609226752), np.float64(0.7973825183985767), np.float64(0.7984001135081588), np.float64(0.7984001135081588), np.float64(0.7948721373771546), np.float64(0.7920911971428074), np.float64(0.7924653009188394), np.float64(0.7880530550122749), np.float64(0.7890730128618646), np.float64(0.7894220777880633), np.float64(0.7895969689388971), np.float64(0.7844888502586631), np.float64(0.7856932071557889), np.float64(0.7816671808422556), np.float64(0.7833397917967484), np.float64(0.7841345932630468), np.float64(0.785046461798982), np.float64(0.7830415429273181), np.float64(0.782793171331501), np.float64(0.7812527685192571), np.float64(0.7808023709948219), np.float64(0.7787292801609729), np.float64(0.7767176031560384), np.float64(0.7782917682382248), np.float64(0.7776448042791394), np.float64(0.7787902929152668), np.float64(0.7757177682358576), np.float64(0.7771823229100207), np.float64(0.778613707279901), np.float64(0.7783117801260705), np.float64(0.7741746480222738), np.float64(0.7715526000450632), np.float64(0.7707929311077123), np.float64(0.7706906712088645), np.float64(0.7721177596949772), np.float64(0.771802628033657), np.float64(0.7733086629002982), np.float64(0.774797716832837), np.float64(0.7719006692867001), np.float64(0.772991954025816), np.float64(0.7740012813141536), np.float64(0.77450821068554), np.float64(0.773941117661023), np.float64(0.7735854301074954), np.float64(0.7749474287460028), np.float64(0.7715860757414498), np.float64(0.7725766334652849), np.float64(0.7734551550734767), np.float64(0.7747844851878575), np.float64(0.7717950089638611), np.float64(0.7726146884102074), np.float64(0.7721414079632346), np.float64(0.7684471654012149), np.float64(0.7689847917778208), np.float64(0.765964942019448), np.float64(0.7654166119487777), np.float64(0.7635136292388965), np.float64(0.7648753592571744), np.float64(0.7650949647802265), np.float64(0.7649189002892691), np.float64(0.7650306158191961), np.float64(0.7657604632758425), np.float64(0.765042622536288), np.float64(0.7657639808942039), np.float64(0.7656586953310519), np.float64(0.7636559290665846), np.float64(0.7642521396609755), np.float64(0.7645796556683183), np.float64(0.7610062145647094), np.float64(0.7621013951475585), np.float64(0.7595709081716444), np.float64(0.759082202327338), np.float64(0.7598055672588612), np.float64(0.7609739856695348), np.float64(0.7610532020267454), np.float64(0.7601764675859074), np.float64(0.7602178247661955), np.float64(0.761128501897347), np.float64(0.7623221261638178), np.float64(0.7614767750526622), np.float64(0.75693675003913), np.float64(0.7575034663232957), np.float64(0.7586639155798227), np.float64(0.7581747448158039), np.float64(0.7581992735121926), np.float64(0.7593279193971151), np.float64(0.7603165237488979), np.float64(0.761376926553412), np.float64(0.7617105889128024), np.float64(0.7625367123609689), np.float64(0.7627266728882043), np.float64(0.7616793316751747), np.float64(0.7612107457078162), np.float64(0.761165315885214), np.float64(0.7621043959712203), np.float64(0.7630641885058415), np.float64(0.7622158344696655), np.float64(0.7605681887282322), np.float64(0.7595951213498683), np.float64(0.7566264787733983), np.float64(0.7577542478012114), np.float64(0.7576669532311677), np.float64(0.7587323876764173), np.float64(0.7593015515983637), np.float64(0.760013632277662), np.float64(0.7608339503198576), np.float64(0.7618906447059088), np.float64(0.7600879605648323), np.float64(0.7586417487675075), np.float64(0.7576117242008716), np.float64(0.7540776748085545), np.float64(0.7549981359283415), np.float64(0.7552431899555193), np.float64(0.7558090294548733), np.float64(0.756657539496327), np.float64(0.7563524583905799), np.float64(0.7567469676674373), np.float64(0.7551750248047343), np.float64(0.7549468086835989), np.float64(0.755743055086039), np.float64(0.7545827890149993), np.float64(0.7548598381050099), np.float64(0.7538885989943475), np.float64(0.7543205502106204), np.float64(0.753645451411331), np.float64(0.7537951773201315), np.float64(0.7536821920180954), np.float64(0.7544070055485305), np.float64(0.755360093878474), np.float64(0.7561635389991077), np.float64(0.75642804483926), np.float64(0.756181772106362), np.float64(0.7571688804554675), np.float64(0.7559668399932452), np.float64(0.7569003285647435), np.float64(0.7569997290710794), np.float64(0.7575045275169422), np.float64(0.7580205285764713), np.float64(0.7557193013621758), np.float64(0.7551157502077427), np.float64(0.7557545698695317), np.float64(0.7556848982445348), np.float64(0.7543869097749953), np.float64(0.7552295855777388), np.float64(0.755517452462518)]</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 6, 7, 7, 8, 9, 10, 11, 12, 13, 14, 14, 15, 16, 17, 18, 19, 20, 20, 20, 20, 20, 21, 21, 22, 22, 22, 22, 22, 22, 23, 23, 24, 24, 25, 26, 26, 27, 27, 28, 29, 29, 30, 30, 30, 30, 30, 31, 32, 32, 33, 33, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 35, 36, 36, 36, 36, 36, 36, 36, 36, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 37, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 39, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40, 40]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>mixI</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>improve</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>181</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.6639151373343027</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.6573148348029541</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.029554302804490992), np.float64(0.029554302804490992), np.float64(0.029554302804490992), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.45645577546690086), np.float64(0.6366100333060568), np.float64(0.6366100333060568), np.float64(0.7197165508443744), np.float64(0.7197165508443744), np.float64(0.7197165508443744), np.float64(0.7197165508443744), np.float64(0.7197165508443744), np.float64(0.7744941415733653), np.float64(0.7744941415733653), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.7744941415733654), np.float64(0.8024568600715082), np.float64(0.8193498787068314), np.float64(0.8193498787068314), np.float64(0.8193498787068314), np.float64(0.7936099623560313), np.float64(0.7804361605062411), np.float64(0.7804361605062411), np.float64(0.7804361605062411), np.float64(0.7804361605062411), np.float64(0.7804361605062411), np.float64(0.7742639437656893), np.float64(0.7124664800466917), np.float64(0.7124664800466917), np.float64(0.7124664800466917), np.float64(0.7124664800466917), np.float64(0.6444545301972461), np.float64(0.6621521887275009), np.float64(0.6862755482545327), np.float64(0.6862755482545327), np.float64(0.6862755482545327), np.float64(0.6862755482545327), np.float64(0.6862755482545327), np.float64(0.6862755482545327), np.float64(0.6862755482545327), np.float64(0.6862755482545327), np.float64(0.7071114954973202), np.float64(0.7071114954973201), np.float64(0.7071114954973201), np.float64(0.7081065282144945), np.float64(0.7130979029358578), np.float64(0.6865588103443958), np.float64(0.6865588103443958), np.float64(0.6865588103443958), np.float64(0.6865588103443958), np.float64(0.6606788741634239), np.float64(0.660678874163424), np.float64(0.6565080882635954), np.float64(0.6688494420741234), np.float64(0.6712276512862677), np.float64(0.6712276512862677), np.float64(0.6712276512862677), np.float64(0.6712276512862677), np.float64(0.6712276512862677), np.float64(0.6594609685553993), np.float64(0.6594609685553993), np.float64(0.6594609685553993), np.float64(0.6524764715277661), np.float64(0.6502955167746023), np.float64(0.6502955167746023), np.float64(0.6418692860448463), np.float64(0.6418692860448463), np.float64(0.6551267027299865), np.float64(0.6551267027299865), np.float64(0.6551267027299865), np.float64(0.6551267027299865), np.float64(0.6551267027299865), np.float64(0.6366928707029935), np.float64(0.6399242314035312), np.float64(0.6430589058554254), np.float64(0.6468089085890488), np.float64(0.6511943415400905), np.float64(0.6237820161982319), np.float64(0.6237820161982319), np.float64(0.6122621826073003), np.float64(0.6122621826073003), np.float64(0.5943513451729403), np.float64(0.6055394758969537), np.float64(0.6151369933551604), np.float64(0.6057655132812603), np.float64(0.6057655132812603), np.float64(0.6057655132812603), np.float64(0.6057655132812603), np.float64(0.6120857570772448), np.float64(0.6121870015154053), np.float64(0.6196664850493195), np.float64(0.6204687155275976), np.float64(0.6204687155275976), np.float64(0.6218606580399719), np.float64(0.6218606580399719), np.float64(0.6218606580399719), np.float64(0.6218606580399719), np.float64(0.6218606580399719), np.float64(0.621860658039972), np.float64(0.621860658039972), np.float64(0.6303986544811891), np.float64(0.6382918244966417), np.float64(0.6390177658275775), np.float64(0.6390177658275775), np.float64(0.6390177658275775), np.float64(0.6390177658275775), np.float64(0.6466887181201801), np.float64(0.6492169651081585), np.float64(0.6492169651081585), np.float64(0.6534912565521002), np.float64(0.6386596140876623), np.float64(0.6386596140876623), np.float64(0.6395290851770492), np.float64(0.6395290851770492), np.float64(0.6212564083978417), np.float64(0.6049103809357653), np.float64(0.6072328258274667), np.float64(0.6072328258274667), np.float64(0.6072328258274667), np.float64(0.6072328258274667), np.float64(0.6122546445747409), np.float64(0.6150917830551224), np.float64(0.6150917830551224), np.float64(0.6150917830551224), np.float64(0.6150917830551224), np.float64(0.6053795825245611), np.float64(0.6053795825245611), np.float64(0.6121797077584702), np.float64(0.6121797077584702), np.float64(0.6123309608803942), np.float64(0.611788981061053), np.float64(0.6178758322093116), np.float64(0.6225834231962688), np.float64(0.6225834231962688), np.float64(0.6231890345993217), np.float64(0.6231890345993217), np.float64(0.6239919352105268), np.float64(0.6225820830795179), np.float64(0.6221104177689949), np.float64(0.6139862263039978), np.float64(0.6139862263039978), np.float64(0.6183896266697859), np.float64(0.609594040104419), np.float64(0.609594040104419), np.float64(0.609594040104419), np.float64(0.61096268290712), np.float64(0.61096268290712), np.float64(0.61096268290712), np.float64(0.612202289798128), np.float64(0.6175444665439837), np.float64(0.6215969086861042), np.float64(0.6221842148965501), np.float64(0.6221842148965501), np.float64(0.6271022465269047), np.float64(0.6271022465269049), np.float64(0.6215009553718893), np.float64(0.6262992193899725), np.float64(0.6310865624700589), np.float64(0.634770290202679), np.float64(0.6359527439134922), np.float64(0.6404381580033963), np.float64(0.6404381580033963), np.float64(0.6404381580033963), np.float64(0.635482162675961), np.float64(0.6379424420737749), np.float64(0.6379424420737749), np.float64(0.6364898859468989), np.float64(0.6399704835693439), np.float64(0.6399704835693439), np.float64(0.6399704835693439), np.float64(0.6416805037979881), np.float64(0.6348481961197892), np.float64(0.6381001125739787), np.float64(0.642165793880649), np.float64(0.642165793880649), np.float64(0.642165793880649), np.float64(0.642165793880649), np.float64(0.6456445209005006), np.float64(0.6493797350846806), np.float64(0.652921162827247), np.float64(0.6557146611317264), np.float64(0.6575688773345443), np.float64(0.6575688773345443), np.float64(0.6594112158409552), np.float64(0.659250966761551), np.float64(0.6627475018020685), np.float64(0.6601160591634514), np.float64(0.6601160591634514), np.float64(0.6601160591634514), np.float64(0.6601160591634514), np.float64(0.6556504155972941), np.float64(0.6548281233452952), np.float64(0.6570583195176385), np.float64(0.6559701063752049), np.float64(0.6591142256150578), np.float64(0.6591142256150578), np.float64(0.6622017188308583), np.float64(0.6637440254662332), np.float64(0.6637440254662332), np.float64(0.6669075364988977), np.float64(0.6681580573979685), np.float64(0.6681580573979685), np.float64(0.670196601747989), np.float64(0.6725861772939412), np.float64(0.6732525849703127), np.float64(0.6732525849703127), np.float64(0.6732525849703127), np.float64(0.6732525849703127), np.float64(0.6732525849703127), np.float64(0.6732525849703127), np.float64(0.6693452583650649), np.float64(0.6693452583650649), np.float64(0.6722618275779471), np.float64(0.6739429187438519), np.float64(0.6715252619072758), np.float64(0.6645796340632303), np.float64(0.6645796340632303), np.float64(0.6659787090116509), np.float64(0.6659787090116509), np.float64(0.6659787090116509), np.float64(0.6674352708506879), np.float64(0.6644233053812365)]</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 27, 28, 29, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 60, 61, 61, 62, 63, 64, 65, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 88, 88, 89, 90, 90, 90, 91, 92, 93, 94, 94, 94, 95, 96, 97, 97, 97, 97, 98, 99, 100, 101, 102, 103, 104, 104, 105, 106, 106, 106, 106, 107, 108, 109, 109, 110, 110, 110, 110, 111, 112, 113, 114, 114, 115, 116, 116, 116, 117, 117, 118, 118, 119, 120, 121, 122, 122, 122, 122, 122, 122, 122, 123, 123, 124, 124, 124, 124, 124, 125, 126, 127, 127, 127, 127, 127, 128, 128, 129, 130, 131, 132, 133, 134, 134, 134, 134, 135, 136, 137, 137, 137, 138, 138, 138, 139, 139, 140, 140, 140, 140, 141, 142, 143, 143, 143, 144, 145, 146, 146, 147, 147, 148, 148, 148, 148, 148, 149, 149, 150, 150, 150, 150, 150, 151, 151, 151, 152, 153, 153, 154, 155, 155, 155, 155, 155, 156, 156, 157, 157, 157, 157, 157, 157, 157, 158, 159, 159, 159, 160, 160, 160, 161, 162, 162, 162, 162, 162, 163, 164, 165, 165, 165, 165, 165, 165, 166, 166, 166, 166, 166, 167, 168, 169, 169, 169, 169, 169, 169, 170, 170, 170, 171, 171, 171, 172, 172, 172, 172, 173, 174, 175, 176, 177, 177, 178, 178, 178, 178, 178, 179, 179, 180, 181, 181, 181]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>mixI</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>improve</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>126</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.8163562733322213</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.8099926111126766</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.7614018926106864), np.float64(0.7614018926106864), np.float64(0.7614018926106864), np.float64(0.7614018926106864), np.float64(0.7614018926106864), np.float64(0.7614018926106864), np.float64(0.7614018926106864), np.float64(0.7614018926106864), np.float64(0.7614018926106864), np.float64(0.7614018926106864), np.float64(0.7614018926106864), np.float64(0.7614018926106864), np.float64(0.7614018926106864), np.float64(0.7614018926106864), np.float64(0.7614018926106864), np.float64(0.7171848385165247), np.float64(0.7171848385165247), np.float64(0.7171848385165247), np.float64(0.7171848385165247), np.float64(0.8002539734643394), np.float64(0.8002539734643394), np.float64(0.8002539734643394), np.float64(0.8002539734643394), np.float64(0.8443700020002071), np.float64(0.8443700020002071), np.float64(0.8443700020002071), np.float64(0.8443700020002071), np.float64(0.8443700020002072), np.float64(0.8443700020002072), np.float64(0.8672013041441311), np.float64(0.8672013041441311), np.float64(0.8672013041441311), np.float64(0.8672013041441311), np.float64(0.8672013041441311), np.float64(0.8672013041441311), np.float64(0.8672013041441311), np.float64(0.8672013041441311), np.float64(0.8672013041441311), np.float64(0.8753290142190066), np.float64(0.8753290142190066), np.float64(0.8753290142190066), np.float64(0.8753290142190066), np.float64(0.8753290142190066), np.float64(0.8753290142190066), np.float64(0.8285579566866863), np.float64(0.8413191841066704), np.float64(0.8413191841066704), np.float64(0.8413191841066704), np.float64(0.8413191841066704), np.float64(0.8413191841066704), np.float64(0.8413191841066704), np.float64(0.8413191841066704), np.float64(0.8413191841066704), np.float64(0.8413191841066704), np.float64(0.8084043753998804), np.float64(0.7934547713356539), np.float64(0.7934547713356539), np.float64(0.7934547713356539), np.float64(0.7934547713356539), np.float64(0.7934547713356538), np.float64(0.8003989836852429), np.float64(0.8003989836852429), np.float64(0.8003989836852429), np.float64(0.7699082366807595), np.float64(0.7699082366807595), np.float64(0.7699082366807595), np.float64(0.7699082366807595), np.float64(0.7699082366807595), np.float64(0.7849929232836106), np.float64(0.7849929232836106), np.float64(0.8001572832019102), np.float64(0.8114843976254448), np.float64(0.8114843976254448), np.float64(0.8114843976254448), np.float64(0.8114843976254448), np.float64(0.8114843976254444), np.float64(0.8114843976254444), np.float64(0.8114843976254444), np.float64(0.8114843976254444), np.float64(0.8114843976254444), np.float64(0.8114843976254444), np.float64(0.8114843976254444), np.float64(0.8148816419182827), np.float64(0.8148816419182827), np.float64(0.8093234726252808), np.float64(0.8157272822569948), np.float64(0.8027297689634357), np.float64(0.8027297689634357), np.float64(0.8027297689634357), np.float64(0.7781091856857427), np.float64(0.7781091856857427), np.float64(0.7871144258190202), np.float64(0.7958550002048898), np.float64(0.7958550002048898), np.float64(0.8045656845197202), np.float64(0.8045656845197202), np.float64(0.8058115216898677), np.float64(0.8084833046334645), np.float64(0.8084833046334645), np.float64(0.8084833046334645), np.float64(0.8022493334284188), np.float64(0.8022493334284188), np.float64(0.8035171767186369), np.float64(0.8035171767186369), np.float64(0.8097661696434099), np.float64(0.8097661696434099), np.float64(0.8097661696434099), np.float64(0.798914083483189), np.float64(0.7969590522297813), np.float64(0.7969590522297813), np.float64(0.795624647068252), np.float64(0.795624647068252), np.float64(0.8011851188431901), np.float64(0.8011851188431901), np.float64(0.8011851188431901), np.float64(0.8072068370443133), np.float64(0.8072068370443133), np.float64(0.8058098295014566), np.float64(0.8058098295014566), np.float64(0.8058098295014566), np.float64(0.8058098295014566), np.float64(0.8058098295014566), np.float64(0.8058098295014566), np.float64(0.8111121475792485), np.float64(0.8065810758795134), np.float64(0.808385503122399), np.float64(0.8074905454829655), np.float64(0.8074905454829655), np.float64(0.8074905454829655), np.float64(0.8122901239499801), np.float64(0.8122901239499801), np.float64(0.8122901239499802), np.float64(0.8122901239499802), np.float64(0.8122901239499802), np.float64(0.8122901239499802), np.float64(0.814439959756508), np.float64(0.8143155812238496), np.float64(0.81234162935352), np.float64(0.8109397020278332), np.float64(0.8109397020278333), np.float64(0.8106513991352557), np.float64(0.8106513991352557), np.float64(0.811143000293224), np.float64(0.8006401428741432), np.float64(0.8006401428741432), np.float64(0.8006401428741432), np.float64(0.8006401428741432), np.float64(0.8006401428741432), np.float64(0.804614474661733), np.float64(0.804614474661733), np.float64(0.805289384990152), np.float64(0.8085940991408098), np.float64(0.8074598733766988), np.float64(0.8074598733766988), np.float64(0.8107592130707864), np.float64(0.8139020059389416), np.float64(0.815376334805612), np.float64(0.815376334805612), np.float64(0.8079334422967401), np.float64(0.8079334422967401), np.float64(0.8079334422967401), np.float64(0.8079721255265422), np.float64(0.8107716528514499), np.float64(0.8117842748465983), np.float64(0.8095504795941941), np.float64(0.8059432881089654), np.float64(0.8059432881089654), np.float64(0.8055958428959009), np.float64(0.8086039409762319), np.float64(0.8086039409762319), np.float64(0.8116456380800835), np.float64(0.8083301769339077), np.float64(0.809977536323725), np.float64(0.8128922292266592), np.float64(0.8128922292266592), np.float64(0.8146364564811761), np.float64(0.816615613355894), np.float64(0.8157592775134099), np.float64(0.8137410402942201), np.float64(0.8137410402942201), np.float64(0.8161871759574325), np.float64(0.8161871759574325), np.float64(0.8178666959510305), np.float64(0.8195401174847237), np.float64(0.8210524232796311), np.float64(0.8210047887934759), np.float64(0.817076228145228), np.float64(0.817076228145228), np.float64(0.8194830779834646), np.float64(0.8209764779113244), np.float64(0.8213759595817773), np.float64(0.8182160772967292), np.float64(0.8173260738724485), np.float64(0.8175359017119358), np.float64(0.819475011132557), np.float64(0.8176433046519469), np.float64(0.816663650501069), np.float64(0.8177720029267468), np.float64(0.8193454367827809), np.float64(0.8175714260006388), np.float64(0.8194416992858309), np.float64(0.8194416992858309), np.float64(0.821458237375787), np.float64(0.8214582373757868), np.float64(0.8214582373757868), np.float64(0.819396871791021), np.float64(0.819396871791021), np.float64(0.8201745854061281), np.float64(0.8213974594094723), np.float64(0.8226715856558955), np.float64(0.819093166934091), np.float64(0.8179694257141573), np.float64(0.819423650656398), np.float64(0.8211930907584625), np.float64(0.8203405720513601), np.float64(0.819966123986861), np.float64(0.8154644175007444), np.float64(0.8113148304122516), np.float64(0.8112675921253699), np.float64(0.8130993197150297), np.float64(0.8141289779461355), np.float64(0.8141696429294487), np.float64(0.8157547403489103), np.float64(0.8144846450968518), np.float64(0.8120424632894414), np.float64(0.8135462482867906), np.float64(0.8135386844092194), np.float64(0.8143093836235298), np.float64(0.8102679706741286), np.float64(0.8119223612972072), np.float64(0.8109050140457992), np.float64(0.8099719010116874), np.float64(0.8099719010116874), np.float64(0.8099283280899966), np.float64(0.8103755794995481), np.float64(0.8099744560529867), np.float64(0.8108787272955584), np.float64(0.8087122665745007), np.float64(0.8102880906632541), np.float64(0.8088094825995739), np.float64(0.8087053985791862), np.float64(0.8102339454037969), np.float64(0.8111452934099572), np.float64(0.8075163451030446), np.float64(0.8075163451030446), np.float64(0.8089046901415291), np.float64(0.8078537380964619), np.float64(0.807984946715885), np.float64(0.807984946715885), np.float64(0.8094365370028926), np.float64(0.810441951861814), np.float64(0.8110876224180922), np.float64(0.8076980435139245), np.float64(0.8046508445077236), np.float64(0.8054748948877966), np.float64(0.8064451267783977), np.float64(0.8078572913725214), np.float64(0.8064235127319531), np.float64(0.8077861510605293), np.float64(0.8060215443224972), np.float64(0.8060215443224972), np.float64(0.8050965741428959), np.float64(0.8064259468141451), np.float64(0.8064259468141451), np.float64(0.8063099872977693), np.float64(0.807262064733326), np.float64(0.808586094808935), np.float64(0.8089555359922902), np.float64(0.8074219349263262), np.float64(0.808105092866759), np.float64(0.8083587153797577), np.float64(0.8089482686782984), np.float64(0.8099464090888129), np.float64(0.808957303544611), np.float64(0.8093357994046172), np.float64(0.8089958421595722), np.float64(0.8069988143574346), np.float64(0.8082352496990964), np.float64(0.8094551938671273), np.float64(0.8092576892512117), np.float64(0.8104564580792037), np.float64(0.8116279209812814), np.float64(0.8127489220231121), np.float64(0.81390394356144), np.float64(0.8142212298163359), np.float64(0.8151088208518886), np.float64(0.8148435348576971), np.float64(0.8158486367356806), np.float64(0.8151373260736383), np.float64(0.8159499247754528), np.float64(0.816249807085452), np.float64(0.8160797452999411), np.float64(0.8151680717313793), np.float64(0.8150507046025215), np.float64(0.8159225840109856)]</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 18, 19, 20, 21, 21, 22, 23, 24, 24, 25, 26, 27, 28, 29, 29, 30, 31, 32, 33, 34, 35, 36, 37, 37, 38, 39, 40, 41, 42, 42, 42, 43, 44, 45, 46, 47, 48, 49, 50, 50, 50, 51, 52, 53, 54, 54, 55, 56, 56, 57, 58, 59, 60, 60, 61, 61, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 71, 72, 72, 72, 72, 73, 74, 74, 75, 75, 75, 76, 76, 77, 77, 77, 78, 79, 79, 80, 80, 81, 81, 82, 83, 83, 83, 84, 84, 85, 85, 86, 87, 87, 88, 88, 89, 90, 91, 92, 93, 93, 93, 93, 93, 94, 95, 95, 96, 97, 98, 99, 100, 100, 100, 100, 100, 101, 101, 102, 102, 102, 103, 104, 105, 106, 106, 107, 107, 107, 107, 108, 108, 108, 108, 109, 109, 110, 111, 111, 111, 111, 111, 111, 112, 112, 112, 113, 113, 113, 113, 113, 114, 114, 114, 114, 114, 115, 115, 116, 116, 116, 116, 116, 116, 117, 117, 117, 117, 117, 117, 117, 117, 117, 117, 117, 117, 117, 117, 118, 118, 119, 120, 120, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 122, 122, 122, 122, 122, 122, 122, 122, 122, 122, 122, 122, 123, 123, 123, 123, 124, 124, 124, 124, 124, 124, 124, 124, 124, 124, 124, 124, 125, 125, 125, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126, 126]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>mixI</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>improve</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>68</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.7229592435687394</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.7234327479535303</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.9435628445321025), np.float64(0.9435628445321025), np.float64(0.9435628445321025), np.float64(0.9435628445321025), np.float64(0.9082599794131795), np.float64(0.9082599794131795), np.float64(0.870679856961511), np.float64(0.7064312573902944), np.float64(0.7064312573902944), np.float64(0.7064312573902944), np.float64(0.7064312573902944), np.float64(0.748321271848646), np.float64(0.6858787343985244), np.float64(0.7298928408128351), np.float64(0.7298928408128351), np.float64(0.7298928408128351), np.float64(0.7298928408128351), np.float64(0.7298928408128351), np.float64(0.729892840812835), np.float64(0.665691774186129), np.float64(0.6189673070553381), np.float64(0.6568101761439101), np.float64(0.6568101761439101), np.float64(0.6568101761439101), np.float64(0.6568101761439101), np.float64(0.6858164329716856), np.float64(0.7072067572214378), np.float64(0.7072067572214378), np.float64(0.7099764921373851), np.float64(0.7304500616726219), np.float64(0.7480994422925158), np.float64(0.7607150960414951), np.float64(0.7607150960414951), np.float64(0.7644179443584347), np.float64(0.7772672665553265), np.float64(0.7772672665553265), np.float64(0.7772672665553265), np.float64(0.7601449159473322), np.float64(0.7709371044859159), np.float64(0.7473782503859897), np.float64(0.7473782503859897), np.float64(0.7488393472792929), np.float64(0.7574045876687932), np.float64(0.7574045876687932), np.float64(0.7574045876687932), np.float64(0.7674874723711668), np.float64(0.7674874723711668), np.float64(0.7763753826320243), np.float64(0.7763753826320243), np.float64(0.7763753826320243), np.float64(0.7763753826320243), np.float64(0.7829304793883269), np.float64(0.7788030260607859), np.float64(0.7788030260607859), np.float64(0.7733214963588255), np.float64(0.7733214963588255), np.float64(0.7810103136569464), np.float64(0.7744673465688178), np.float64(0.7744673465688178), np.float64(0.7566962774069705), np.float64(0.7566962774069705), np.float64(0.7346418136746773), np.float64(0.7248965424195932), np.float64(0.7309714149037854), np.float64(0.7146897202859651), np.float64(0.7058363489059298), np.float64(0.706961378508707), np.float64(0.706961378508707), np.float64(0.7114425531333958), np.float64(0.7095965607720391), np.float64(0.7095965607720391), np.float64(0.7080058440710776), np.float64(0.7137940012322966), np.float64(0.7041080805650618), np.float64(0.6956108897265021), np.float64(0.6956108897265021), np.float64(0.6956108897265021), np.float64(0.6870357354988732), np.float64(0.6902517200151759), np.float64(0.6965938343421729), np.float64(0.6965938343421729), np.float64(0.6965938343421729), np.float64(0.7030451534630401), np.float64(0.7000792673493076), np.float64(0.7060568718232213), np.float64(0.7101417105690733), np.float64(0.703494719053722), np.float64(0.7069382536434821), np.float64(0.7118532375793143), np.float64(0.7023822322428762), np.float64(0.6955162104912724), np.float64(0.6955162104912724), np.float64(0.6955162104912724), np.float64(0.6992294165334385), np.float64(0.6954618751957774), np.float64(0.6954618751957774), np.float64(0.6954618751957774), np.float64(0.6909780280226602), np.float64(0.695410735990402), np.float64(0.7003400633632406), np.float64(0.7036993566866897), np.float64(0.7022023683341467), np.float64(0.7019596713821161), np.float64(0.7004446161595309), np.float64(0.7003674326155412), np.float64(0.702536378543467), np.float64(0.7069428186253042), np.float64(0.7042018865823834), np.float64(0.7033056199583057), np.float64(0.7033056199583057), np.float64(0.7054589386456377), np.float64(0.7069524844599867), np.float64(0.7109466414316097), np.float64(0.7101434755670238), np.float64(0.7086582491494982), np.float64(0.7087983643322925), np.float64(0.7116754797996453), np.float64(0.7150487370632558), np.float64(0.7150487370632558), np.float64(0.7131412469303028), np.float64(0.7083957736582287), np.float64(0.7109530285721399), np.float64(0.7143340194300871), np.float64(0.7176319595094077), np.float64(0.7200093171645994), np.float64(0.7211420808521292), np.float64(0.724215518508828), np.float64(0.7268407205634309), np.float64(0.7267485095592415), np.float64(0.724146198072822), np.float64(0.7234660990668702), np.float64(0.7265049383533732), np.float64(0.726111388254249), np.float64(0.7290739114120525), np.float64(0.7307940998398076), np.float64(0.7334145905595767), np.float64(0.7322990672244154), np.float64(0.735017947932309), np.float64(0.7305492031202466), np.float64(0.7294677060722209), np.float64(0.7265369073240808), np.float64(0.7224007098618156), np.float64(0.7247154327577033), np.float64(0.7247154327577033), np.float64(0.7247154327577033), np.float64(0.7274104889994537), np.float64(0.7285396794177336), np.float64(0.7290464422402606), np.float64(0.7316268344148354), np.float64(0.7340552214785714), np.float64(0.7352561079200127), np.float64(0.7355287768631213), np.float64(0.7375596257720314), np.float64(0.7357451772742101), np.float64(0.7300039097625549), np.float64(0.7300039097625549), np.float64(0.7273568849696682), np.float64(0.7281081131000949), np.float64(0.7276358703584419), np.float64(0.7285211663362589), np.float64(0.7298641566765298), np.float64(0.7287328924801597), np.float64(0.7287328924801597), np.float64(0.7306128612083042), np.float64(0.7262780957896965), np.float64(0.7262624656856468), np.float64(0.7284277241144966), np.float64(0.7274488855707626), np.float64(0.7295350041506793), np.float64(0.7317093966571148), np.float64(0.733667945360857), np.float64(0.7286149329738968), np.float64(0.726379375255583), np.float64(0.7284420286858364), np.float64(0.7258400335621799), np.float64(0.7255853461291637), np.float64(0.7243587967093891), np.float64(0.7207769857173594), np.float64(0.7167354526861464), np.float64(0.7186706595699887), np.float64(0.7172843228431935), np.float64(0.7193627227745374), np.float64(0.7167249511617736), np.float64(0.7158476888715342), np.float64(0.7176174644455232), np.float64(0.7156009205160061), np.float64(0.715480161186444), np.float64(0.7169133926514487), np.float64(0.7183554886570566), np.float64(0.7171782631740893), np.float64(0.7122044499058262), np.float64(0.7139829894254415), np.float64(0.7135890586722994), np.float64(0.7153490348256779), np.float64(0.7171717002463763), np.float64(0.7138441393131959), np.float64(0.7105924905297086), np.float64(0.7124762837108027), np.float64(0.7105611533852451), np.float64(0.712439951149056), np.float64(0.7141678564395453), np.float64(0.714726157513061), np.float64(0.7164118491636042), np.float64(0.7160965601083975), np.float64(0.7115713249803104), np.float64(0.7132328638260361), np.float64(0.7145549007375342), np.float64(0.7145549007375342), np.float64(0.7136041008434646), np.float64(0.7134386385237396), np.float64(0.7124138521275873), np.float64(0.7083182841796003), np.float64(0.7045632063474558), np.float64(0.7054781642034116), np.float64(0.706484727541232), np.float64(0.7074273991356553), np.float64(0.7064191838340838), np.float64(0.705788936089892), np.float64(0.7073092402292019), np.float64(0.707871592106192), np.float64(0.705922746818592), np.float64(0.7064161229940026), np.float64(0.7079187737490431), np.float64(0.7088777299624442), np.float64(0.7082246292222122), np.float64(0.7096826292974812), np.float64(0.7090549624687534), np.float64(0.7099342467767426), np.float64(0.7114665165259844), np.float64(0.7130121476797167), np.float64(0.712439717641869), np.float64(0.7139341453507744), np.float64(0.7128244806014605), np.float64(0.7136352014624264), np.float64(0.7148367777898655), np.float64(0.7163154214357684), np.float64(0.7158179187965963), np.float64(0.7171709431020334), np.float64(0.7160679665831794), np.float64(0.716010054881464), np.float64(0.7157311840192726), np.float64(0.7162373803613663), np.float64(0.7176800398947446), np.float64(0.7184900316706229), np.float64(0.7193243066688466), np.float64(0.7186616692139547), np.float64(0.719876125892508), np.float64(0.7197924256765283), np.float64(0.7191699303341296), np.float64(0.7181948071897423), np.float64(0.7187870787759543), np.float64(0.7172990119717957), np.float64(0.7178219923302465), np.float64(0.7187952423399232), np.float64(0.7180372228819676), np.float64(0.7176372604436638), np.float64(0.7159516302713993), np.float64(0.7155442717862905), np.float64(0.7168852013205222), np.float64(0.7181899199786238), np.float64(0.7194690671542584), np.float64(0.719769491448115), np.float64(0.7194570940801726), np.float64(0.71847398375133), np.float64(0.7191942526186477), np.float64(0.7196146035915999), np.float64(0.7208743309200213), np.float64(0.7191570723611571), np.float64(0.7199670169373634), np.float64(0.7212227409703775), np.float64(0.722328325540344), np.float64(0.7231668198681772), np.float64(0.7210242897253263), np.float64(0.7205938987900283), np.float64(0.7204982443536648), np.float64(0.7216753072919198), np.float64(0.72287121177623), np.float64(0.724069026236367)]</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 21, 22, 23, 24, 24, 25, 25, 25, 26, 27, 28, 28, 28, 28, 29, 30, 31, 32, 33, 33, 33, 33, 34, 35, 36, 36, 36, 37, 37, 37, 37, 37, 38, 38, 38, 39, 40, 40, 40, 40, 41, 41, 41, 42, 43, 43, 44, 44, 45, 46, 47, 47, 47, 48, 48, 49, 49, 49, 50, 50, 51, 51, 51, 51, 51, 51, 51, 52, 52, 52, 53, 53, 53, 53, 53, 54, 55, 55, 55, 55, 56, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 58, 59, 59, 59, 60, 61, 61, 61, 61, 61, 61, 61, 61, 61, 61, 61, 61, 61, 62, 62, 62, 62, 62, 62, 62, 62, 62, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 64, 65, 65, 65, 65, 65, 65, 65, 65, 65, 65, 65, 66, 66, 66, 66, 66, 66, 66, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 67, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68]</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>mixII</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>improve</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>116</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.7216159970849434</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.6759130059294983</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.9797843895118907), np.float64(0.9797843895118907), np.float64(0.2927672409434795), np.float64(0.2927672409434795), np.float64(0.2927672409434795), np.float64(0.2927672409434795), np.float64(0.5115956296972458), np.float64(0.5115956296972458), np.float64(0.6207757025110822), np.float64(0.6207757025110822), np.float64(0.6207757025110822), np.float64(0.588893144837389), np.float64(0.588893144837389), np.float64(0.6574109515169105), np.float64(0.6574109515169105), np.float64(0.5069505089112132), np.float64(0.5420310716834609), np.float64(0.47633344229463287), np.float64(0.516804308903461), np.float64(0.516804308903461), np.float64(0.516804308903461), np.float64(0.516804308903461), np.float64(0.516804308903461), np.float64(0.516804308903461), np.float64(0.556567565810055), np.float64(0.556567565810055), np.float64(0.556567565810055), np.float64(0.556567565810055), np.float64(0.5932323301314105), np.float64(0.5962034589270115), np.float64(0.5962034589270115), np.float64(0.5962034589270115), np.float64(0.5962034589270115), np.float64(0.5962034589270115), np.float64(0.5962034589270115), np.float64(0.5962034589270115), np.float64(0.5962034589270115), np.float64(0.5954067202077905), np.float64(0.5954067202077905), np.float64(0.5954067202077906), np.float64(0.5954067202077906), np.float64(0.5954067202077906), np.float64(0.6136705469313765), np.float64(0.6304343210068553), np.float64(0.6304343210068553), np.float64(0.6423780499046484), np.float64(0.6423780499046484), np.float64(0.6423780499046484), np.float64(0.6423780499046484), np.float64(0.6423780499046484), np.float64(0.6492263496768245), np.float64(0.6607664580661151), np.float64(0.6607664580661151), np.float64(0.6607664580661151), np.float64(0.6607664580661151), np.float64(0.6607664580661151), np.float64(0.6607664580661151), np.float64(0.6607664580661151), np.float64(0.6607664580661151), np.float64(0.6776056702421884), np.float64(0.6776056702421884), np.float64(0.6782794588792492), np.float64(0.6729919719222286), np.float64(0.6729919719222285), np.float64(0.6871771758147033), np.float64(0.6949425154672028), np.float64(0.6820343605932652), np.float64(0.6937928664817832), np.float64(0.6937928664817832), np.float64(0.6961633687621972), np.float64(0.6878864745599564), np.float64(0.6862568549678458), np.float64(0.6862568549678458), np.float64(0.6862568549678458), np.float64(0.6958363623072578), np.float64(0.7000475799919729), np.float64(0.7000475799919729), np.float64(0.7073289943254674), np.float64(0.7073289943254674), np.float64(0.7161976838882368), np.float64(0.7169389806229154), np.float64(0.7246382388288365), np.float64(0.7246382388288365), np.float64(0.7182074916113097), np.float64(0.7205552401514126), np.float64(0.7176566201333758), np.float64(0.7176566201333758), np.float64(0.7176566201333759), np.float64(0.7176566201333759), np.float64(0.7196506477647089), np.float64(0.7196506477647089), np.float64(0.7196506477647089), np.float64(0.7192398081146997), np.float64(0.726020986909259), np.float64(0.7271993653058876), np.float64(0.7215149171861497), np.float64(0.7039272345517513), np.float64(0.7096289366063802), np.float64(0.7105323188925758), np.float64(0.6903534822985842), np.float64(0.6956232874099614), np.float64(0.6956232874099614), np.float64(0.6956232874099614), np.float64(0.7011102253888769), np.float64(0.7041995126064576), np.float64(0.7099469804207682), np.float64(0.7117475863718371), np.float64(0.7152953207723227), np.float64(0.710190889400686), np.float64(0.710190889400686), np.float64(0.710190889400686), np.float64(0.710190889400686), np.float64(0.7085822725083915), np.float64(0.7085822725083915), np.float64(0.7136626696760702), np.float64(0.7136626696760702), np.float64(0.7177996323459217), np.float64(0.7177996323459217), np.float64(0.7133430199213499), np.float64(0.6981798848295204), np.float64(0.6981798848295204), np.float64(0.7031031461420254), np.float64(0.7079577875997671), np.float64(0.7079577875997671), np.float64(0.7103321582989287), np.float64(0.7147965464395764), np.float64(0.7147965464395764), np.float64(0.7108134800452081), np.float64(0.7108134800452081), np.float64(0.7128526251066827), np.float64(0.7128526251066827), np.float64(0.7155254310104587), np.float64(0.7102114268632235), np.float64(0.7118584158507419), np.float64(0.7115930620621721), np.float64(0.7115930620621721), np.float64(0.712643306831952), np.float64(0.71468398208487), np.float64(0.7127744390831237), np.float64(0.7159057386763055), np.float64(0.7196866126490251), np.float64(0.7202547853486189), np.float64(0.7190225824946722), np.float64(0.721605875450603), np.float64(0.721605875450603), np.float64(0.721605875450603), np.float64(0.7244195725336611), np.float64(0.7254710959277998), np.float64(0.7254710959277998), np.float64(0.728274351156767), np.float64(0.7229750237221958), np.float64(0.7251474308050193), np.float64(0.7284482719612252), np.float64(0.7271168405046281), np.float64(0.72031443893153), np.float64(0.72031443893153), np.float64(0.7190305491079783), np.float64(0.714107325596018), np.float64(0.714107325596018), np.float64(0.7104087275000412), np.float64(0.7136454837725181), np.float64(0.7136454837725181), np.float64(0.7157016686111665), np.float64(0.7157016686111665), np.float64(0.7167091614357765), np.float64(0.7167091614357765), np.float64(0.7167091614357765), np.float64(0.7167091614357765), np.float64(0.7142523271814778), np.float64(0.7079189540441101), np.float64(0.7079189540441101), np.float64(0.7109950126839857), np.float64(0.7109950126839857), np.float64(0.7109950126839857), np.float64(0.7084113825649135), np.float64(0.7107266832038611), np.float64(0.7107266832038611), np.float64(0.7107266832038611), np.float64(0.7082955825203586), np.float64(0.7077735340545901), np.float64(0.7077735340545901), np.float64(0.7102782585177104), np.float64(0.7049884289847244), np.float64(0.707227980399573), np.float64(0.707227980399573), np.float64(0.7100868284589897), np.float64(0.7116339038964499), np.float64(0.7116339038964499), np.float64(0.7136341075885616), np.float64(0.7118395120261136), np.float64(0.7083951650307622), np.float64(0.7083951650307624), np.float64(0.7087452384405466), np.float64(0.7112738033905751), np.float64(0.711169210456109), np.float64(0.7088732331967086), np.float64(0.7114910970653225), np.float64(0.7120413985951934), np.float64(0.713604531966724), np.float64(0.7159901054127074), np.float64(0.7159901054127074), np.float64(0.7184396119729464), np.float64(0.7208508655225675), np.float64(0.72275860379047), np.float64(0.7239641722275897), np.float64(0.7261683257828043), np.float64(0.7279398902951896), np.float64(0.7279398902951895), np.float64(0.7275962656188664), np.float64(0.7275962656188664), np.float64(0.7282602109679812), np.float64(0.7300515997534872), np.float64(0.7299778421660352), np.float64(0.7267713724175051), np.float64(0.7272478979731414), np.float64(0.7292362149233034), np.float64(0.7305729163659519), np.float64(0.7314382881037967), np.float64(0.7314382881037967), np.float64(0.7264678708284791), np.float64(0.728249695563811), np.float64(0.730026241844849), np.float64(0.7271361238860905), np.float64(0.7286678515512743), np.float64(0.729478951973815), np.float64(0.7255855047875286), np.float64(0.7275402020252947), np.float64(0.729103171849446), np.float64(0.7269859255145866), np.float64(0.7272979820511517), np.float64(0.7272979820511517), np.float64(0.7277864510875504), np.float64(0.729700765550531), np.float64(0.7266033995952403), np.float64(0.7243783101429743), np.float64(0.7256000265564592), np.float64(0.7271292405096872), np.float64(0.728586827820387), np.float64(0.7263049840700624), np.float64(0.7268542425599445), np.float64(0.7284796270137814), np.float64(0.7258625896868808), np.float64(0.7274863003674292), np.float64(0.7221268369515107), np.float64(0.721334199810655), np.float64(0.721086943930938), np.float64(0.7219251291742363), np.float64(0.7219251291742363), np.float64(0.719943247972204), np.float64(0.717274484578021), np.float64(0.716542094783561), np.float64(0.7182642741711153), np.float64(0.7180023642186606), np.float64(0.7180023642186606), np.float64(0.7193981210129596), np.float64(0.7204012067354525), np.float64(0.7204012067354525), np.float64(0.7209797930377855), np.float64(0.7209797930377855), np.float64(0.7209797930377855), np.float64(0.7209797930377855), np.float64(0.7226705911547859), np.float64(0.7236819754005716), np.float64(0.7238170395129008), np.float64(0.7228182111412017), np.float64(0.7218301009944181), np.float64(0.7218450493679628), np.float64(0.7226369124925278), np.float64(0.7210707411637576), np.float64(0.7226367033336277), np.float64(0.7207029193299916), np.float64(0.7220500233108753), np.float64(0.7220500233108753), np.float64(0.719596940689173), np.float64(0.7198283678551121), np.float64(0.7204082642782474), np.float64(0.7217450694663275), np.float64(0.7225085586626024), np.float64(0.7204388013568079), np.float64(0.7195568583863647), np.float64(0.7195568583863647), np.float64(0.720162455419041), np.float64(0.720162455419041)]</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 16, 17, 17, 18, 19, 20, 20, 21, 21, 22, 23, 23, 24, 24, 25, 25, 25, 25, 25, 26, 27, 28, 29, 30, 30, 31, 32, 33, 33, 33, 34, 35, 36, 37, 38, 39, 40, 40, 41, 42, 43, 44, 44, 44, 45, 45, 46, 47, 48, 49, 49, 49, 50, 51, 52, 53, 54, 55, 56, 56, 57, 57, 57, 58, 58, 58, 58, 58, 59, 59, 59, 59, 60, 61, 61, 61, 62, 62, 63, 63, 63, 63, 64, 64, 64, 64, 65, 66, 67, 67, 68, 69, 69, 69, 69, 69, 69, 69, 69, 69, 69, 70, 71, 71, 71, 71, 71, 71, 71, 72, 73, 74, 74, 75, 75, 76, 76, 77, 77, 77, 78, 78, 78, 79, 79, 79, 80, 80, 81, 81, 82, 82, 82, 82, 82, 83, 83, 83, 83, 83, 83, 83, 83, 83, 84, 85, 85, 85, 86, 86, 86, 86, 86, 86, 86, 87, 87, 87, 88, 88, 88, 89, 89, 90, 90, 91, 92, 93, 93, 93, 94, 94, 95, 96, 96, 96, 97, 98, 98, 98, 99, 99, 99, 99, 100, 100, 100, 101, 101, 101, 101, 102, 102, 102, 102, 102, 102, 102, 102, 102, 103, 103, 103, 103, 103, 103, 103, 104, 104, 105, 105, 105, 105, 105, 105, 105, 105, 105, 106, 106, 106, 106, 106, 106, 106, 106, 106, 106, 106, 106, 107, 107, 107, 107, 107, 107, 107, 107, 107, 107, 107, 107, 107, 107, 107, 107, 107, 108, 108, 108, 108, 108, 108, 109, 109, 109, 110, 110, 111, 112, 113, 113, 113, 113, 113, 113, 113, 113, 113, 113, 113, 113, 114, 114, 114, 114, 114, 114, 114, 114, 115, 115, 116]</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>mixII</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>improve</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>63</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.4034908979272998</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.4089644959772276</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.7313489049967915), np.float64(-0.07699813164334979), np.float64(-0.07699813164334979), np.float64(-0.07699813164334979), np.float64(-0.2706265198314451), np.float64(0.04315947678765539), np.float64(0.04315947678765539), np.float64(0.04315947678765539), np.float64(0.04315947678765539), np.float64(0.22527392394446233), np.float64(0.22527392394446233), np.float64(0.22527392394446233), np.float64(0.35166555400711125), np.float64(0.35166555400711125), np.float64(0.43468365670912473), np.float64(0.36309227710398057), np.float64(0.3503612015417457), np.float64(0.3503612015417457), np.float64(0.24933746448379696), np.float64(0.24933746448379696), np.float64(0.3089282946136068), np.float64(0.36266953708902655), np.float64(0.36266953708902655), np.float64(0.3881618487153905), np.float64(0.3881618487153905), np.float64(0.31161511178424034), np.float64(0.31099574181482664), np.float64(0.32148214800235686), np.float64(0.32148214800235686), np.float64(0.29955054891641386), np.float64(0.2591266553831674), np.float64(0.2847384439221849), np.float64(0.3022106671372705), np.float64(0.3347288602376643), np.float64(0.3594252047696514), np.float64(0.3594252047696513), np.float64(0.3170632359547085), np.float64(0.33339616693346413), np.float64(0.36004736411359906), np.float64(0.37123835874609384), np.float64(0.32758615772278227), np.float64(0.3468095550194271), np.float64(0.3468095550194271), np.float64(0.3218274034405205), np.float64(0.33309735668572593), np.float64(0.3450359483718463), np.float64(0.3332079474214558), np.float64(0.3332079474214558), np.float64(0.3520896739943615), np.float64(0.3520896739943615), np.float64(0.3520896739943615), np.float64(0.3520896739943615), np.float64(0.3480873819413748), np.float64(0.3480873819413748), np.float64(0.32916913312476764), np.float64(0.322862369519876), np.float64(0.322862369519876), np.float64(0.3398303517741525), np.float64(0.3383148967496913), np.float64(0.3491436743157664), np.float64(0.36253516730371105), np.float64(0.36253516730371105), np.float64(0.3778040832234304), np.float64(0.3923384863529523), np.float64(0.37419134882954636), np.float64(0.37419134882954636), np.float64(0.37419134882954636), np.float64(0.38814065103257395), np.float64(0.400399190060611), np.float64(0.41340562471075687), np.float64(0.41513364933725433), np.float64(0.4272910125975548), np.float64(0.4272910125975548), np.float64(0.42958303065176207), np.float64(0.41863490803947173), np.float64(0.4298335711428632), np.float64(0.4298335711428632), np.float64(0.43471889000574654), np.float64(0.434410724949108), np.float64(0.4272016055419409), np.float64(0.4305108068538653), np.float64(0.4235983592058191), np.float64(0.4333826797114828), np.float64(0.43967821985530847), np.float64(0.44901390806770086), np.float64(0.440258475894173), np.float64(0.448823827942079), np.float64(0.448823827942079), np.float64(0.4312288679035612), np.float64(0.43898573117819156), np.float64(0.4248117060218814), np.float64(0.43209178894496314), np.float64(0.44066267989139773), np.float64(0.44066267989139773), np.float64(0.4393492526301799), np.float64(0.4449909210935975), np.float64(0.45217601360790427), np.float64(0.45815761734524896), np.float64(0.4418821449291877), np.float64(0.44663077820084873), np.float64(0.4388212287310726), np.float64(0.43049475975137436), np.float64(0.43316034242126117), np.float64(0.43316034242126117), np.float64(0.4361477831055912), np.float64(0.4427299444373569), np.float64(0.42925041375799483), np.float64(0.4306109960846018), np.float64(0.4309011555869585), np.float64(0.4346617990291454), np.float64(0.4415189020684394), np.float64(0.4328180183358197), np.float64(0.4345301536424491), np.float64(0.43947296517577705), np.float64(0.4408089878752411), np.float64(0.44215819650301796), np.float64(0.4484633347448492), np.float64(0.44444362201787924), np.float64(0.43219389908558825), np.float64(0.42809771814809394), np.float64(0.43400013731343157), np.float64(0.4398092117143725), np.float64(0.44301665109210303), np.float64(0.431852073176715), np.float64(0.43646692372040513), np.float64(0.43819240749611543), np.float64(0.4278323270169824), np.float64(0.43241241991710716), np.float64(0.4307579330053332), np.float64(0.4330551978109511), np.float64(0.4361857320886675), np.float64(0.4245405709846568), np.float64(0.4139282415680388), np.float64(0.418887869566297), np.float64(0.42413861993985347), np.float64(0.42907590410523244), np.float64(0.43361753177399576), np.float64(0.4269025418041826), np.float64(0.4158286020298276), np.float64(0.4158286020298276), np.float64(0.4209593428860382), np.float64(0.4258500176548627), np.float64(0.42451998755285447), np.float64(0.4264523691527048), np.float64(0.42037524204815807), np.float64(0.42400325491416735), np.float64(0.42879481073176284), np.float64(0.4297852186388398), np.float64(0.4342695115080186), np.float64(0.43775537389127367), np.float64(0.42954053178042334), np.float64(0.42384823774139285), np.float64(0.4280418678052806), np.float64(0.4247667372797626), np.float64(0.4178190749697453), np.float64(0.42199297341098946), np.float64(0.42199297341098946), np.float64(0.42615997013193), np.float64(0.4247781364907719), np.float64(0.42327495827027745), np.float64(0.42364621188382273), np.float64(0.4234434060318761), np.float64(0.4259903486916906), np.float64(0.42940477562168394), np.float64(0.42940477562168394), np.float64(0.4275921497834983), np.float64(0.4318321150203819), np.float64(0.43586769794304203), np.float64(0.4399788788679675), np.float64(0.43222567214485696), np.float64(0.43351745513569573), np.float64(0.43351745513569573), np.float64(0.43351745513569573), np.float64(0.4313053860537895), np.float64(0.4284806309078638), np.float64(0.4258825159642465), np.float64(0.4291093311082097), np.float64(0.4326059024716943), np.float64(0.43264076616580155), np.float64(0.43649334670850015), np.float64(0.43788290852571643), np.float64(0.44009151239597555), np.float64(0.4438413246937115), np.float64(0.4438413246937115), np.float64(0.4414438989685916), np.float64(0.43431598131967497), np.float64(0.43404840341264633), np.float64(0.4323427043167418), np.float64(0.43377224034927175), np.float64(0.43581843748516547), np.float64(0.43481903959137785), np.float64(0.438196524026174), np.float64(0.44138904654478395), np.float64(0.435648327975376), np.float64(0.43870647618547015), np.float64(0.4327733103683483), np.float64(0.43018541227869345), np.float64(0.4328929301718439), np.float64(0.43634375498084105), np.float64(0.43975427717211585), np.float64(0.44247549565285627), np.float64(0.437545544616388), np.float64(0.4344441576657708), np.float64(0.43237744469514), np.float64(0.43571584634564414), np.float64(0.43254962228460325), np.float64(0.4323672432093182), np.float64(0.426375936686131), np.float64(0.42200179165800333), np.float64(0.42440699012810507), np.float64(0.4263676442296394), np.float64(0.42412687894137097), np.float64(0.4272449092532283), np.float64(0.4302641790242181), np.float64(0.42964391378946387), np.float64(0.43254115975411783), np.float64(0.4333986269364773), np.float64(0.4356694041157308), np.float64(0.43865798351923835), np.float64(0.4401784747034367), np.float64(0.44315889098712574), np.float64(0.44570586278774643), np.float64(0.4485808510278115), np.float64(0.44603385263006645), np.float64(0.4444545148888547), np.float64(0.4442112488191762), np.float64(0.43899734845786126), np.float64(0.4418706637526179), np.float64(0.4444765889393764), np.float64(0.4390342357626539), np.float64(0.43688472536571565), np.float64(0.4311509697326517), np.float64(0.4254081048068737), np.float64(0.4280226823338264), np.float64(0.4301567611163197), np.float64(0.4327104379114978), np.float64(0.4284851224258703), np.float64(0.4262030163753873), np.float64(0.4229081681861284), np.float64(0.4200870148160755), np.float64(0.41942460373766827), np.float64(0.42213351281014566), np.float64(0.4213743324426621), np.float64(0.41715083500684785), np.float64(0.4189835439457278), np.float64(0.41415043660772194), np.float64(0.4084016193566791), np.float64(0.40506312295397606), np.float64(0.40639830408475813), np.float64(0.4088705747645416), np.float64(0.4114687817096165), np.float64(0.4096002277039886), np.float64(0.4120618782982088), np.float64(0.40913351847922663), np.float64(0.41147481431382044), np.float64(0.4139046448912721), np.float64(0.41641387128165336), np.float64(0.41733027027050634), np.float64(0.41557074109783926), np.float64(0.41233960214186616), np.float64(0.41174453034734454), np.float64(0.41386006121364144), np.float64(0.4164021813404835), np.float64(0.41156082926767323), np.float64(0.41401504434862796), np.float64(0.4143756062471596), np.float64(0.4100399320197783), np.float64(0.4120627175790948), np.float64(0.40871978313342094), np.float64(0.40478334684153106), np.float64(0.40728945985472303)]</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 28, 29, 30, 30, 30, 31, 32, 33, 33, 34, 35, 35, 36, 36, 36, 36, 37, 37, 38, 38, 38, 39, 39, 40, 40, 40, 40, 41, 41, 41, 41, 41, 41, 41, 42, 42, 42, 42, 42, 42, 42, 43, 43, 43, 43, 43, 44, 44, 45, 46, 47, 47, 48, 48, 48, 49, 49, 49, 49, 49, 50, 50, 50, 50, 51, 52, 52, 52, 52, 52, 52, 53, 53, 53, 53, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 55, 55, 55, 55, 55, 55, 56, 56, 56, 56, 56, 56, 56, 56, 56, 56, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 58, 59, 59, 59, 59, 59, 59, 59, 59, 60, 60, 60, 60, 60, 60, 60, 61, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 62, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63, 63]</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>mixII</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>improve</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>35</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.6310935825061664</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.6343641837410061</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.7380547636189551), np.float64(0.7380547636189551), np.float64(0.7380547636189551), np.float64(0.7380547636189551), np.float64(0.8162019780566931), np.float64(0.8755501480492246), np.float64(0.8721957546448864), np.float64(0.8721957546448864), np.float64(0.8713318189883328), np.float64(0.8713318189883328), np.float64(0.7949920536785267), np.float64(0.711762686833432), np.float64(0.731230382415854), np.float64(0.756014150191566), np.float64(0.756014150191566), np.float64(0.756014150191566), np.float64(0.7022040294683551), np.float64(0.7022040294683551), np.float64(0.7021399369682043), np.float64(0.6984770578029345), np.float64(0.6603882918242137), np.float64(0.6843603796819347), np.float64(0.6889681515778605), np.float64(0.6889681515778605), np.float64(0.6889681515778605), np.float64(0.7015132312247188), np.float64(0.7015132312247188), np.float64(0.7114257660552287), np.float64(0.7114257660552287), np.float64(0.6989700778899103), np.float64(0.6749880988976888), np.float64(0.6665085034323185), np.float64(0.6332509097154436), np.float64(0.6160291599473277), np.float64(0.6260181387188846), np.float64(0.6400371975706117), np.float64(0.637927137291049), np.float64(0.6379271372910489), np.float64(0.6069584351964908), np.float64(0.6069584351964908), np.float64(0.6069584351964908), np.float64(0.6061198990579777), np.float64(0.6200935162302738), np.float64(0.6134869275314325), np.float64(0.6233270161528782), np.float64(0.6339639868311641), np.float64(0.6419753700733437), np.float64(0.6486368655531606), np.float64(0.658936426017342), np.float64(0.658936426017342), np.float64(0.658936426017342), np.float64(0.6512723394426972), np.float64(0.6593615950945471), np.float64(0.6681212501012422), np.float64(0.6748311548317019), np.float64(0.6758177350905237), np.float64(0.6758177350905237), np.float64(0.677940613531284), np.float64(0.663846559907008), np.float64(0.6689234921783024), np.float64(0.6672067912123719), np.float64(0.6602591625921438), np.float64(0.6578509543666514), np.float64(0.6415404139995315), np.float64(0.6397872060882038), np.float64(0.6426389368076945), np.float64(0.649908657417942), np.float64(0.6568987468497107), np.float64(0.6633013653511807), np.float64(0.6673535977119107), np.float64(0.6656663587920141), np.float64(0.6716820353454845), np.float64(0.6716820353454845), np.float64(0.6744008257633481), np.float64(0.674938023372121), np.float64(0.6709308151132924), np.float64(0.669248417277815), np.float64(0.6747578182514136), np.float64(0.67137437973003), np.float64(0.661557038468462), np.float64(0.6586006410335036), np.float64(0.6587429782568084), np.float64(0.656491544596325), np.float64(0.660183319693093), np.float64(0.6619605823372228), np.float64(0.665158846696507), np.float64(0.6614135619631761), np.float64(0.6608553853130236), np.float64(0.6609760890458429), np.float64(0.6656171053197146), np.float64(0.6607797974503269), np.float64(0.6635705671361543), np.float64(0.6670044084208031), np.float64(0.6631866712102616), np.float64(0.6631866712102616), np.float64(0.6561645125973259), np.float64(0.6605617604621598), np.float64(0.6605617604621598), np.float64(0.6556346821046689), np.float64(0.6562937199811768), np.float64(0.6549056861540622), np.float64(0.6578386981160914), np.float64(0.6578386981160914), np.float64(0.6539599205417289), np.float64(0.658077700194405), np.float64(0.6581807824859525), np.float64(0.6574617512578999), np.float64(0.6597287800902932), np.float64(0.6552198606950732), np.float64(0.6588072336615813), np.float64(0.6613196411611852), np.float64(0.6563918135438805), np.float64(0.6598658525642742), np.float64(0.6634648412530864), np.float64(0.6634648412530864), np.float64(0.6634648412530864), np.float64(0.6652851757113186), np.float64(0.6640100487933993), np.float64(0.659897673774114), np.float64(0.6634404036143251), np.float64(0.6634404036143251), np.float64(0.6652881249550198), np.float64(0.6611903959277224), np.float64(0.6605451709141439), np.float64(0.6625239513916479), np.float64(0.6598431303306579), np.float64(0.6615811513070147), np.float64(0.6634042688625398), np.float64(0.6588467854549838), np.float64(0.653325276193854), np.float64(0.6497428381862257), np.float64(0.650654475705929), np.float64(0.6504284893091667), np.float64(0.6526556618695452), np.float64(0.6557639326636384), np.float64(0.6519335192063638), np.float64(0.6495024663389471), np.float64(0.6525689823153341), np.float64(0.6524472259840896), np.float64(0.6540632764659066), np.float64(0.647207195188357), np.float64(0.6475844651887175), np.float64(0.6505697511968537), np.float64(0.6523950789699584), np.float64(0.6489656524376888), np.float64(0.6518624467286588), np.float64(0.6530296137497098), np.float64(0.654259564806596), np.float64(0.6490341437261021), np.float64(0.6478976544991322), np.float64(0.6504337487423271), np.float64(0.647512647668899), np.float64(0.6460044142583855), np.float64(0.6452517746493113), np.float64(0.6456334721615001), np.float64(0.6428659691677572), np.float64(0.6449780956578548), np.float64(0.6425868848835129), np.float64(0.6399430918907678), np.float64(0.642594062624843), np.float64(0.6445597616509505), np.float64(0.6443049787063745), np.float64(0.6408439827040466), np.float64(0.6389632144234133), np.float64(0.6334488790807308), np.float64(0.6360118906286918), np.float64(0.637881827136212), np.float64(0.6369779997527762), np.float64(0.6365108728272302), np.float64(0.6352199557133076), np.float64(0.6366605304627416), np.float64(0.6373683459688103), np.float64(0.6396998416009075), np.float64(0.6420602084538227), np.float64(0.6380780713537043), np.float64(0.6391920044942966), np.float64(0.6371044830282442), np.float64(0.6344725586977324), np.float64(0.6334476068265085), np.float64(0.6358068817113681), np.float64(0.6370931840188262), np.float64(0.6367139062079284), np.float64(0.6375433793558385), np.float64(0.6393227644650065), np.float64(0.6414529300292244), np.float64(0.6436423503751801), np.float64(0.6454071591888063), np.float64(0.6446760156857679), np.float64(0.6467940817702101), np.float64(0.6449762717015942), np.float64(0.643437653972719), np.float64(0.6397503216382721), np.float64(0.6384172609935729), np.float64(0.6366232668212055), np.float64(0.6380769987424872), np.float64(0.6365976239549033), np.float64(0.6344420001375699), np.float64(0.636554320888741), np.float64(0.6371849755511925), np.float64(0.6348514810326923), np.float64(0.6364881765910815), np.float64(0.6368994847989645), np.float64(0.6382496749979998), np.float64(0.6362868469259789), np.float64(0.6361637180487291), np.float64(0.6363493315356483), np.float64(0.634583621624981), np.float64(0.6336051062006046), np.float64(0.6327775756856522), np.float64(0.629816849141662), np.float64(0.6312467424832671), np.float64(0.6320169807377591), np.float64(0.6332741532564596), np.float64(0.6341268135663456), np.float64(0.6360196981565748), np.float64(0.6363999101836056), np.float64(0.6369995418107716), np.float64(0.6375111613769809), np.float64(0.6386411845789163), np.float64(0.6399844481067082), np.float64(0.6390395811507517), np.float64(0.6402116429315358), np.float64(0.6381886629288306), np.float64(0.6371769868256576), np.float64(0.6341141988752257), np.float64(0.633409483671541), np.float64(0.6352211478307753), np.float64(0.6368745074201128), np.float64(0.6357510853862), np.float64(0.6328955362699124), np.float64(0.6341016022713113), np.float64(0.634550500848425), np.float64(0.6351559462368793), np.float64(0.6361033990862086), np.float64(0.6373168176750363), np.float64(0.6349410189029943), np.float64(0.6344534844001285), np.float64(0.6361648142864924), np.float64(0.6355579140923092), np.float64(0.6372400026558643), np.float64(0.638511605142346), np.float64(0.6390890310346129), np.float64(0.6388167948077087), np.float64(0.638394986837329), np.float64(0.6369874178265106), np.float64(0.638547193584392), np.float64(0.6395764370395604), np.float64(0.6386802275181316), np.float64(0.6354276049142114), np.float64(0.6332263401043605), np.float64(0.6328707004691548), np.float64(0.632891281356695), np.float64(0.6332152299418424), np.float64(0.6321594300217601), np.float64(0.6293446426699925), np.float64(0.6293497356009126), np.float64(0.6270055111520372), np.float64(0.628536596424095), np.float64(0.6295475030049055), np.float64(0.630978353837482), np.float64(0.6316214659151969), np.float64(0.6293333347682168), np.float64(0.6303361543701458), np.float64(0.6316905091403053), np.float64(0.6308070042409245), np.float64(0.6307658130969974), np.float64(0.6278020098647706), np.float64(0.6290416500566232), np.float64(0.6305619702219071), np.float64(0.6302691813001962), np.float64(0.6314170157003781), np.float64(0.6290269001156258), np.float64(0.630058670225516), np.float64(0.6302256092662072), np.float64(0.6302477786174123), np.float64(0.6306101403894279), np.float64(0.630590392562737), np.float64(0.6318577683922351), np.float64(0.6332592502951839), np.float64(0.6344496110877352), np.float64(0.6358512894177517), np.float64(0.6336766246695957), np.float64(0.632652629322222), np.float64(0.6305282309684138), np.float64(0.6317136045968007), np.float64(0.6326912340356676), np.float64(0.6328914211084183), np.float64(0.6336828827388136), np.float64(0.6313879786723252)]</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 10, 11, 12, 13, 13, 13, 13, 14, 14, 15, 15, 15, 15, 15, 16, 17, 17, 18, 18, 18, 18, 18, 18, 19, 20, 20, 21, 21, 22, 22, 22, 22, 22, 22, 22, 22, 22, 23, 23, 24, 25, 25, 25, 25, 25, 25, 25, 25, 25, 26, 27, 27, 27, 27, 27, 27, 28, 28, 28, 28, 28, 28, 28, 28, 28, 28, 28, 28, 28, 28, 28, 28, 29, 29, 29, 29, 29, 29, 29, 29, 29, 29, 29, 29, 29, 29, 29, 29, 29, 29, 29, 29, 29, 29, 30, 30, 30, 31, 31, 31, 31, 31, 32, 32, 32, 32, 32, 32, 32, 32, 32, 32, 32, 32, 33, 34, 34, 34, 34, 34, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35]</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>mixI</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>reward_punish</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>191</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.6771431394819154</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.6717640916223196</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(-0.4717280456498435), np.float64(-0.4717280456498435), np.float64(-0.4717280456498435), np.float64(-0.4717280456498435), np.float64(-0.4717280456498435), np.float64(-0.4717280456498435), np.float64(-0.4717280456498435), np.float64(-0.4717280456498435), np.float64(-0.4717280456498435), np.float64(-0.4717280456498435), np.float64(-0.4717280456498435), np.float64(0.1754490911365198), np.float64(0.1754490911365198), np.float64(0.1754490911365198), np.float64(0.1754490911365198), np.float64(0.1754490911365198), np.float64(0.1754490911365198), np.float64(0.1754490911365198), np.float64(0.1754490911365198), np.float64(0.308281216623905), np.float64(0.308281216623905), np.float64(0.30828121662390495), np.float64(-0.005453594428952463), np.float64(0.19363171720292632), np.float64(0.19363171720292632), np.float64(0.19363171720292632), np.float64(0.19363171720292632), np.float64(0.19363171720292632), np.float64(0.19363171720292632), np.float64(0.19363171720292632), np.float64(0.19363171720292632), np.float64(0.19363171720292632), np.float64(0.19363171720292632), np.float64(0.19363171720292632), np.float64(0.19363171720292632), np.float64(0.19363171720292632), np.float64(0.29310058158190105), np.float64(0.2931005815819011), np.float64(0.37218092399344194), np.float64(0.37218092399344194), np.float64(0.37218092399344194), np.float64(0.37218092399344194), np.float64(0.37218092399344194), np.float64(0.37218092399344194), np.float64(0.4324067370530005), np.float64(0.363238854641043), np.float64(0.363238854641043), np.float64(0.363238854641043), np.float64(0.363238854641043), np.float64(0.42691219603178343), np.float64(0.42691219603178343), np.float64(0.43701784186736226), np.float64(0.43701784186736226), np.float64(0.43701784186736226), np.float64(0.4568596951152421), np.float64(0.4568596951152421), np.float64(0.4841474626784331), np.float64(0.4841474626784331), np.float64(0.4841474626784331), np.float64(0.4841474626784331), np.float64(0.505428021583511), np.float64(0.5039689024298204), np.float64(0.48969296938459433), np.float64(0.5180471404304975), np.float64(0.5180471404304975), np.float64(0.5180471404304975), np.float64(0.5180471404304975), np.float64(0.5180471404304975), np.float64(0.5180471404304975), np.float64(0.5180471404304976), np.float64(0.5180471404304976), np.float64(0.5255286121219265), np.float64(0.5255286121219265), np.float64(0.5255286121219265), np.float64(0.5413393193067451), np.float64(0.5413393193067451), np.float64(0.5413393193067451), np.float64(0.541339319306745), np.float64(0.541339319306745), np.float64(0.541339319306745), np.float64(0.5607173094896801), np.float64(0.5607173094896801), np.float64(0.5623493028904661), np.float64(0.5623493028904661), np.float64(0.5623493028904661), np.float64(0.562349302890466), np.float64(0.562349302890466), np.float64(0.562349302890466), np.float64(0.562349302890466), np.float64(0.562349302890466), np.float64(0.562349302890466), np.float64(0.562349302890466), np.float64(0.562349302890466), np.float64(0.562349302890466), np.float64(0.562349302890466), np.float64(0.5807951264671533), np.float64(0.5807951264671533), np.float64(0.5807951264671533), np.float64(0.5938918982677578), np.float64(0.5969360935462589), np.float64(0.5969360935462589), np.float64(0.6054681367469986), np.float64(0.6054681367469986), np.float64(0.6054681367469986), np.float64(0.6054681367469986), np.float64(0.6054681367469986), np.float64(0.6054681367469986), np.float64(0.6054681367469986), np.float64(0.6182795180978025), np.float64(0.6182795180978025), np.float64(0.6182795180978025), np.float64(0.6182795180978025), np.float64(0.6182795180978025), np.float64(0.6182795180978025), np.float64(0.6182795180978025), np.float64(0.6182795180978025), np.float64(0.6182795180978025), np.float64(0.623454846141073), np.float64(0.6159863558966598), np.float64(0.6159863558966598), np.float64(0.6159863558966598), np.float64(0.6223438523898525), np.float64(0.6223438523898525), np.float64(0.6010193875445974), np.float64(0.6010193875445974), np.float64(0.6010193875445974), np.float64(0.6010193875445974), np.float64(0.6010193875445974), np.float64(0.6028658852925114), np.float64(0.6028658852925114), np.float64(0.6133120571897117), np.float64(0.6133120571897117), np.float64(0.6133120571897117), np.float64(0.6243039718315162), np.float64(0.6268868100855715), np.float64(0.618546390933979), np.float64(0.617848961371369), np.float64(0.617848961371369), np.float64(0.6270324533655629), np.float64(0.6270324533655629), np.float64(0.6150554419005366), np.float64(0.6150554419005366), np.float64(0.6150554419005366), np.float64(0.6150554419005366), np.float64(0.6241526942882781), np.float64(0.6241526942882781), np.float64(0.6122891564750063), np.float64(0.6122891564750063), np.float64(0.6030801848036259), np.float64(0.6030801848036259), np.float64(0.6030801848036259), np.float64(0.5963472227607804), np.float64(0.5963472227607804), np.float64(0.5963472227607804), np.float64(0.6049175958580268), np.float64(0.6049175958580268), np.float64(0.6049175958580268), np.float64(0.6087318395068302), np.float64(0.6093977310574724), np.float64(0.6093977310574724), np.float64(0.5963530513414845), np.float64(0.5963530513414845), np.float64(0.5883301764084207), np.float64(0.5883301764084207), np.float64(0.5887186976522275), np.float64(0.5887186976522275), np.float64(0.5887186976522275), np.float64(0.5887186976522275), np.float64(0.5887186976522275), np.float64(0.5887186976522275), np.float64(0.5887186976522275), np.float64(0.5887186976522275), np.float64(0.5887186976522275), np.float64(0.5799784380174685), np.float64(0.5674671855853216), np.float64(0.5674671855853216), np.float64(0.5742991980313104), np.float64(0.5824489136164431), np.float64(0.5824489136164431), np.float64(0.5824489136164431), np.float64(0.5824489136164431), np.float64(0.582448913616443), np.float64(0.5879376383602815), np.float64(0.5885882931392062), np.float64(0.5889730938538053), np.float64(0.5889730938538053), np.float64(0.5806551995500661), np.float64(0.5775127967747827), np.float64(0.5739675439856853), np.float64(0.5677125857540184), np.float64(0.5677125857540184), np.float64(0.5677125857540184), np.float64(0.5699901313197915), np.float64(0.5699901313197915), np.float64(0.5699901313197915), np.float64(0.5699901313197915), np.float64(0.5699901313197915), np.float64(0.5763864186741738), np.float64(0.5763864186741738), np.float64(0.5831463056847486), np.float64(0.5851952534189313), np.float64(0.5895342986401483), np.float64(0.595798755789893), np.float64(0.595798755789893), np.float64(0.5993935104393522), np.float64(0.5993935104393522), np.float64(0.6046314969434997), np.float64(0.6046314969434997), np.float64(0.6061243236127388), np.float64(0.6061243236127388), np.float64(0.6061243236127388), np.float64(0.6083265471960139), np.float64(0.6083265471960139), np.float64(0.6083265471960139), np.float64(0.6083265471960139), np.float64(0.6139122016034683), np.float64(0.6157665496562311), np.float64(0.6187340382924188), np.float64(0.6235898740257475), np.float64(0.6279981521939335), np.float64(0.6279981521939335), np.float64(0.6279981521939335), np.float64(0.6325274891807228), np.float64(0.6305048931935854), np.float64(0.6350316940357055), np.float64(0.6397072319821351), np.float64(0.6397072319821351), np.float64(0.6435501755565173), np.float64(0.6459578639646887), np.float64(0.6482069884936523), np.float64(0.6482069884936523), np.float64(0.6482069884936523), np.float64(0.6500689293320061), np.float64(0.6500689293320061), np.float64(0.6500689293320061), np.float64(0.6542232901246823), np.float64(0.6582724568361373), np.float64(0.6620051694770145), np.float64(0.6616359025573951), np.float64(0.665484855808474), np.float64(0.665484855808474), np.float64(0.661938618876022), np.float64(0.6584839766259231), np.float64(0.6617527369193581), np.float64(0.6559604204527555), np.float64(0.6559604204527555), np.float64(0.6596887814579319), np.float64(0.6627460941779512), np.float64(0.6640536627880418), np.float64(0.6640536627880418), np.float64(0.6661403073117361), np.float64(0.6673048776007007), np.float64(0.6682579995623383), np.float64(0.6682579995623383), np.float64(0.6712679127818518), np.float64(0.6698954376897974), np.float64(0.6701684288535354), np.float64(0.6701684288535354), np.float64(0.6701684288535354), np.float64(0.6654759116468832), np.float64(0.6654759116468832), np.float64(0.6682520587057665), np.float64(0.6696029118535534), np.float64(0.6696029118535534), np.float64(0.6727583874152899), np.float64(0.6758431332533508), np.float64(0.6786288733585385), np.float64(0.6786288733585385), np.float64(0.6814236137111503), np.float64(0.6814236137111503), np.float64(0.6798845001896725), np.float64(0.6771431394819154), np.float64(0.6771431394819154)]</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 36, 37, 38, 39, 40, 41, 42, 43, 43, 44, 45, 45, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 57, 58, 58, 59, 60, 61, 62, 63, 63, 63, 64, 65, 66, 66, 67, 67, 68, 69, 69, 70, 70, 71, 72, 73, 73, 73, 73, 73, 74, 75, 76, 77, 78, 79, 80, 80, 81, 82, 82, 83, 84, 85, 86, 87, 87, 88, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 100, 101, 102, 102, 102, 103, 103, 104, 105, 106, 107, 108, 109, 109, 110, 111, 112, 113, 114, 115, 116, 117, 117, 117, 118, 119, 119, 120, 120, 121, 122, 123, 124, 124, 125, 125, 126, 127, 127, 127, 127, 127, 128, 128, 129, 129, 130, 131, 132, 132, 133, 133, 134, 134, 135, 136, 136, 137, 138, 138, 139, 140, 140, 140, 141, 141, 142, 142, 143, 143, 144, 145, 146, 147, 148, 149, 150, 151, 151, 151, 152, 152, 152, 153, 154, 155, 156, 156, 156, 156, 157, 157, 157, 157, 157, 158, 159, 159, 160, 161, 162, 163, 163, 164, 164, 164, 164, 164, 165, 165, 166, 166, 167, 167, 168, 169, 169, 170, 171, 172, 172, 172, 172, 172, 172, 173, 174, 174, 174, 174, 174, 175, 175, 175, 175, 176, 177, 177, 178, 179, 179, 179, 179, 179, 179, 180, 180, 180, 180, 180, 181, 181, 181, 181, 182, 182, 182, 182, 183, 183, 183, 183, 184, 185, 185, 186, 186, 186, 187, 187, 187, 187, 188, 188, 189, 189, 189, 190]</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>mixI</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>reward_punish</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>105</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.812549181524435</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.8043196193350594</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.4697216667761318), np.float64(0.4697216667761318), np.float64(0.4697216667761318), np.float64(0.4697216667761318), np.float64(0.4697216667761318), np.float64(0.4697216667761318), np.float64(0.4697216667761318), np.float64(0.4697216667761318), np.float64(0.4697216667761318), np.float64(0.4697216667761318), np.float64(0.4697216667761318), np.float64(0.4697216667761318), np.float64(0.534445097775688), np.float64(0.6888830437586436), np.float64(0.6888830437586436), np.float64(0.6888830437586436), np.float64(0.6888830437586436), np.float64(0.5929716685984509), np.float64(0.5929716685984509), np.float64(0.5929716685984509), np.float64(0.5929716685984509), np.float64(0.6743690564542906), np.float64(0.6743690564542906), np.float64(0.6743690564542906), np.float64(0.6917125704956845), np.float64(0.6917125704956845), np.float64(0.6917125704956845), np.float64(0.6917125704956845), np.float64(0.7266901377797045), np.float64(0.7266901377797045), np.float64(0.7266901377797045), np.float64(0.7266901377797045), np.float64(0.7266901377797045), np.float64(0.7565234418798423), np.float64(0.7829290221850366), np.float64(0.7829290221850367), np.float64(0.7829290221850367), np.float64(0.7829290221850367), np.float64(0.7829290221850367), np.float64(0.7829290221850367), np.float64(0.7829290221850367), np.float64(0.7968242185211174), np.float64(0.7968242185211174), np.float64(0.7968242185211174), np.float64(0.7968242185211174), np.float64(0.7968242185211174), np.float64(0.7968242185211174), np.float64(0.7968242185211174), np.float64(0.8046478699824255), np.float64(0.8138948565246419), np.float64(0.8188543788127755), np.float64(0.8188543788127753), np.float64(0.8188543788127753), np.float64(0.8248212207028035), np.float64(0.8248212207028035), np.float64(0.8248212207028035), np.float64(0.8248212207028035), np.float64(0.8248212207028035), np.float64(0.8289214142345381), np.float64(0.8289214142345381), np.float64(0.8289214142345381), np.float64(0.7943229333114997), np.float64(0.8005995189952393), np.float64(0.8116435318583439), np.float64(0.8116435318583439), np.float64(0.8116435318583439), np.float64(0.810497599164728), np.float64(0.8145042157658672), np.float64(0.823139388902104), np.float64(0.823139388902104), np.float64(0.823139388902104), np.float64(0.823139388902104), np.float64(0.823904398096013), np.float64(0.823904398096013), np.float64(0.823904398096013), np.float64(0.8180016486905517), np.float64(0.8180016486905517), np.float64(0.8230205555803011), np.float64(0.8230205555803011), np.float64(0.8230205555803011), np.float64(0.8249516148203304), np.float64(0.830074130333701), np.float64(0.8321715571362118), np.float64(0.8346494821159537), np.float64(0.8346494821159537), np.float64(0.839469164972543), np.float64(0.839469164972543), np.float64(0.8429871333023213), np.float64(0.8470317953265671), np.float64(0.8410932278540714), np.float64(0.8362249032729145), np.float64(0.8407244417934351), np.float64(0.8407244417934351), np.float64(0.8449342585565282), np.float64(0.8414611678563546), np.float64(0.8414611678563546), np.float64(0.8414611678563546), np.float64(0.8297089574029636), np.float64(0.8153622905252382), np.float64(0.8188849204008898), np.float64(0.8188849204008898), np.float64(0.8104945058433252), np.float64(0.8079267501159785), np.float64(0.8120395868905261), np.float64(0.8120395868905261), np.float64(0.8120395868905261), np.float64(0.8120395868905261), np.float64(0.8163492576192243), np.float64(0.8163492576192243), np.float64(0.8127404060700574), np.float64(0.8127404060700574), np.float64(0.8092629168118027), np.float64(0.8085485571902489), np.float64(0.8118557858398286), np.float64(0.8118557858398286), np.float64(0.8152347997270116), np.float64(0.8169630550365601), np.float64(0.8169630550365601), np.float64(0.8169630550365601), np.float64(0.8169630550365601), np.float64(0.8169878913217559), np.float64(0.818562599868305), np.float64(0.8217723237365812), np.float64(0.8211895314783444), np.float64(0.8098457004893362), np.float64(0.8046474463004184), np.float64(0.800056570024014), np.float64(0.8032644384947828), np.float64(0.8019975277036948), np.float64(0.8053474445737488), np.float64(0.8053474445737488), np.float64(0.8085807467558372), np.float64(0.8117180228726847), np.float64(0.8139727420704174), np.float64(0.8139727420704174), np.float64(0.8143145195060403), np.float64(0.8135201210440468), np.float64(0.8162017774566501), np.float64(0.806698315318052), np.float64(0.8066983153180521), np.float64(0.8066983153180521), np.float64(0.8084205362018411), np.float64(0.8088724570008572), np.float64(0.8088724570008572), np.float64(0.8088724570008572), np.float64(0.8076743062945908), np.float64(0.8098813193990585), np.float64(0.8098813193990583), np.float64(0.8098813193990583), np.float64(0.8086463684428256), np.float64(0.8102881219128777), np.float64(0.8096599559329315), np.float64(0.8101570591858153), np.float64(0.8125207911943273), np.float64(0.8136223076300869), np.float64(0.8155923201446725), np.float64(0.8155923201446725), np.float64(0.816652993351685), np.float64(0.8188949251951885), np.float64(0.8196492724126546), np.float64(0.8218753973423202), np.float64(0.8237606500201442), np.float64(0.8234296017752617), np.float64(0.8251137225072411), np.float64(0.8265805841171973), np.float64(0.8281190571783695), np.float64(0.8281190571783695), np.float64(0.8300596212371452), np.float64(0.8295298353366579), np.float64(0.8311696557078947), np.float64(0.8276028900955025), np.float64(0.8294972366197341), np.float64(0.8294972366197341), np.float64(0.8313352767903948), np.float64(0.8330333332523987), np.float64(0.8336775935941504), np.float64(0.8354152291294779), np.float64(0.8364269984236254), np.float64(0.8361669610779606), np.float64(0.8355486380505832), np.float64(0.8363977148530031), np.float64(0.8372855930359302), np.float64(0.8361411151604126), np.float64(0.8377473921744744), np.float64(0.839183664924637), np.float64(0.8364155710726723), np.float64(0.836413461967831), np.float64(0.8369679775628782), np.float64(0.8369679775628782), np.float64(0.8318273972925955), np.float64(0.8306464184867548), np.float64(0.8310351679647607), np.float64(0.8321996630099702), np.float64(0.8336550667564119), np.float64(0.8345826652922295), np.float64(0.8345826652922295), np.float64(0.8345826652922295), np.float64(0.8360453071873695), np.float64(0.832687756257979), np.float64(0.8339896351366196), np.float64(0.8318090276551355), np.float64(0.8303317411037772), np.float64(0.8286185468064228), np.float64(0.829913397177053), np.float64(0.8313099902588481), np.float64(0.8313099902588481), np.float64(0.8327041177683349), np.float64(0.8335565757638264), np.float64(0.8329850361925609), np.float64(0.8323964188409354), np.float64(0.8323964188409354), np.float64(0.8320851891160653), np.float64(0.8327173662828815), np.float64(0.8327173662828815), np.float64(0.8327173662828815), np.float64(0.8330535934300323), np.float64(0.8330470307786426), np.float64(0.834030039216344), np.float64(0.8313350714339425), np.float64(0.8326216685306904), np.float64(0.8338555514326184), np.float64(0.8344204837619454), np.float64(0.8355379647188341), np.float64(0.8364975046928306), np.float64(0.8376304571448829), np.float64(0.8376111689599068), np.float64(0.838759366681592), np.float64(0.8359615879440583), np.float64(0.8359615879440583), np.float64(0.8357525418050674), np.float64(0.8343429074303608), np.float64(0.8351457997864997), np.float64(0.8362781431206802), np.float64(0.8326593940850967), np.float64(0.8326794089800091), np.float64(0.8337778591608417), np.float64(0.8337778591608417), np.float64(0.8348812072812511), np.float64(0.8358877201928799), np.float64(0.8330214680864108), np.float64(0.8329902199829426), np.float64(0.8340721938943358), np.float64(0.835143031932864), np.float64(0.8360461667639132), np.float64(0.8364411818157903), np.float64(0.8346015576142689), np.float64(0.8346015576142689), np.float64(0.8336565352590387), np.float64(0.8303362559975067), np.float64(0.830793184170227), np.float64(0.8315276587301016), np.float64(0.8281977300200211), np.float64(0.8276004085029183), np.float64(0.8271125964118641), np.float64(0.8263181882502754), np.float64(0.8228010303869702), np.float64(0.8230452758353484), np.float64(0.823895375233497), np.float64(0.8249498660216392), np.float64(0.8256931867123383), np.float64(0.8249859923392701), np.float64(0.8257722011829605), np.float64(0.824927715764691), np.float64(0.8246768520590716), np.float64(0.8248814034775218), np.float64(0.8257822554868266), np.float64(0.8267749703905273), np.float64(0.8243215744119687), np.float64(0.8216404843301626), np.float64(0.8203592824533278), np.float64(0.8203551566544227), np.float64(0.8194296300564389), np.float64(0.819647561860467), np.float64(0.8206189174152392), np.float64(0.8195878622253587), np.float64(0.8167662145897343), np.float64(0.8151403535792723), np.float64(0.8156871815550956), np.float64(0.8158865899854691), np.float64(0.816823906686358), np.float64(0.8177896632968713), np.float64(0.8153717445673144), np.float64(0.8150414680919188), np.float64(0.8150905230346739), np.float64(0.8138935472006693), np.float64(0.811794691258258), np.float64(0.812549181524435)]</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 23, 23, 24, 25, 26, 26, 27, 28, 29, 29, 30, 31, 31, 32, 33, 34, 34, 35, 36, 37, 38, 38, 38, 39, 40, 41, 42, 43, 44, 44, 45, 46, 47, 48, 49, 50, 50, 50, 50, 51, 52, 52, 53, 54, 55, 56, 56, 57, 58, 58, 58, 58, 59, 60, 60, 60, 60, 61, 62, 63, 63, 64, 65, 65, 66, 66, 67, 68, 68, 68, 68, 68, 69, 69, 70, 70, 70, 70, 70, 70, 71, 71, 71, 72, 73, 73, 73, 73, 74, 74, 74, 74, 75, 76, 77, 77, 78, 78, 79, 79, 79, 79, 80, 80, 80, 81, 82, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 83, 84, 84, 84, 84, 85, 85, 85, 85, 85, 86, 87, 87, 87, 88, 89, 89, 89, 90, 91, 91, 91, 91, 91, 91, 91, 91, 92, 92, 92, 92, 92, 92, 92, 92, 92, 92, 93, 93, 93, 93, 93, 93, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 94, 95, 95, 95, 95, 95, 95, 95, 96, 97, 97, 97, 97, 97, 97, 97, 97, 97, 98, 98, 98, 98, 98, 99, 99, 99, 100, 101, 101, 101, 101, 101, 101, 101, 101, 101, 101, 101, 101, 101, 101, 102, 102, 102, 102, 102, 102, 102, 102, 103, 103, 103, 103, 103, 103, 103, 103, 103, 103, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104, 104]</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>mixI</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>reward_punish</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>77</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.7585955548786277</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.7564709667588666</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.8567795454328626), np.float64(0.8567795454328626), np.float64(0.8567795454328626), np.float64(0.8567795454328626), np.float64(0.8567795454328626), np.float64(0.8567795454328626), np.float64(0.8567795454328626), np.float64(0.8567795454328626), np.float64(0.8567795454328626), np.float64(0.8567795454328626), np.float64(0.8567795454328626), np.float64(0.8567795454328626), np.float64(0.9283497463522254), np.float64(0.9283497463522254), np.float64(0.9283497463522254), np.float64(0.9283497463522254), np.float64(0.9497536547979273), np.float64(0.9497536547979273), np.float64(0.9497536547979273), np.float64(0.9497536547979273), np.float64(0.8862091543592353), np.float64(0.8862091543592353), np.float64(0.8862091543592352), np.float64(0.8862091543592352), np.float64(0.8862091543592352), np.float64(0.8517346072396668), np.float64(0.8517346072396668), np.float64(0.8517346072396668), np.float64(0.8517346072396668), np.float64(0.7673081044417769), np.float64(0.7673081044417769), np.float64(0.7673081044417769), np.float64(0.7673081044417769), np.float64(0.7673081044417769), np.float64(0.7673081044417769), np.float64(0.7673081044417769), np.float64(0.7673081044417769), np.float64(0.7673081044417769), np.float64(0.7673081044417769), np.float64(0.7947918911421025), np.float64(0.7788836963202569), np.float64(0.7992908864420314), np.float64(0.7992908864420314), np.float64(0.7992908864420314), np.float64(0.7992908864420314), np.float64(0.7992908864420314), np.float64(0.7992908864420314), np.float64(0.7960804777528019), np.float64(0.8144976001061269), np.float64(0.7961653484185062), np.float64(0.7961653484185062), np.float64(0.7981872913190795), np.float64(0.8122775837812212), np.float64(0.8122775837812212), np.float64(0.8122775837812212), np.float64(0.8241198651067952), np.float64(0.8241198651067952), np.float64(0.8350892747652143), np.float64(0.8350892747652143), np.float64(0.8424675674600877), np.float64(0.8498355057091902), np.float64(0.854665511694947), np.float64(0.8617322950212767), np.float64(0.8617322950212767), np.float64(0.8377886132506763), np.float64(0.8411883258306687), np.float64(0.8411883258306687), np.float64(0.8411883258306687), np.float64(0.8365326419750317), np.float64(0.8145664225936516), np.float64(0.8145664225936516), np.float64(0.8034497751717896), np.float64(0.8034497751717896), np.float64(0.8084719063821547), np.float64(0.7830406971332567), np.float64(0.7830406971332567), np.float64(0.7848475322422603), np.float64(0.7873820797085007), np.float64(0.7889178540876732), np.float64(0.7712984710352371), np.float64(0.7712984710352371), np.float64(0.7712984710352371), np.float64(0.7656353489753327), np.float64(0.7719999627519766), np.float64(0.7653042215902759), np.float64(0.768861342623047), np.float64(0.7748174314962943), np.float64(0.7760685426148859), np.float64(0.7802238293142879), np.float64(0.7858480192822489), np.float64(0.7906046225896316), np.float64(0.7849627123818248), np.float64(0.7845532377202945), np.float64(0.7845532377202945), np.float64(0.7894438609911141), np.float64(0.7923548408360308), np.float64(0.7904736981514046), np.float64(0.7904736981514046), np.float64(0.7950162260908741), np.float64(0.7927489063978114), np.float64(0.7927489063978114), np.float64(0.7908741416810249), np.float64(0.7788881240611942), np.float64(0.7788881240611942), np.float64(0.7821410573034163), np.float64(0.7821410573034163), np.float64(0.7765403205132619), np.float64(0.7649518409596326), np.float64(0.7655614522193565), np.float64(0.7688632148434871), np.float64(0.7669941337725428), np.float64(0.7708740083030772), np.float64(0.7748709953961667), np.float64(0.7748709953961667), np.float64(0.7648599518088057), np.float64(0.7648599518088057), np.float64(0.7657369663768139), np.float64(0.7695583848693184), np.float64(0.771255770095002), np.float64(0.7664128680921045), np.float64(0.7665678642441692), np.float64(0.762295009051855), np.float64(0.7586722059535225), np.float64(0.7622673589223847), np.float64(0.7653405426742901), np.float64(0.7596466601928071), np.float64(0.7553419926294974), np.float64(0.7515128956712125), np.float64(0.7497723501825863), np.float64(0.7531020557649282), np.float64(0.7521594526881864), np.float64(0.7527123776643425), np.float64(0.7521207992423717), np.float64(0.7496483319307305), np.float64(0.7523010723062045), np.float64(0.7458876834014608), np.float64(0.7379685465396613), np.float64(0.7330154067053682), np.float64(0.7352822695316259), np.float64(0.7384440897988728), np.float64(0.7406670739908479), np.float64(0.7404033923483312), np.float64(0.7404033923483312), np.float64(0.7420021768296191), np.float64(0.7435648326445247), np.float64(0.7455197373526969), np.float64(0.7457347007739638), np.float64(0.7454282268280124), np.float64(0.7411966892591617), np.float64(0.7440054698933345), np.float64(0.7467836766437516), np.float64(0.7479962551020225), np.float64(0.7501814920354305), np.float64(0.752639408070111), np.float64(0.7517363734552887), np.float64(0.7496855181579272), np.float64(0.7508124234843705), np.float64(0.7532760408747993), np.float64(0.7532760408747992), np.float64(0.7556237518162103), np.float64(0.7557087995176974), np.float64(0.7570746701041502), np.float64(0.755542230125858), np.float64(0.7575900802506855), np.float64(0.7589849178827761), np.float64(0.7570758280690632), np.float64(0.75493130715296), np.float64(0.7553747798949387), np.float64(0.7549516154002773), np.float64(0.7504794185189644), np.float64(0.7527093844877315), np.float64(0.7499388561919308), np.float64(0.7509600662087639), np.float64(0.7531430175387905), np.float64(0.7530181283097044), np.float64(0.753905469638443), np.float64(0.755648809538643), np.float64(0.7575278122781963), np.float64(0.7590656683350951), np.float64(0.7565825130833103), np.float64(0.7583155616335465), np.float64(0.7601524247815046), np.float64(0.7609838011746407), np.float64(0.7614379585841458), np.float64(0.7611707683882404), np.float64(0.7624936549670005), np.float64(0.7612067565446188), np.float64(0.7603348950589486), np.float64(0.7615316761113309), np.float64(0.7580795799159544), np.float64(0.7597756003691195), np.float64(0.7611490354883198), np.float64(0.7629441078892196), np.float64(0.7636289535531214), np.float64(0.7646515185018858), np.float64(0.7660227938524162), np.float64(0.7675162733786531), np.float64(0.7657283473789673), np.float64(0.764496493657276), np.float64(0.7661772368504474), np.float64(0.7622357572125023), np.float64(0.7633308059140962), np.float64(0.7649649229344725), np.float64(0.7637575553967401), np.float64(0.7616645429667634), np.float64(0.760665368772082), np.float64(0.7620843008202385), np.float64(0.7605162388716038), np.float64(0.7619073382072249), np.float64(0.7630408197664018), np.float64(0.7646039111942784), np.float64(0.7648318080313785), np.float64(0.7642080966198088), np.float64(0.7627051675145791), np.float64(0.7588783072023157), np.float64(0.7603186198816054), np.float64(0.7607604593379879), np.float64(0.762160517767655), np.float64(0.7628821768860407), np.float64(0.7607144062682518), np.float64(0.758813856845764), np.float64(0.7602735397589115), np.float64(0.7605496892698506), np.float64(0.7618632305496079), np.float64(0.7631361689344188), np.float64(0.7637496836609524), np.float64(0.7604489001281781), np.float64(0.759625738147413), np.float64(0.7591369688784232), np.float64(0.7593499529957797), np.float64(0.757897060651183), np.float64(0.7584368343620758), np.float64(0.758714333258191), np.float64(0.7588085813253869), np.float64(0.7592030177682175), np.float64(0.7605579922041954), np.float64(0.7608185513288653), np.float64(0.7619301306573947), np.float64(0.7628144145340399), np.float64(0.7639103982059877), np.float64(0.7640604733338848), np.float64(0.7651947986302285), np.float64(0.7664149557293445), np.float64(0.7643872699623006), np.float64(0.7656605769364978), np.float64(0.7647897747505719), np.float64(0.7660332549977955), np.float64(0.7631480892032749), np.float64(0.7639835266481068), np.float64(0.7622815677097855), np.float64(0.7630016261346121), np.float64(0.7616752458984424), np.float64(0.762643751004237), np.float64(0.7636433154201968), np.float64(0.7629687016257063), np.float64(0.7604225749439282), np.float64(0.759844750218493), np.float64(0.7586202947511941), np.float64(0.7576626469724039), np.float64(0.7546623185024031), np.float64(0.7532938505541118), np.float64(0.7544353522879536), np.float64(0.7549929812089098), np.float64(0.7553939587505403), np.float64(0.7562527525104921), np.float64(0.7573768471977133), np.float64(0.7579296699922838), np.float64(0.7589920197809632), np.float64(0.7575041537617934), np.float64(0.7584827870221135), np.float64(0.7596181753327249), np.float64(0.757649167131071), np.float64(0.758771378651007), np.float64(0.7571209182013018), np.float64(0.7556387201446231), np.float64(0.7562173147702054), np.float64(0.7573005398396361), np.float64(0.7577827748881416), np.float64(0.7556142804693124), np.float64(0.7565055437642119), np.float64(0.7567821994608723), np.float64(0.7577954917906368)]</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 28, 29, 30, 31, 31, 32, 33, 34, 34, 35, 36, 37, 38, 38, 39, 40, 41, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 50, 50, 50, 51, 52, 53, 54, 55, 55, 55, 55, 56, 56, 56, 57, 58, 58, 59, 59, 60, 60, 60, 60, 60, 61, 61, 61, 62, 63, 63, 63, 64, 64, 65, 65, 65, 66, 66, 66, 66, 66, 67, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 68, 69, 69, 69, 69, 70, 70, 70, 71, 71, 71, 72, 72, 73, 73, 73, 73, 73, 73, 73, 73, 74, 74, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 75, 76, 76, 76, 76, 76, 76, 76, 76, 76, 76, 76, 76, 76, 76, 76, 76, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77, 77]</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>mixII</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>reward_punish</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>117</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.6448170747317308</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.6536293437487554</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.4919570893063493), np.float64(0.4919570893063493), np.float64(0.4919570893063493), np.float64(0.4919570893063493), np.float64(0.4919570893063493), np.float64(0.4919570893063493), np.float64(0.4919570893063493), np.float64(0.4919570893063493), np.float64(0.4919570893063493), np.float64(0.4919570893063493), np.float64(0.4919570893063493), np.float64(0.4919570893063493), np.float64(0.4919570893063493), np.float64(0.4919570893063493), np.float64(0.16092144722605156), np.float64(0.16092144722605156), np.float64(0.4357031079368448), np.float64(0.4357031079368448), np.float64(0.4357031079368448), np.float64(0.512122020790251), np.float64(0.512122020790251), np.float64(0.512122020790251), np.float64(0.512122020790251), np.float64(0.512122020790251), np.float64(0.512122020790251), np.float64(0.512122020790251), np.float64(0.512122020790251), np.float64(0.5229257798243436), np.float64(0.4377847067570724), np.float64(0.4377847067570724), np.float64(0.5100841780119031), np.float64(0.5100841780119031), np.float64(0.5587079549689816), np.float64(0.5587079549689816), np.float64(0.5587079549689816), np.float64(0.5156762403281087), np.float64(0.5156762403281087), np.float64(0.5156762403281087), np.float64(0.5156762403281087), np.float64(0.48297294373465915), np.float64(0.46099728064538237), np.float64(0.46099728064538237), np.float64(0.4370977181981326), np.float64(0.4370977181981326), np.float64(0.4370977181981326), np.float64(0.4370977181981326), np.float64(0.3942271509500002), np.float64(0.39422715095000027), np.float64(0.39422715095000027), np.float64(0.39422715095000027), np.float64(0.39422715095000027), np.float64(0.39422715095000027), np.float64(0.39422715095000027), np.float64(0.39422715095000027), np.float64(0.39422715095000027), np.float64(0.39422715095000027), np.float64(0.39422715095000027), np.float64(0.39422715095000027), np.float64(0.39422715095000027), np.float64(0.39422715095000027), np.float64(0.4374663542340607), np.float64(0.4239383783350996), np.float64(0.4239383783350996), np.float64(0.4239383783350996), np.float64(0.4517838453410717), np.float64(0.4517838453410717), np.float64(0.47076429116383617), np.float64(0.47076429116383617), np.float64(0.47076429116383617), np.float64(0.4960758250265648), np.float64(0.4960758250265648), np.float64(0.4960758250265648), np.float64(0.4960758250265648), np.float64(0.522528093762471), np.float64(0.5447960553877824), np.float64(0.5241871414847662), np.float64(0.5241871414847662), np.float64(0.5241871414847662), np.float64(0.5241871414847662), np.float64(0.5417567215544598), np.float64(0.5596619089304238), np.float64(0.5596619089304238), np.float64(0.5596619089304238), np.float64(0.5596619089304238), np.float64(0.5596619089304238), np.float64(0.5596619089304238), np.float64(0.5778441034559957), np.float64(0.5730443647534329), np.float64(0.5730443647534329), np.float64(0.5730443647534329), np.float64(0.5730443647534329), np.float64(0.5863716999132504), np.float64(0.5863716999132504), np.float64(0.5863716999132504), np.float64(0.60162487186007), np.float64(0.60162487186007), np.float64(0.5906127630975894), np.float64(0.6047074019210469), np.float64(0.6171514892725533), np.float64(0.6259536042048859), np.float64(0.637046390666899), np.float64(0.637046390666899), np.float64(0.6432685437178511), np.float64(0.6290668479513276), np.float64(0.6367041961466757), np.float64(0.6429674629613437), np.float64(0.6505768408891828), np.float64(0.6505768408891828), np.float64(0.6505768408891828), np.float64(0.6298270933102588), np.float64(0.6393174786534264), np.float64(0.6393174786534264), np.float64(0.6476736381723696), np.float64(0.6562627126799111), np.float64(0.6466963474833146), np.float64(0.6501758729231996), np.float64(0.6580971555217573), np.float64(0.6640849227090294), np.float64(0.6640849227090294), np.float64(0.6554945898531681), np.float64(0.6612531782247155), np.float64(0.6631371224870691), np.float64(0.6653821507822607), np.float64(0.6654977166258479), np.float64(0.6486262747746551), np.float64(0.6486262747746551), np.float64(0.6464502900573804), np.float64(0.6516953551084398), np.float64(0.6516953551084398), np.float64(0.6516953551084398), np.float64(0.6383898255852565), np.float64(0.6422186379666674), np.float64(0.6422186379666674), np.float64(0.6324078520065195), np.float64(0.6382356314892419), np.float64(0.642210136264843), np.float64(0.6407566463556841), np.float64(0.631078287903005), np.float64(0.631078287903005), np.float64(0.631078287903005), np.float64(0.631078287903005), np.float64(0.6330481447164091), np.float64(0.6330481447164091), np.float64(0.6371178099606756), np.float64(0.6371178099606756), np.float64(0.640886109242991), np.float64(0.6412682197298232), np.float64(0.6369554293487717), np.float64(0.64242741512374), np.float64(0.6446401694507203), np.float64(0.6446401694507203), np.float64(0.6462034614315089), np.float64(0.6346063965863165), np.float64(0.6392193252838252), np.float64(0.6392193252838252), np.float64(0.6430057540063996), np.float64(0.640712515390667), np.float64(0.6386691628725462), np.float64(0.6294402360087263), np.float64(0.6343617178118819), np.float64(0.6280925983763632), np.float64(0.6280925983763632), np.float64(0.6281312946358661), np.float64(0.6273865320686698), np.float64(0.6318201562938391), np.float64(0.6347857882909282), np.float64(0.6347857882909282), np.float64(0.6347857882909282), np.float64(0.6344126860252212), np.float64(0.6322390390801869), np.float64(0.6354408472389544), np.float64(0.6339183699968185), np.float64(0.6382234387252494), np.float64(0.6421611047924206), np.float64(0.6421611047924206), np.float64(0.6421611047924205), np.float64(0.6421611047924205), np.float64(0.645373115614408), np.float64(0.6445523583244843), np.float64(0.6371773099551087), np.float64(0.6371773099551087), np.float64(0.6409940138947202), np.float64(0.6409940138947202), np.float64(0.6409940138947201), np.float64(0.6409940138947201), np.float64(0.6343187909173293), np.float64(0.6347516836598082), np.float64(0.6373130446681092), np.float64(0.6358203417346503), np.float64(0.6395759245645508), np.float64(0.6323300547759462), np.float64(0.6349320780521598), np.float64(0.6385676230375673), np.float64(0.6385676230375673), np.float64(0.6364006392094396), np.float64(0.6316915874371923), np.float64(0.6316915874371923), np.float64(0.6316915874371923), np.float64(0.6236464349419442), np.float64(0.623646434941944), np.float64(0.623646434941944), np.float64(0.6273360826673672), np.float64(0.6287695505333101), np.float64(0.6265703455128111), np.float64(0.6265703455128111), np.float64(0.619499045500658), np.float64(0.619913164033681), np.float64(0.6234454222975663), np.float64(0.6172992072566166), np.float64(0.6196474820791487), np.float64(0.6226353555041443), np.float64(0.6251770983465005), np.float64(0.6243481068565477), np.float64(0.6252747897943245), np.float64(0.6269184413450272), np.float64(0.6298573969553675), np.float64(0.6298573969553675), np.float64(0.632614310444184), np.float64(0.6305151537707391), np.float64(0.6267154287836674), np.float64(0.6295508310673689), np.float64(0.631401259355457), np.float64(0.6341078985450984), np.float64(0.6370039668591878), np.float64(0.6345694793107056), np.float64(0.6329842486966687), np.float64(0.6318054823614089), np.float64(0.634109461674175), np.float64(0.6355663848239569), np.float64(0.6352575571402543), np.float64(0.6341224824078523), np.float64(0.6366677291767845), np.float64(0.639346544869755), np.float64(0.639423920406525), np.float64(0.6350420030086815), np.float64(0.6307529298742331), np.float64(0.6326290539269023), np.float64(0.6330902572874245), np.float64(0.6340220136912132), np.float64(0.6350974990907491), np.float64(0.6346202195192864), np.float64(0.6371654610595987), np.float64(0.6311497129923878), np.float64(0.6311497129923878), np.float64(0.6334047012313773), np.float64(0.6345164474180941), np.float64(0.636326231296473), np.float64(0.6372987938610845), np.float64(0.6388856846965046), np.float64(0.6388856846965046), np.float64(0.6374334856978399), np.float64(0.6361912056796865), np.float64(0.6373996908824533), np.float64(0.6388431839046983), np.float64(0.641149981742405), np.float64(0.6423052447816193), np.float64(0.6426718018643217), np.float64(0.6382405156811907), np.float64(0.6395422677107626), np.float64(0.6418465437589846), np.float64(0.6418465437589846), np.float64(0.6440460349246719), np.float64(0.6406970852293287), np.float64(0.6415108107308157), np.float64(0.6365294626664776), np.float64(0.6383788802131092), np.float64(0.6383788802131092), np.float64(0.636883951066845), np.float64(0.6385704800575476), np.float64(0.6405454890359983), np.float64(0.6406196846377499), np.float64(0.6426882830782247), np.float64(0.6420938264174034), np.float64(0.6414121815164412), np.float64(0.6431671700929376), np.float64(0.6442290242883488), np.float64(0.643181316630154), np.float64(0.6452435847959326), np.float64(0.6452435847959326), np.float64(0.6462642686623539), np.float64(0.643110737818188), np.float64(0.645075944407676), np.float64(0.645075944407676), np.float64(0.6421771770767489), np.float64(0.6441929080170081), np.float64(0.6416751125045186), np.float64(0.6435418570681429), np.float64(0.6405356750321657), np.float64(0.6425026672509141), np.float64(0.6428734364908327), np.float64(0.6428734364908327)]</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 21, 22, 22, 23, 24, 24, 25, 26, 27, 28, 29, 30, 31, 31, 31, 32, 32, 33, 33, 34, 35, 35, 36, 37, 38, 38, 38, 39, 39, 40, 41, 42, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 55, 55, 56, 57, 57, 58, 58, 59, 60, 60, 61, 62, 63, 63, 63, 63, 64, 65, 66, 66, 66, 67, 68, 69, 70, 71, 71, 71, 72, 73, 74, 74, 75, 76, 76, 77, 77, 77, 77, 77, 77, 78, 78, 78, 78, 78, 78, 79, 80, 80, 80, 81, 81, 81, 81, 81, 81, 81, 82, 82, 82, 82, 82, 82, 82, 83, 83, 83, 84, 85, 85, 85, 86, 86, 86, 86, 86, 86, 87, 88, 89, 89, 90, 90, 91, 91, 91, 91, 91, 91, 92, 92, 92, 92, 93, 93, 93, 93, 93, 93, 93, 94, 94, 94, 94, 94, 95, 96, 96, 96, 96, 96, 96, 96, 97, 98, 99, 99, 99, 99, 100, 100, 101, 102, 103, 103, 103, 103, 103, 103, 103, 103, 103, 104, 104, 104, 105, 106, 106, 107, 108, 108, 108, 108, 109, 109, 109, 109, 109, 109, 109, 109, 109, 109, 109, 109, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 110, 111, 111, 111, 111, 111, 111, 112, 112, 112, 112, 112, 112, 112, 112, 112, 112, 112, 113, 113, 113, 113, 113, 113, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 115, 115, 115, 115, 116, 116, 116, 116, 116, 116, 116, 116, 117]</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>mixII</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>reward_punish</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>48</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.7102607879914284</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.711652274929273</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.8410895395009476), np.float64(0.8410895395009476), np.float64(0.8578133858046781), np.float64(0.8578133858046781), np.float64(0.8578133858046781), np.float64(0.8578133858046781), np.float64(0.8578133858046781), np.float64(0.8578133858046781), np.float64(0.8578133858046781), np.float64(0.8726268451472685), np.float64(0.8726268451472685), np.float64(0.8401709939919815), np.float64(0.8401709939919815), np.float64(0.8621688308130853), np.float64(0.7974854700945254), np.float64(0.7974854700945254), np.float64(0.7634183501906745), np.float64(0.7448599022597524), np.float64(0.7448599022597524), np.float64(0.7225384971430757), np.float64(0.7225384971430757), np.float64(0.7225384971430757), np.float64(0.7225384971430757), np.float64(0.7225384971430757), np.float64(0.6661857307328606), np.float64(0.6475828072235158), np.float64(0.6475828072235158), np.float64(0.6664000095956254), np.float64(0.6664000095956254), np.float64(0.6909474021082459), np.float64(0.6435114203161385), np.float64(0.6669971095155014), np.float64(0.6669971095155014), np.float64(0.6669971095155014), np.float64(0.6870717688267796), np.float64(0.6942281528545325), np.float64(0.6942281528545325), np.float64(0.6826721153067883), np.float64(0.6993539676979846), np.float64(0.7141126798298022), np.float64(0.7269958489167057), np.float64(0.7385616607185898), np.float64(0.7385616607185898), np.float64(0.7499074916476364), np.float64(0.7538027316482819), np.float64(0.7453331910820893), np.float64(0.7550560782759648), np.float64(0.7477907507351744), np.float64(0.7477907507351744), np.float64(0.7556523605069172), np.float64(0.761603757336559), np.float64(0.7447637646104164), np.float64(0.7447637646104164), np.float64(0.7447637646104164), np.float64(0.7315325957742199), np.float64(0.7315325957742199), np.float64(0.7315325957742199), np.float64(0.7315325957742199), np.float64(0.7281177438695859), np.float64(0.7354454211377988), np.float64(0.7408606681568959), np.float64(0.7393258333549154), np.float64(0.7439181284219466), np.float64(0.7439181284219466), np.float64(0.740857845302976), np.float64(0.7476314933305052), np.float64(0.7397272512196), np.float64(0.7308155400723643), np.float64(0.7200153237597322), np.float64(0.7250482476352244), np.float64(0.725587797383463), np.float64(0.7272098560863948), np.float64(0.7247550321150215), np.float64(0.7163348239694419), np.float64(0.7202858992526775), np.float64(0.7202858992526775), np.float64(0.712796990474771), np.float64(0.7132596829501074), np.float64(0.7148937291420367), np.float64(0.7148937291420367), np.float64(0.7199947206730982), np.float64(0.7199947206730982), np.float64(0.7166906994568827), np.float64(0.7166906994568827), np.float64(0.7197494871632433), np.float64(0.7242005595186642), np.float64(0.7280663400692771), np.float64(0.7307806655746891), np.float64(0.7210870219128929), np.float64(0.7257981122588788), np.float64(0.7257981122588788), np.float64(0.7303591012435308), np.float64(0.7294116558417266), np.float64(0.7297511457076672), np.float64(0.7253672522791349), np.float64(0.7131734565917703), np.float64(0.7159056825057295), np.float64(0.7199604223486842), np.float64(0.7127300355959619), np.float64(0.7162528218544271), np.float64(0.7162528218544271), np.float64(0.7159647577398363), np.float64(0.7070304504646405), np.float64(0.7105626095607759), np.float64(0.7098957610383779), np.float64(0.7138430123354588), np.float64(0.7165235149119215), np.float64(0.7193530334539724), np.float64(0.7193530334539724), np.float64(0.7138940122264673), np.float64(0.7176398124072453), np.float64(0.7193957682270481), np.float64(0.7226395794697825), np.float64(0.7261180217061878), np.float64(0.7251122362432457), np.float64(0.7275940507654223), np.float64(0.7271882845042769), np.float64(0.730436600111491), np.float64(0.7320491158087205), np.float64(0.7286390858801788), np.float64(0.7286390858801788), np.float64(0.7314514380263273), np.float64(0.7314514380263273), np.float64(0.7257524637068591), np.float64(0.7246380608120112), np.float64(0.7215911225268935), np.float64(0.7238215046065112), np.float64(0.717436340890489), np.float64(0.7204975244129603), np.float64(0.7234278854212155), np.float64(0.7256013766783529), np.float64(0.7214614072775887), np.float64(0.7139717561646276), np.float64(0.7149566822681618), np.float64(0.7177831508055007), np.float64(0.7206268243264263), np.float64(0.7233726905338136), np.float64(0.726093493634274), np.float64(0.7259858858006722), np.float64(0.7286095817977757), np.float64(0.7208959564241937), np.float64(0.7206219341294907), np.float64(0.7176957787160146), np.float64(0.716061604309669), np.float64(0.7185019560353036), np.float64(0.7115326524218698), np.float64(0.7136471385856291), np.float64(0.7072180983514039), np.float64(0.7097776674632522), np.float64(0.7118043181302024), np.float64(0.7063907166296535), np.float64(0.70569249098489), np.float64(0.7080614330805127), np.float64(0.7093495857676752), np.float64(0.7041429370283061), np.float64(0.6994952419486682), np.float64(0.6999362321190368), np.float64(0.6996136679709711), np.float64(0.7019828898472382), np.float64(0.7031874943326734), np.float64(0.7055689679190388), np.float64(0.7033703279562411), np.float64(0.7037215609721917), np.float64(0.7031665082481082), np.float64(0.7036633501301757), np.float64(0.7056149697585702), np.float64(0.7039247186944642), np.float64(0.7012848639364511), np.float64(0.7034733814617609), np.float64(0.705695913745329), np.float64(0.7078228854655771), np.float64(0.7081860781289382), np.float64(0.7077468217138452), np.float64(0.7063678811394172), np.float64(0.7080676065160609), np.float64(0.709668832186856), np.float64(0.7103246831036151), np.float64(0.712006579435992), np.float64(0.7136218630730468), np.float64(0.7100312799623559), np.float64(0.711048869698748), np.float64(0.7112893474013228), np.float64(0.7130615123594906), np.float64(0.7116066718918898), np.float64(0.7132559935231142), np.float64(0.7100835076545603), np.float64(0.7108561094440004), np.float64(0.7056680240487667), np.float64(0.707581122120068), np.float64(0.7094615588351596), np.float64(0.7111062393656233), np.float64(0.7121181505655533), np.float64(0.7081467033265492), np.float64(0.7068464720503367), np.float64(0.708056554266966), np.float64(0.7098585909115482), np.float64(0.7083058077297834), np.float64(0.7099829993956036), np.float64(0.7117582802527087), np.float64(0.7135264680738327), np.float64(0.7121491493935367), np.float64(0.7115946977749774), np.float64(0.7116533422655881), np.float64(0.7119892722832856), np.float64(0.7085601849770475), np.float64(0.7094328338347604), np.float64(0.711110560506859), np.float64(0.7091717526052975), np.float64(0.7088557423602668), np.float64(0.7087144069669458), np.float64(0.7103822833125136), np.float64(0.7058735895327514), np.float64(0.7075364513667015), np.float64(0.7090254193133239), np.float64(0.7066364481939147), np.float64(0.7081724983235733), np.float64(0.7082329113736314), np.float64(0.7075922838564239), np.float64(0.7056128605058387), np.float64(0.7068013741497712), np.float64(0.7050879147707726), np.float64(0.7046718330543962), np.float64(0.7061367736354807), np.float64(0.7075112221624036), np.float64(0.708805622245102), np.float64(0.7103384445937587), np.float64(0.7108140242830775), np.float64(0.7105495509080301), np.float64(0.7110566336919587), np.float64(0.710841727384732), np.float64(0.7120810671825666), np.float64(0.7131801349959804), np.float64(0.7119110572481478), np.float64(0.7132174050641679), np.float64(0.7144974364727574), np.float64(0.7148375034301506), np.float64(0.7152613634566566), np.float64(0.7153094601547747), np.float64(0.7144931649763268), np.float64(0.7154414526247889), np.float64(0.7153637048636468), np.float64(0.7145246640630162), np.float64(0.7139189686067506), np.float64(0.7152948534651288), np.float64(0.7165870372843869), np.float64(0.7158063857650039), np.float64(0.7153037987795098), np.float64(0.7157401379047126), np.float64(0.7168334490049612), np.float64(0.7175181958595742), np.float64(0.7175181958595742), np.float64(0.7134264653409316), np.float64(0.713732903557961), np.float64(0.7148619844901553), np.float64(0.7160938027805517), np.float64(0.7171303651218779), np.float64(0.7179710098510692), np.float64(0.7155518196992479), np.float64(0.7164093956438273), np.float64(0.7173326063963402), np.float64(0.7168813551885608), np.float64(0.7165812998611619), np.float64(0.7160750063469801), np.float64(0.717004703823999), np.float64(0.7170661785500378), np.float64(0.7180328533004232), np.float64(0.7191987199790228), np.float64(0.7204111745955389), np.float64(0.7174119590140544), np.float64(0.7183495332619741), np.float64(0.7185190519262766), np.float64(0.7186843382780828), np.float64(0.7184889677257499), np.float64(0.7150457352591543), np.float64(0.7162163936492195), np.float64(0.7138209694137907), np.float64(0.710295738293223), np.float64(0.7114189557849911), np.float64(0.7095177189264246), np.float64(0.7098462426590237), np.float64(0.7108668168726369), np.float64(0.7117852703645388), np.float64(0.7103701827422418), np.float64(0.7112929132594646), np.float64(0.7111934725784603), np.float64(0.7117355572511612), np.float64(0.7118341118051368), np.float64(0.7126008642415961), np.float64(0.7092084795061184)]</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 10, 11, 11, 12, 13, 14, 15, 16, 17, 17, 18, 18, 19, 19, 19, 20, 20, 20, 21, 21, 22, 23, 24, 25, 25, 25, 26, 26, 27, 27, 27, 27, 28, 29, 29, 29, 30, 30, 30, 30, 30, 30, 31, 31, 31, 31, 31, 31, 32, 32, 32, 32, 33, 34, 34, 35, 36, 37, 37, 37, 37, 37, 37, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 38, 39, 39, 39, 39, 40, 40, 41, 41, 42, 42, 42, 42, 42, 42, 42, 43, 43, 43, 43, 43, 43, 43, 43, 43, 43, 44, 44, 44, 44, 44, 44, 44, 44, 45, 45, 45, 45, 45, 45, 45, 45, 45, 45, 45, 45, 46, 46, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 47, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48]</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>mixII</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>reward_punish</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>35</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.3510915378241632</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.3549424459164915</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.5613809972975317), np.float64(0.5613809972975317), np.float64(0.5613809972975317), np.float64(0.5613809972975317), np.float64(0.5613809972975317), np.float64(0.5613809972975317), np.float64(0.1739677338504445), np.float64(-0.10079867175297282), np.float64(0.1630354075060363), np.float64(0.1630354075060363), np.float64(0.1630354075060363), np.float64(0.1630354075060363), np.float64(0.1630354075060363), np.float64(0.1630354075060363), np.float64(0.33018606079636587), np.float64(0.33018606079636587), np.float64(0.33018606079636587), np.float64(0.33018606079636587), np.float64(0.4404042685197001), np.float64(0.4404042685197001), np.float64(0.5015510382632048), np.float64(0.4622076708640761), np.float64(0.517458391392391), np.float64(0.5572095971454201), np.float64(0.556821087078938), np.float64(0.4541153797479944), np.float64(0.4863283290185275), np.float64(0.42860636515453093), np.float64(0.4563059435259486), np.float64(0.48946237075926335), np.float64(0.48946237075926335), np.float64(0.5183972483198762), np.float64(0.5183972483198762), np.float64(0.4363352342724409), np.float64(0.4074632055723228), np.float64(0.43557647256873855), np.float64(0.37974978249572106), np.float64(0.3928276438212515), np.float64(0.3928276438212515), np.float64(0.3928276438212515), np.float64(0.40587714288675786), np.float64(0.39884559454484037), np.float64(0.3435438910682807), np.float64(0.3585437537523559), np.float64(0.30867202054582354), np.float64(0.3275764827154422), np.float64(0.3275764827154422), np.float64(0.33869601084950696), np.float64(0.3072831348936663), np.float64(0.3082387437352893), np.float64(0.32920145956000646), np.float64(0.3207236151611045), np.float64(0.3207236151611045), np.float64(0.28648974181018566), np.float64(0.2766234340433504), np.float64(0.2791905192799358), np.float64(0.2915270847986704), np.float64(0.2915270847986704), np.float64(0.3062513379761245), np.float64(0.2873003053068835), np.float64(0.28192104817445357), np.float64(0.29923221312156006), np.float64(0.30792336910283824), np.float64(0.28744680080686336), np.float64(0.30249262491428275), np.float64(0.3179766853427923), np.float64(0.31904722654964074), np.float64(0.3334888751516638), np.float64(0.31326205754931796), np.float64(0.3091162155998719), np.float64(0.3193142811417012), np.float64(0.320456612699788), np.float64(0.31177929310055436), np.float64(0.3117792931005544), np.float64(0.32170847042051476), np.float64(0.3314363590726107), np.float64(0.31766893304980676), np.float64(0.31766893304980676), np.float64(0.319336125440348), np.float64(0.32260990680051643), np.float64(0.30377556365205954), np.float64(0.3059892423987712), np.float64(0.30703704893332584), np.float64(0.30200394230948924), np.float64(0.31150659457834073), np.float64(0.31150659457834073), np.float64(0.31817010119691225), np.float64(0.3063601865014078), np.float64(0.3020429387071867), np.float64(0.28871888532220685), np.float64(0.28613144373619936), np.float64(0.2945479781122053), np.float64(0.28846803482058736), np.float64(0.28846803482058736), np.float64(0.29814534995689207), np.float64(0.2957665233123193), np.float64(0.3047139959604847), np.float64(0.29337591760580983), np.float64(0.3024765482707148), np.float64(0.3095071569591138), np.float64(0.3185433343499989), np.float64(0.32739323780291246), np.float64(0.33410810724623663), np.float64(0.33438655660406597), np.float64(0.3225915309624984), np.float64(0.3275983369362411), np.float64(0.3310224437313963), np.float64(0.3384498566461792), np.float64(0.3460377396427358), np.float64(0.3442530172737583), np.float64(0.3442530172737583), np.float64(0.3507528618210181), np.float64(0.3501859281838194), np.float64(0.3555116128696033), np.float64(0.36169536098444743), np.float64(0.3666210723650544), np.float64(0.3666210723650544), np.float64(0.3703541088488923), np.float64(0.3769881130113498), np.float64(0.38024030064708275), np.float64(0.3860761006567135), np.float64(0.3860761006567135), np.float64(0.3923285209409924), np.float64(0.3890583698060963), np.float64(0.393670330961823), np.float64(0.399572163160991), np.float64(0.4036505364216684), np.float64(0.40806140748999686), np.float64(0.39598246571881535), np.float64(0.39747596219056947), np.float64(0.38544205372234785), np.float64(0.38827548970134357), np.float64(0.3846108757192838), np.float64(0.39040070949968614), np.float64(0.38523759621429576), np.float64(0.37739097441765806), np.float64(0.3675615449302574), np.float64(0.3637470702242581), np.float64(0.36920719541808955), np.float64(0.3723688558968118), np.float64(0.3768764038461648), np.float64(0.37268222352789354), np.float64(0.37810752488735205), np.float64(0.3809980677821648), np.float64(0.3823289945466001), np.float64(0.3846088123186497), np.float64(0.38953209870876165), np.float64(0.39352306750814287), np.float64(0.3826374793130622), np.float64(0.37305422819823614), np.float64(0.37799012908400503), np.float64(0.3771761718871732), np.float64(0.37107898434611236), np.float64(0.3704669630144669), np.float64(0.36237796206701284), np.float64(0.35420343658328074), np.float64(0.3587117814875577), np.float64(0.36079573945569193), np.float64(0.3594102676234934), np.float64(0.36396106310995696), np.float64(0.3664624877586593), np.float64(0.36796350700351044), np.float64(0.37229044038134873), np.float64(0.3764824021711175), np.float64(0.37870210863783627), np.float64(0.3827547405025246), np.float64(0.37546940462603073), np.float64(0.36774519181940024), np.float64(0.3721262664276968), np.float64(0.37212626642769686), np.float64(0.36974977963712496), np.float64(0.3710572105602825), np.float64(0.37323076027330937), np.float64(0.369521897811015), np.float64(0.37102706605784347), np.float64(0.3673035352628817), np.float64(0.3685805772280483), np.float64(0.3698270904504334), np.float64(0.3732102636786698), np.float64(0.3757934159110923), np.float64(0.369290390160939), np.float64(0.3680903636791163), np.float64(0.37187020159561557), np.float64(0.3693523436908121), np.float64(0.37337295294130296), np.float64(0.3769155055397727), np.float64(0.3795420193572501), np.float64(0.377487825267318), np.float64(0.3710670214139914), np.float64(0.36460038124566196), np.float64(0.36849452080165207), np.float64(0.3722747700240199), np.float64(0.3689647059195922), np.float64(0.3725403058873431), np.float64(0.3763169713713887), np.float64(0.38002707111549217), np.float64(0.37595702646865464), np.float64(0.3729556061502693), np.float64(0.3765176185850817), np.float64(0.36933394453595964), np.float64(0.3648569610961828), np.float64(0.3685011675228905), np.float64(0.3694003146538964), np.float64(0.36380223027337), np.float64(0.35695272602894224), np.float64(0.35892341834551617), np.float64(0.35289262272547994), np.float64(0.35085078526694896), np.float64(0.3516791550549986), np.float64(0.3452459855977261), np.float64(0.3478352018407684), np.float64(0.3420145106878128), np.float64(0.3455166412367966), np.float64(0.3399221797834742), np.float64(0.3344713791605137), np.float64(0.3296552849240229), np.float64(0.32932061959867964), np.float64(0.3316480529897263), np.float64(0.3265322821869523), np.float64(0.3223343030860195), np.float64(0.3255134124478255), np.float64(0.32880038001226214), np.float64(0.33199645203168393), np.float64(0.3286947993120513), np.float64(0.3315305446337774), np.float64(0.3330821813616705), np.float64(0.33345590787917007), np.float64(0.3355505078438535), np.float64(0.33202907770604156), np.float64(0.3353489615978137), np.float64(0.3378406346075396), np.float64(0.3351878637296499), np.float64(0.32970072220097757), np.float64(0.33296102886713846), np.float64(0.33491331777275407), np.float64(0.3313596588334464), np.float64(0.32858078883648906), np.float64(0.3316570957841863), np.float64(0.3339000996089306), np.float64(0.33698395063890174), np.float64(0.3400457305366238), np.float64(0.3344845923762294), np.float64(0.33660256430752267), np.float64(0.3396827614797636), np.float64(0.33880965547414704), np.float64(0.3417521061181514), np.float64(0.34457879045447504), np.float64(0.347381801614765), np.float64(0.34547958542669993), np.float64(0.34089164887318835), np.float64(0.3373424693285098), np.float64(0.3402931811778694), np.float64(0.34251552987899914), np.float64(0.3452895890741458), np.float64(0.34705928082832804), np.float64(0.3477638850063495), np.float64(0.350578678568804), np.float64(0.35332876531734514), np.float64(0.3507901475959249), np.float64(0.3532764719193097), np.float64(0.3520494778321772), np.float64(0.35454838108475595), np.float64(0.3500684107343667), np.float64(0.3481596297446729), np.float64(0.34695066021180165), np.float64(0.3420691379293914), np.float64(0.34468872158540154), np.float64(0.3451672782678478), np.float64(0.3474823599272539), np.float64(0.349215216881792), np.float64(0.35037289897121554), np.float64(0.3483288738867663), np.float64(0.35051201397696535), np.float64(0.34770276170084335), np.float64(0.3492607535571197), np.float64(0.3489245866274832), np.float64(0.3462708687075007), np.float64(0.3455474008223551), np.float64(0.3415680470126389), np.float64(0.341478983090023), np.float64(0.34309317208256856), np.float64(0.3453840502617439), np.float64(0.34422652566921547), np.float64(0.34661791709309525), np.float64(0.34400744531347016), np.float64(0.3465204329074737), np.float64(0.3472317129886112), np.float64(0.347419195753027), np.float64(0.3498816302970681), np.float64(0.345980358794265), np.float64(0.3484683984300726), np.float64(0.3508416029862603), np.float64(0.3533005140258961)]</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 6, 7, 8, 9, 10, 11, 11, 11, 11, 12, 13, 14, 15, 16, 16, 17, 18, 19, 19, 20, 20, 20, 20, 20, 20, 20, 20, 20, 20, 20, 21, 21, 22, 22, 22, 22, 22, 22, 23, 24, 24, 24, 24, 24, 24, 24, 25, 25, 25, 25, 25, 25, 26, 26, 26, 26, 26, 27, 27, 27, 27, 27, 27, 27, 27, 27, 27, 27, 27, 27, 27, 27, 27, 28, 28, 28, 28, 29, 29, 29, 29, 29, 29, 29, 29, 30, 30, 30, 30, 30, 30, 30, 30, 31, 31, 31, 31, 31, 31, 31, 31, 31, 31, 31, 31, 31, 31, 31, 31, 31, 32, 32, 32, 32, 32, 32, 33, 33, 33, 33, 33, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35]</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>mixI</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>185</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.6579821206204129</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.4113455932716717</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(-0.49393714136525446), np.float64(-0.49393714136525446), np.float64(-0.49393714136525446), np.float64(-0.49393714136525446), np.float64(-0.49393714136525446), np.float64(-0.49393714136525446), np.float64(-0.49393714136525446), np.float64(-0.5714409464334387), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.09692152855000591), np.float64(-0.10639738460402695), np.float64(-0.10639738460402695), np.float64(-0.10639738460402695), np.float64(-0.10639738460402695), np.float64(-0.10639738460402695), np.float64(-0.10639738460402695), np.float64(-0.10639738460402695), np.float64(-0.10639738460402695), np.float64(-0.10639738460402695), np.float64(-0.09518986181830841), np.float64(-0.09518986181830841), np.float64(-0.0951898618183084), np.float64(-0.0951898618183084), np.float64(-0.0951898618183084), np.float64(-0.0951898618183084), np.float64(-0.0951898618183084), np.float64(-0.0951898618183084), np.float64(-0.0951898618183084), np.float64(-0.0951898618183084), np.float64(-0.0951898618183084), np.float64(-0.0951898618183084), np.float64(-0.0951898618183084), np.float64(-0.0951898618183084), np.float64(-0.0951898618183084), np.float64(-0.0951898618183084), np.float64(-0.08586392978501721), np.float64(-0.08586392978501721), np.float64(-0.08586392978501721), np.float64(-0.08586392978501721), np.float64(-0.08586392978501721), np.float64(-0.08586392978501721), np.float64(-0.08586392978501721), np.float64(-0.08586392978501721), np.float64(-0.08586392978501721), np.float64(-0.08586392978501721), np.float64(0.03494795609981912), np.float64(0.03494795609981912), np.float64(0.03494795609981912), np.float64(0.03494795609981912), np.float64(0.03494795609981912), np.float64(0.03494795609981912), np.float64(0.03494795609981912), np.float64(0.03494795609981912), np.float64(0.12353466986452286), np.float64(0.12353466986452286), np.float64(0.12353466986452286), np.float64(0.12353466986452286), np.float64(0.12353466986452286), np.float64(0.12353466986452286), np.float64(0.12353466986452286), np.float64(0.19324481192885357), np.float64(0.19324481192885354), np.float64(0.26047646741471525), np.float64(0.26047646741471525), np.float64(0.26047646741471525), np.float64(0.26047646741471525), np.float64(0.26047646741471525), np.float64(0.3183376558842619), np.float64(0.37384035051102), np.float64(0.4216066157126692), np.float64(0.4216066157126692), np.float64(0.4216066157126692), np.float64(0.4216066157126692), np.float64(0.46067292873313515), np.float64(0.46067292873313515), np.float64(0.46067292873313515), np.float64(0.46067292873313515), np.float64(0.4606729287331351), np.float64(0.4606729287331351), np.float64(0.4606729287331351), np.float64(0.4606729287331351), np.float64(0.4606729287331351), np.float64(0.4606729287331351), np.float64(0.4606729287331351), np.float64(0.4956613286347599), np.float64(0.4956613286347599), np.float64(0.49566132863476003), np.float64(0.49566132863476003), np.float64(0.5091536117265651), np.float64(0.5091536117265651), np.float64(0.5091536117265651), np.float64(0.48649218011873563), np.float64(0.48649218011873563), np.float64(0.4907234775377204), np.float64(0.4974733954533376), np.float64(0.4974733954533376), np.float64(0.4974733954533376), np.float64(0.5162345542398394), np.float64(0.5162345542398394), np.float64(0.5162345542398394), np.float64(0.501327365647377), np.float64(0.501327365647377), np.float64(0.5062891973678847), np.float64(0.5190235169175185), np.float64(0.5317237584199066), np.float64(0.5317237584199066), np.float64(0.5317237584199066), np.float64(0.5479224810814469), np.float64(0.5479224810814469), np.float64(0.5479224810814469), np.float64(0.5479224810814469), np.float64(0.5645276510460683), np.float64(0.5645276510460683), np.float64(0.5645276510460683), np.float64(0.5601606888812619), np.float64(0.5748685720559313), np.float64(0.5640370898489133), np.float64(0.5527106612243196), np.float64(0.5578022327512662), np.float64(0.5578022327512662), np.float64(0.5578022327512662), np.float64(0.5578022327512662), np.float64(0.5578022327512662), np.float64(0.5578022327512662), np.float64(0.5578022327512662), np.float64(0.5674951300910202), np.float64(0.5674951300910202), np.float64(0.5674951300910202), np.float64(0.5792836251812168), np.float64(0.5792836251812168), np.float64(0.5819052022113153), np.float64(0.5819052022113153), np.float64(0.5920352034746454), np.float64(0.5793506549583891), np.float64(0.5637250955634879), np.float64(0.5637250955634879), np.float64(0.5751971767317262), np.float64(0.5751971767317262), np.float64(0.5732909075484943), np.float64(0.5799517778278995), np.float64(0.5799517778278995), np.float64(0.5885461760938175), np.float64(0.5885461760938175), np.float64(0.5885461760938175), np.float64(0.5885461760938175), np.float64(0.5885461760938175), np.float64(0.5955200944343709), np.float64(0.5955200944343709), np.float64(0.5955200944343709), np.float64(0.5955200944343709), np.float64(0.5955200944343709), np.float64(0.5918070387015469), np.float64(0.599457162792564), np.float64(0.599457162792564), np.float64(0.599457162792564), np.float64(0.599457162792564), np.float64(0.5893251991966869), np.float64(0.5893251991966868), np.float64(0.5837104447565615), np.float64(0.5713806089894532), np.float64(0.5705500030237598), np.float64(0.5705500030237598), np.float64(0.5667731350110558), np.float64(0.5623510810583886), np.float64(0.5630309785714526), np.float64(0.5712698595918912), np.float64(0.5712698595918912), np.float64(0.5712698595918912), np.float64(0.579305999359755), np.float64(0.5711312772790963), np.float64(0.5711312772790963), np.float64(0.5783300643931965), np.float64(0.5783300643931965), np.float64(0.5797544476140402), np.float64(0.5752328509083187), np.float64(0.5814572624289017), np.float64(0.5814572624289017), np.float64(0.5863300831660974), np.float64(0.5900647578428528), np.float64(0.5900647578428528), np.float64(0.5895722791161847), np.float64(0.5895722791161847), np.float64(0.5895722791161847), np.float64(0.5895722791161847), np.float64(0.5947293458441972), np.float64(0.592029284948779), np.float64(0.5863176013519452), np.float64(0.5910097106750793), np.float64(0.5961252872624796), np.float64(0.6020435312192932), np.float64(0.606019154955155), np.float64(0.6115064736280236), np.float64(0.6162527112809949), np.float64(0.6203450388449935), np.float64(0.6203450388449935), np.float64(0.6203450388449935), np.float64(0.6232941853609426), np.float64(0.6283969087515835), np.float64(0.6283969087515835), np.float64(0.6322378059063797), np.float64(0.6269753017521844), np.float64(0.6318164987328269), np.float64(0.6318164987328269), np.float64(0.6318164987328269), np.float64(0.6318164987328269), np.float64(0.6362652025027488), np.float64(0.6362652025027488), np.float64(0.6362652025027488), np.float64(0.640344167663331), np.float64(0.6343960395279763), np.float64(0.6242893042661865), np.float64(0.6242893042661865), np.float64(0.6242893042661865), np.float64(0.6242893042661863), np.float64(0.6289150789953041), np.float64(0.6330379335327032), np.float64(0.6330379335327032), np.float64(0.6330379335327032), np.float64(0.6330379335327032), np.float64(0.6352786532339406), np.float64(0.6334379013444978), np.float64(0.6374845038885044), np.float64(0.6305526159107614), np.float64(0.6249726048040534), np.float64(0.6249726048040534), np.float64(0.6259090124854331), np.float64(0.6295711765297695), np.float64(0.6332687669861777), np.float64(0.6365461859668706), np.float64(0.6401873809203902), np.float64(0.6440491653063734), np.float64(0.6390702513412837), np.float64(0.6420814322295436), np.float64(0.645471771946651), np.float64(0.645471771946651), np.float64(0.645471771946651), np.float64(0.645471771946651), np.float64(0.6454487157976904), np.float64(0.6484419053632245), np.float64(0.6493527368861908), np.float64(0.652442798360144), np.float64(0.6547090615496977), np.float64(0.6527152308560095), np.float64(0.6527152308560095), np.float64(0.6553659801973452), np.float64(0.6474799901793625), np.float64(0.6499674136786612), np.float64(0.6532662144742678), np.float64(0.6562736737477113), np.float64(0.6498238792014749), np.float64(0.6498238792014749), np.float64(0.6489120656893929), np.float64(0.6513251520289497), np.float64(0.6497074553970666), np.float64(0.6523971944082886), np.float64(0.6548004878281657), np.float64(0.6577793904710671)]</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 22, 23, 24, 25, 26, 27, 28, 28, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 49, 50, 51, 52, 53, 54, 55, 56, 57, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 81, 82, 83, 84, 85, 86, 87, 88, 88, 89, 90, 91, 92, 93, 94, 94, 95, 95, 96, 97, 98, 99, 99, 99, 99, 100, 101, 102, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 112, 113, 114, 115, 115, 116, 117, 117, 118, 118, 118, 119, 120, 120, 121, 122, 122, 123, 123, 123, 123, 124, 125, 125, 126, 127, 128, 128, 129, 130, 130, 130, 130, 130, 130, 131, 132, 133, 134, 135, 136, 136, 137, 138, 138, 139, 139, 140, 140, 140, 140, 141, 141, 142, 142, 142, 143, 143, 144, 145, 146, 147, 147, 148, 149, 150, 151, 151, 151, 152, 153, 154, 154, 155, 155, 155, 155, 156, 156, 156, 156, 156, 157, 158, 158, 158, 159, 159, 160, 160, 160, 160, 161, 161, 161, 162, 162, 163, 164, 165, 165, 165, 165, 165, 165, 165, 165, 165, 165, 165, 166, 167, 167, 167, 168, 168, 168, 168, 169, 170, 171, 171, 172, 173, 173, 173, 173, 174, 175, 176, 176, 176, 177, 178, 179, 179, 179, 179, 179, 179, 180, 180, 180, 180, 180, 180, 180, 180, 180, 180, 181, 182, 183, 183, 183, 183, 183, 183, 183, 184, 184, 184, 184, 184, 184, 184, 185, 185, 185, 185, 185, 185, 185]</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>mixI</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>103</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.1803470604523821</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.1576546978169831</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(0.31113636172530224), np.float64(-0.2250785080901173), np.float64(-0.2250785080901173), np.float64(-0.4805650548152232), np.float64(-0.4805650548152232), np.float64(-0.4805650548152232), np.float64(-0.4805650548152232), np.float64(-0.5891219680066612), np.float64(-0.5891219680066612), np.float64(-0.5891219680066612), np.float64(-0.5333505894699295), np.float64(-0.49794557992155647), np.float64(-0.49794557992155647), np.float64(-0.49794557992155647), np.float64(-0.3755526345438485), np.float64(-0.3755526345438485), np.float64(-0.3755526345438485), np.float64(-0.40341052033660435), np.float64(-0.40341052033660435), np.float64(-0.40341052033660435), np.float64(-0.40341052033660435), np.float64(-0.2530282628333266), np.float64(-0.20959617829344243), np.float64(-0.28007586429223824), np.float64(-0.28007586429223824), np.float64(-0.28007586429223824), np.float64(-0.28007586429223824), np.float64(-0.2438864999189009), np.float64(-0.2438864999189009), np.float64(-0.2438864999189009), np.float64(-0.2438864999189009), np.float64(-0.2438864999189009), np.float64(-0.3009064276957767), np.float64(-0.2998827509515736), np.float64(-0.3136692405137592), np.float64(-0.3136692405137592), np.float64(-0.3187059934267828), np.float64(-0.2667462267407242), np.float64(-0.2684257108743633), np.float64(-0.27481178624210434), np.float64(-0.27481178624210434), np.float64(-0.27481178624210434), np.float64(-0.27481178624210434), np.float64(-0.24213250354126886), np.float64(-0.20495512840081717), np.float64(-0.20495512840081717), np.float64(-0.2398104898891202), np.float64(-0.19321570701613713), np.float64(-0.14734941175022373), np.float64(-0.14734941175022373), np.float64(-0.14734941175022373), np.float64(-0.14734941175022373), np.float64(-0.14734941175022373), np.float64(-0.14734941175022376), np.float64(-0.10460096315500841), np.float64(-0.10460096315500841), np.float64(-0.10460096315500841), np.float64(-0.13893131225577696), np.float64(-0.09882403262788055), np.float64(-0.1142181546020858), np.float64(-0.1142181546020858), np.float64(-0.11421815460208577), np.float64(-0.11421815460208577), np.float64(-0.129612798610955), np.float64(-0.1223538865052653), np.float64(-0.1223538865052653), np.float64(-0.1223538865052653), np.float64(-0.14840730035681593), np.float64(-0.14840730035681593), np.float64(-0.1125210261280292), np.float64(-0.1125210261280292), np.float64(-0.1125210261280292), np.float64(-0.09753021351217922), np.float64(-0.09753021351217922), np.float64(-0.06555011447639177), np.float64(-0.06555011447639177), np.float64(-0.06555011447639177), np.float64(-0.07425481767440215), np.float64(-0.08290649097209868), np.float64(-0.08290649097209868), np.float64(-0.08290649097209868), np.float64(-0.08986515082298474), np.float64(-0.11084714853190511), np.float64(-0.12986808705482636), np.float64(-0.10205475591449242), np.float64(-0.076061570034091), np.float64(-0.076061570034091), np.float64(-0.076061570034091), np.float64(-0.051420056398353765), np.float64(-0.046833593790006636), np.float64(-0.02337350137226335), np.float64(-0.02337350137226335), np.float64(-0.011287895612809306), np.float64(-0.007719137793543746), np.float64(-0.0045299242468052935), np.float64(0.004280725245734612), np.float64(-0.008381270761773401), np.float64(-0.008381270761773401), np.float64(-0.02125102720086476), np.float64(-0.022404642046132277), np.float64(-0.020451042698728043), np.float64(-0.005755424618429735), np.float64(0.012149629327621939), np.float64(0.0004747675181463523), np.float64(0.015236636963380623), np.float64(0.020814423245386442), np.float64(0.03686261136129739), np.float64(0.02115590787840739), np.float64(0.03101134271094231), np.float64(0.027111847379788105), np.float64(0.028945590245973006), np.float64(0.013897084555865906), np.float64(0.02828648927632961), np.float64(0.02828648927632961), np.float64(0.03681273899682782), np.float64(0.05140462487019775), np.float64(0.05140462487019775), np.float64(0.039780700328707765), np.float64(0.03816731752645846), np.float64(0.04655039418197278), np.float64(0.058550616910373776), np.float64(0.0700075213136863), np.float64(0.0675656248890301), np.float64(0.05965767745362396), np.float64(0.07174682937274404), np.float64(0.07752918019970198), np.float64(0.07752918019970198), np.float64(0.08887518782404574), np.float64(0.0982286656277055), np.float64(0.0948045216158178), np.float64(0.10321579107936954), np.float64(0.11154264427684749), np.float64(0.10754332931473654), np.float64(0.11074966098309053), np.float64(0.11955385970093867), np.float64(0.11955385970093867), np.float64(0.10924066664025808), np.float64(0.10390258511684954), np.float64(0.10390258511684954), np.float64(0.11316454471748688), np.float64(0.12327115648526726), np.float64(0.1302135770256754), np.float64(0.1302135770256754), np.float64(0.12373626566707716), np.float64(0.13235767206073348), np.float64(0.14078089454659815), np.float64(0.13592498872768083), np.float64(0.14517420477708268), np.float64(0.13327538423985186), np.float64(0.12742963967295473), np.float64(0.13650758473732813), np.float64(0.12865552295927157), np.float64(0.12570601995993574), np.float64(0.11455015951533959), np.float64(0.12027378921460312), np.float64(0.12817979625221854), np.float64(0.12556624713299622), np.float64(0.13220020818534248), np.float64(0.139879891072102), np.float64(0.139879891072102), np.float64(0.13769210132458276), np.float64(0.13020713735345976), np.float64(0.12158782323527398), np.float64(0.12644643311324888), np.float64(0.1250118244395743), np.float64(0.1150752070989359), np.float64(0.1150752070989359), np.float64(0.12098302801915259), np.float64(0.11160753298549965), np.float64(0.11824400182554712), np.float64(0.11311928849516488), np.float64(0.12076679201214117), np.float64(0.127542208715724), np.float64(0.12594060216674102), np.float64(0.1301957933730072), np.float64(0.13590929911294572), np.float64(0.14302705491233653), np.float64(0.1500227157304517), np.float64(0.141826635548661), np.float64(0.13896007021413923), np.float64(0.14320085114082853), np.float64(0.14843142986133873), np.float64(0.15064085754202716), np.float64(0.1447123324692446), np.float64(0.14961769692558535), np.float64(0.1541779409115114), np.float64(0.1541779409115114), np.float64(0.14834635689022502), np.float64(0.15394962248458785), np.float64(0.15868055310461895), np.float64(0.16493984173003526), np.float64(0.15665665335342543), np.float64(0.16290052462389212), np.float64(0.1675608496564299), np.float64(0.1709295490921691), np.float64(0.17568369352786184), np.float64(0.17568369352786184), np.float64(0.16939310431345045), np.float64(0.16720931031649444), np.float64(0.16370708460041575), np.float64(0.16786026291672757), np.float64(0.161530096626373), np.float64(0.1627809681095746), np.float64(0.15834552586059905), np.float64(0.1610469963100576), np.float64(0.15719823737183355), np.float64(0.15553030679995145), np.float64(0.15393456650943593), np.float64(0.1591947405127328), np.float64(0.1560490683790735), np.float64(0.1615922678964832), np.float64(0.1615922678964832), np.float64(0.15506592522636262), np.float64(0.16039073442529186), np.float64(0.16128358233551165), np.float64(0.1627659900647094), np.float64(0.1670991527490001), np.float64(0.1613808233983422), np.float64(0.15692628412190449), np.float64(0.15550852089337122), np.float64(0.1516615293485032), np.float64(0.1551172466054411), np.float64(0.1572214260969021), np.float64(0.15342180036730532), np.float64(0.14936451130736764), np.float64(0.1507923882815351), np.float64(0.1557992262044189), np.float64(0.14967640533857962), np.float64(0.15450385506053652), np.float64(0.15902738166301553), np.float64(0.15793693345670975), np.float64(0.15169265824919104), np.float64(0.1563495222844683), np.float64(0.16019747561377104), np.float64(0.1614214962442379), np.float64(0.1570388924638599), np.float64(0.16114679808771895), np.float64(0.1658512174839787), np.float64(0.1691257184694408), np.float64(0.17369780269990354), np.float64(0.1751000810921239), np.float64(0.17679827950156987), np.float64(0.17843067259734927), np.float64(0.17951581043563752), np.float64(0.17324487585496337), np.float64(0.17406379053323906), np.float64(0.17787213241339478), np.float64(0.18205818685422342), np.float64(0.1849873861335459), np.float64(0.1790871643841847), np.float64(0.17298428179799197), np.float64(0.17467560924283043), np.float64(0.17809574554886404), np.float64(0.181616254397011), np.float64(0.18312755464677405), np.float64(0.18312755464677405), np.float64(0.18323028636932506)]</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 42, 43, 43, 44, 45, 46, 46, 47, 48, 48, 48, 49, 50, 50, 51, 52, 52, 53, 54, 55, 55, 55, 55, 56, 57, 58, 58, 59, 60, 61, 62, 62, 62, 62, 63, 63, 63, 63, 63, 64, 65, 66, 66, 66, 67, 67, 67, 67, 68, 69, 70, 71, 72, 72, 73, 74, 74, 74, 74, 75, 76, 77, 77, 77, 78, 79, 79, 80, 80, 81, 82, 82, 83, 83, 84, 85, 85, 85, 86, 87, 87, 87, 87, 87, 87, 88, 89, 89, 89, 89, 90, 90, 90, 90, 90, 90, 91, 91, 91, 91, 91, 91, 91, 91, 91, 91, 91, 91, 91, 91, 91, 91, 92, 92, 92, 93, 93, 93, 93, 93, 93, 93, 93, 93, 93, 94, 94, 94, 94, 94, 94, 94, 94, 94, 95, 95, 95, 96, 96, 96, 96, 97, 97, 97, 97, 97, 97, 97, 97, 97, 97, 97, 97, 97, 97, 97, 97, 97, 98, 98, 98, 98, 98, 98, 98, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 99, 100, 100, 100, 100, 100, 100, 100, 100, 100, 100, 101, 101, 101, 101, 101, 101, 101, 101, 101, 101, 101, 101, 101, 101, 101, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 102, 103, 103]</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>mixI</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>57</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.6004929440777184</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.513054021482158</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(-0.8597994054785424), np.float64(-0.8597994054785424), np.float64(-0.8597994054785424), np.float64(-0.8597994054785424), np.float64(-0.8597994054785424), np.float64(-0.8597994054785424), np.float64(-0.8597994054785424), np.float64(-0.8597994054785424), np.float64(-0.8597994054785424), np.float64(-0.17146676633603147), np.float64(-0.17146676633603147), np.float64(-0.17146676633603147), np.float64(0.21785296231540993), np.float64(0.21785296231540993), np.float64(0.21785296231540993), np.float64(0.10948597293748477), np.float64(0.14709862570012316), np.float64(0.12180497334994467), np.float64(0.12180497334994467), np.float64(0.12180497334994467), np.float64(0.2393530965284458), np.float64(0.323614491668785), np.float64(0.323614491668785), np.float64(0.3736514839193856), np.float64(0.3736514839193856), np.float64(0.3736514839193856), np.float64(0.2675216287975024), np.float64(0.28045751079715325), np.float64(0.33989244489322257), np.float64(0.33989244489322257), np.float64(0.33989244489322257), np.float64(0.3398924448932225), np.float64(0.3398924448932225), np.float64(0.38823290380997527), np.float64(0.38823290380997527), np.float64(0.43107819111840323), np.float64(0.43107819111840323), np.float64(0.37879028308284296), np.float64(0.40884506334419307), np.float64(0.38800145789006646), np.float64(0.3820159194654068), np.float64(0.4077006826972157), np.float64(0.4077006826972157), np.float64(0.4077006826972157), np.float64(0.4077006826972157), np.float64(0.4077006826972157), np.float64(0.39059754605735897), np.float64(0.4195347953878245), np.float64(0.42364120393065136), np.float64(0.4147035177073334), np.float64(0.4147035177073334), np.float64(0.3842359357092884), np.float64(0.3842359357092884), np.float64(0.3842359357092884), np.float64(0.408084280581422), np.float64(0.43050852904427206), np.float64(0.41468742571844086), np.float64(0.41468742571844086), np.float64(0.41764839498073175), np.float64(0.41764839498073175), np.float64(0.4207919626410809), np.float64(0.4207919626410809), np.float64(0.4355419328217341), np.float64(0.4355419328217341), np.float64(0.45062645828784076), np.float64(0.4656633734399445), np.float64(0.48114323656467783), np.float64(0.45503592357979117), np.float64(0.4698938170309191), np.float64(0.47773056837967687), np.float64(0.47852842017374503), np.float64(0.47852842017374525), np.float64(0.4699895855341401), np.float64(0.4773168211929746), np.float64(0.4773168211929746), np.float64(0.4773168211929746), np.float64(0.477883079370743), np.float64(0.46404324808047653), np.float64(0.47673406842469257), np.float64(0.48064598937027375), np.float64(0.4921805318505873), np.float64(0.4921805318505873), np.float64(0.5029543694004985), np.float64(0.48264169742561885), np.float64(0.49254844558055455), np.float64(0.5002346132873216), np.float64(0.5048985379030451), np.float64(0.5104046605718991), np.float64(0.5195994690357756), np.float64(0.5168698114060406), np.float64(0.5159980992896049), np.float64(0.5246823801473182), np.float64(0.5050803520090877), np.float64(0.4913503318005283), np.float64(0.4722830230392229), np.float64(0.46665596498137646), np.float64(0.475041084448779), np.float64(0.4730530083254905), np.float64(0.48098006649474356), np.float64(0.4870780210837809), np.float64(0.4851228957216217), np.float64(0.48642555838229445), np.float64(0.4913538599812907), np.float64(0.499036032508454), np.float64(0.4870586711632476), np.float64(0.4942841605474675), np.float64(0.49807934289924044), np.float64(0.4943793398844442), np.float64(0.4904116672272636), np.float64(0.49517998608346514), np.float64(0.4924003850232352), np.float64(0.47872485056548403), np.float64(0.48305960301369133), np.float64(0.48848255580074396), np.float64(0.48782044527306306), np.float64(0.4854140608127537), np.float64(0.4910889153877904), np.float64(0.4961274198676267), np.float64(0.4961274198676267), np.float64(0.4961274198676267), np.float64(0.49677321079263764), np.float64(0.5016789517187502), np.float64(0.5060312490384042), np.float64(0.5093486106118278), np.float64(0.513887969868217), np.float64(0.513887969868217), np.float64(0.5111975465916495), np.float64(0.5149449513770324), np.float64(0.5181402035207441), np.float64(0.5179779857808282), np.float64(0.5209882087400847), np.float64(0.5203945543688147), np.float64(0.523261690574689), np.float64(0.5278188466208471), np.float64(0.5279923723520294), np.float64(0.5276980462056616), np.float64(0.5271011709149537), np.float64(0.5318777915819378), np.float64(0.5309562723243904), np.float64(0.5350946493125595), np.float64(0.5395524691638179), np.float64(0.5405060810249718), np.float64(0.5369900380067529), np.float64(0.5323569798489985), np.float64(0.5352093769244575), np.float64(0.5374638367677137), np.float64(0.5357149124623383), np.float64(0.5351914969376036), np.float64(0.5370336727151412), np.float64(0.5392791225628291), np.float64(0.5405112817479552), np.float64(0.5438369035956656), np.float64(0.54594671175303), np.float64(0.5497761019338756), np.float64(0.553673879244921), np.float64(0.554032173989663), np.float64(0.5556158892801015), np.float64(0.553210134210711), np.float64(0.5557008299952246), np.float64(0.5591646299198373), np.float64(0.5628294971783192), np.float64(0.5620832453568495), np.float64(0.5652641803990756), np.float64(0.5677376146084526), np.float64(0.5705833222712801), np.float64(0.5738607422299465), np.float64(0.5769181265131829), np.float64(0.5801580135771526), np.float64(0.5825483431682251), np.float64(0.58140212631794), np.float64(0.580540854814201), np.float64(0.5823490484778664), np.float64(0.5801587706581888), np.float64(0.5781983982568094), np.float64(0.5807318076558673), np.float64(0.5808258894759798), np.float64(0.5817162885178252), np.float64(0.5847681223317565), np.float64(0.5792123882202724), np.float64(0.5813026569392531), np.float64(0.583514992696516), np.float64(0.5797431375565667), np.float64(0.5724582341800003), np.float64(0.5666230176739715), np.float64(0.5689876985122352), np.float64(0.5714962651656842), np.float64(0.5707898551852243), np.float64(0.5636452114889352), np.float64(0.5643592846513176), np.float64(0.5624936751140719), np.float64(0.565149748698268), np.float64(0.5666164007617994), np.float64(0.5678765432178595), np.float64(0.5686815457562379), np.float64(0.5713370562188577), np.float64(0.5698754753961084), np.float64(0.5681872083085613), np.float64(0.5689634829693619), np.float64(0.5684050313180093), np.float64(0.5710694585809412), np.float64(0.573505718185626), np.float64(0.5751106528490829), np.float64(0.575405994489803), np.float64(0.5707413222078274), np.float64(0.5686463159911737), np.float64(0.5702356418948918), np.float64(0.5662279407671588), np.float64(0.5679279321885864), np.float64(0.5685334101544293), np.float64(0.5697924760690497), np.float64(0.5637327267604688), np.float64(0.5654331958761348), np.float64(0.5642471406019127), np.float64(0.5635292820708993), np.float64(0.563965972834844), np.float64(0.5664388111943822), np.float64(0.5688046170860481), np.float64(0.569711563874697), np.float64(0.5721049097591274), np.float64(0.5737420816684474), np.float64(0.5739417065800437), np.float64(0.5762671142119807), np.float64(0.5776983508215789), np.float64(0.5797049436952898), np.float64(0.5810528911393671), np.float64(0.5817671903037719), np.float64(0.5829504525667073), np.float64(0.5847775622615431), np.float64(0.5833515551714219), np.float64(0.5833239059689431), np.float64(0.5824959125367074), np.float64(0.5844862814058435), np.float64(0.5862254027898927), np.float64(0.5862518821389903), np.float64(0.5878884169849365), np.float64(0.5899951753540672), np.float64(0.5913238575384079), np.float64(0.5922019123425364), np.float64(0.5930654890983065), np.float64(0.5932385645006962), np.float64(0.5922837012942255), np.float64(0.5943119952955865), np.float64(0.5944673377673046), np.float64(0.5911773054295686), np.float64(0.5929010348088202), np.float64(0.5879147171771845), np.float64(0.589732413178959), np.float64(0.5917105646023328), np.float64(0.5936064561580966), np.float64(0.594016874199661), np.float64(0.5959487291292845), np.float64(0.5972512236681223), np.float64(0.5952545918650363), np.float64(0.5971388825983799), np.float64(0.5988248815010437), np.float64(0.5998352826897531), np.float64(0.6010394622170894), np.float64(0.6004047581775399), np.float64(0.6007862096977515), np.float64(0.6021381178281952), np.float64(0.6025280983849671), np.float64(0.6032858622200871), np.float64(0.6050602636632854), np.float64(0.6067995461212717), np.float64(0.6085225877269774), np.float64(0.6101006848944559), np.float64(0.6091213671193241), np.float64(0.6081596116870848), np.float64(0.608866878436647), np.float64(0.6043301639078847), np.float64(0.604314239157023), np.float64(0.60536482015954), np.float64(0.607056980751157), np.float64(0.6087364371351053), np.float64(0.6081500782189534), np.float64(0.6076342696394528), np.float64(0.6046109174283995), np.float64(0.6037331904858322), np.float64(0.6022219428148777), np.float64(0.6031485964140868), np.float64(0.6022496090606945), np.float64(0.6038977571384326), np.float64(0.6024791507802545)]</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 16, 17, 18, 19, 20, 21, 22, 23, 24, 24, 25, 26, 26, 27, 28, 28, 28, 28, 29, 30, 30, 30, 31, 31, 32, 33, 33, 33, 33, 34, 35, 36, 37, 37, 38, 38, 39, 39, 39, 39, 39, 39, 40, 41, 42, 43, 43, 43, 43, 43, 44, 44, 45, 46, 46, 46, 46, 47, 47, 48, 48, 49, 49, 50, 50, 50, 50, 50, 50, 50, 50, 51, 51, 51, 52, 53, 53, 53, 53, 53, 53, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 54, 55, 56, 56, 56, 56, 56, 56, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57, 57]</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>mixII</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>122</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.6534994447742879</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.5390622690667929</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.91958658990241), np.float64(0.91958658990241), np.float64(0.91958658990241), np.float64(0.7935726983565947), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7637020221683654), np.float64(0.7065525398050047), np.float64(0.7065525398050047), np.float64(0.7065525398050047), np.float64(0.7065525398050047), np.float64(0.7065525398050047), np.float64(0.7065525398050047), np.float64(0.7065525398050047), np.float64(0.7065525398050047), np.float64(0.7065525398050047), np.float64(0.7065525398050047), np.float64(0.7065525398050047), np.float64(0.5761123686078854), np.float64(0.5761123686078854), np.float64(0.5761123686078854), np.float64(0.5761123686078854), np.float64(0.6048436217548551), np.float64(0.6440933409907983), np.float64(0.6440933409907983), np.float64(0.6830435084056021), np.float64(0.6829700937068787), np.float64(0.6829700937068787), np.float64(0.6794762093972945), np.float64(0.6794762093972945), np.float64(0.6794762093972946), np.float64(0.6794762093972946), np.float64(0.6794762093972946), np.float64(0.6794762093972946), np.float64(0.7074977760460858), np.float64(0.7074977760460858), np.float64(0.7074977760460858), np.float64(0.71632141057035), np.float64(0.7163214105703499), np.float64(0.7163214105703499), np.float64(0.7163214105703499), np.float64(0.7163214105703499), np.float64(0.7031118968318981), np.float64(0.7227610217494751), np.float64(0.7227610217494751), np.float64(0.705990122938078), np.float64(0.6960693815838394), np.float64(0.6960693815838394), np.float64(0.7104762681624796), np.float64(0.7104762681624796), np.float64(0.7131194898637034), np.float64(0.7202252120680767), np.float64(0.7202252120680767), np.float64(0.7202252120680767), np.float64(0.7202252120680767), np.float64(0.7202252120680767), np.float64(0.7133908494289222), np.float64(0.7052545504617498), np.float64(0.7052545504617498), np.float64(0.7052545504617498), np.float64(0.6990998739642392), np.float64(0.6787337187469145), np.float64(0.6787337187469145), np.float64(0.6787337187469145), np.float64(0.6787337187469145), np.float64(0.6634195363900203), np.float64(0.6694352917531947), np.float64(0.6694352917531947), np.float64(0.6687932474230132), np.float64(0.6687932474230132), np.float64(0.650272133887289), np.float64(0.650272133887289), np.float64(0.6383431335260913), np.float64(0.6507485466629006), np.float64(0.6507485466629006), np.float64(0.6552282089719427), np.float64(0.646360718307802), np.float64(0.646360718307802), np.float64(0.6502042024250835), np.float64(0.6502042024250835), np.float64(0.6428121337330357), np.float64(0.627655635504842), np.float64(0.6378825709870846), np.float64(0.6378825709870846), np.float64(0.6471694981718628), np.float64(0.6366161062574643), np.float64(0.6289583429603013), np.float64(0.6328475655478798), np.float64(0.6328475655478798), np.float64(0.6328475655478798), np.float64(0.6375596789435136), np.float64(0.6375596789435136), np.float64(0.6375596789435136), np.float64(0.6425691052438933), np.float64(0.6508366660676831), np.float64(0.6508366660676831), np.float64(0.6578155232368494), np.float64(0.6578155232368494), np.float64(0.6578155232368494), np.float64(0.6629948932758238), np.float64(0.6629948932758238), np.float64(0.6629948932758238), np.float64(0.6544209423364612), np.float64(0.661933265631222), np.float64(0.6594531838551762), np.float64(0.6644916736670635), np.float64(0.6644916736670635), np.float64(0.6708468963413278), np.float64(0.673522080422579), np.float64(0.6765498349714233), np.float64(0.6774841318742003), np.float64(0.6774841318742003), np.float64(0.6783854138082531), np.float64(0.6760346878111653), np.float64(0.6803238241061388), np.float64(0.6684537989436878), np.float64(0.6684537989436878), np.float64(0.6597518340860921), np.float64(0.665582149833302), np.float64(0.6575682117548072), np.float64(0.6552888141215736), np.float64(0.660938699205615), np.float64(0.6584191832809093), np.float64(0.6584191832809093), np.float64(0.6584191832809093), np.float64(0.657414647856234), np.float64(0.6574146478562339), np.float64(0.6625776745760921), np.float64(0.6625776745760921), np.float64(0.6667911415861464), np.float64(0.6667911415861464), np.float64(0.6665666139527222), np.float64(0.6705023780958932), np.float64(0.6705023780958932), np.float64(0.6752604366601629), np.float64(0.6752604366601629), np.float64(0.676691641182464), np.float64(0.6811741494986384), np.float64(0.6854822020774373), np.float64(0.6854822020774373), np.float64(0.6813271947299165), np.float64(0.6813271947299165), np.float64(0.682064767411145), np.float64(0.6714733136160734), np.float64(0.6714733136160734), np.float64(0.6695339194659073), np.float64(0.6717928678589246), np.float64(0.6689638360369495), np.float64(0.6729097344804242), np.float64(0.6747793808938205), np.float64(0.6714195365330302), np.float64(0.6714195365330302), np.float64(0.6675334090567532), np.float64(0.6648880315326373), np.float64(0.6609538906207766), np.float64(0.6649811144854516), np.float64(0.6612280444304282), np.float64(0.6628763402477581), np.float64(0.6618794177038549), np.float64(0.6653194233976766), np.float64(0.6620015371143662), np.float64(0.6657570018260689), np.float64(0.6613415298155161), np.float64(0.6613415298155161), np.float64(0.6613415298155161), np.float64(0.6591261064800202), np.float64(0.6627606276790606), np.float64(0.6627606276790606), np.float64(0.6642074897370084), np.float64(0.667734711166115), np.float64(0.667734711166115), np.float64(0.667734711166115), np.float64(0.667734711166115), np.float64(0.669980827136742), np.float64(0.6642776671769652), np.float64(0.666967821557757), np.float64(0.6699429421346119), np.float64(0.6697810904347605), np.float64(0.6651266636060208), np.float64(0.6660883057268038), np.float64(0.6654264012898171), np.float64(0.66607766710235), np.float64(0.660534150752117), np.float64(0.6629446788280332), np.float64(0.6648953835389861), np.float64(0.6679704268757625), np.float64(0.6630946369948268), np.float64(0.6658399375471888), np.float64(0.6640715798729545), np.float64(0.6640715798729545), np.float64(0.6577930714486361), np.float64(0.6579062900210454), np.float64(0.6532218946259029), np.float64(0.6556435078454088), np.float64(0.6575679568227081), np.float64(0.6554073681362687), np.float64(0.6519423208200763), np.float64(0.6519423208200763), np.float64(0.6548344601975649), np.float64(0.6548344601975649), np.float64(0.6570354185713592), np.float64(0.6593842802224942), np.float64(0.6603082636932881), np.float64(0.6624338918245697), np.float64(0.6595760083584478), np.float64(0.6622847780518721), np.float64(0.6609561052165991), np.float64(0.6600809482008794), np.float64(0.6622557056148485), np.float64(0.6622557056148485), np.float64(0.662581197818262), np.float64(0.6617543237217599), np.float64(0.6609990427006225), np.float64(0.657105691643002), np.float64(0.6594254781227714), np.float64(0.6580897241450728), np.float64(0.6605161656802037), np.float64(0.6579331573019305), np.float64(0.6549003163920428), np.float64(0.6544131595981317), np.float64(0.6544131595981317), np.float64(0.6538686101415824), np.float64(0.6538686101415822), np.float64(0.6553785097249246), np.float64(0.6574371247626808), np.float64(0.6574371247626808), np.float64(0.6553747337418588), np.float64(0.654165736396285), np.float64(0.6562746520817164), np.float64(0.6561256025917067), np.float64(0.6551898036586804), np.float64(0.6551898036586804), np.float64(0.6498241407797112), np.float64(0.6520242683238003), np.float64(0.6540979606033163), np.float64(0.6522643030748795), np.float64(0.6522643030748795), np.float64(0.6522643030748795), np.float64(0.6526293441603808), np.float64(0.6522904550539202), np.float64(0.6486679764883869), np.float64(0.650385469045119), np.float64(0.6490228737053408), np.float64(0.651228422133028), np.float64(0.6499160398424014), np.float64(0.6512741131133057), np.float64(0.6488523291998195), np.float64(0.6484250220653772), np.float64(0.6504640030899863), np.float64(0.6493616941787763), np.float64(0.6513502462222032), np.float64(0.6523369385217422), np.float64(0.6515560056903477), np.float64(0.6531911820873929), np.float64(0.654247959331015), np.float64(0.655069311159344), np.float64(0.6566912902054699), np.float64(0.6559954627630786), np.float64(0.6527712084935241), np.float64(0.6502316411174762), np.float64(0.65034132337444), np.float64(0.6512069888608751), np.float64(0.6531569521125858), np.float64(0.6524616537609091), np.float64(0.6521915074854334), np.float64(0.6521915074854334)]</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 11, 12, 13, 13, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 47, 48, 49, 50, 50, 50, 51, 51, 51, 52, 52, 53, 54, 55, 56, 57, 57, 58, 59, 59, 60, 61, 62, 63, 63, 63, 64, 64, 64, 65, 65, 66, 66, 66, 67, 68, 69, 70, 70, 70, 71, 72, 72, 72, 73, 74, 75, 75, 75, 76, 76, 77, 77, 78, 78, 78, 79, 79, 79, 80, 80, 81, 81, 81, 81, 82, 82, 82, 82, 82, 83, 84, 84, 85, 86, 86, 86, 87, 87, 88, 89, 89, 90, 91, 91, 91, 91, 91, 92, 92, 92, 92, 92, 93, 93, 93, 93, 93, 94, 94, 94, 94, 94, 94, 94, 95, 96, 96, 97, 97, 98, 98, 99, 99, 99, 100, 100, 101, 101, 101, 101, 102, 102, 103, 103, 103, 104, 104, 104, 104, 104, 104, 104, 105, 105, 105, 105, 105, 105, 105, 105, 105, 105, 105, 105, 106, 107, 107, 107, 108, 108, 108, 109, 110, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 111, 112, 112, 112, 112, 112, 112, 112, 112, 113, 113, 114, 114, 114, 114, 114, 114, 114, 114, 114, 114, 115, 115, 115, 115, 115, 115, 115, 115, 115, 115, 115, 116, 116, 117, 117, 117, 118, 118, 118, 118, 118, 118, 119, 119, 119, 119, 119, 120, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 121, 122]</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>mixII</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>56</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.4093708094944672</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.332158180164872</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, np.float64(-0.5051623382760406), np.float64(-0.5051623382760406), np.float64(-0.5051623382760406), np.float64(-0.5051623382760406), np.float64(-0.014332918280086343), np.float64(-0.014332918280086343), np.float64(-0.014332918280086343), np.float64(-0.014332918280086343), np.float64(-0.014332918280086343), np.float64(0.24646408354725682), np.float64(0.24646408354725682), np.float64(0.24646408354725682), np.float64(0.24646408354725682), np.float64(0.24646408354725682), np.float64(0.24646408354725682), np.float64(0.24646408354725682), np.float64(0.24646408354725682), np.float64(0.24646408354725682), np.float64(0.4103111627476207), np.float64(0.4103111627476207), np.float64(0.41031116274762064), np.float64(0.41031116274762064), np.float64(0.41031116274762064), np.float64(0.41031116274762064), np.float64(0.41031116274762064), np.float64(0.1316118202911185), np.float64(0.1146362681780884), np.float64(0.1146362681780884), np.float64(0.1146362681780884), np.float64(0.1146362681780884), np.float64(0.1146362681780884), np.float64(0.0039343526772174075), np.float64(0.0039343526772174075), np.float64(0.0039343526772174075), np.float64(0.0039343526772174075), np.float64(0.12844038474890324), np.float64(0.1792981508517354), np.float64(0.13855076274029843), np.float64(0.13855076274029843), np.float64(0.21603967031067528), np.float64(0.21603967031067528), np.float64(0.24381921908428542), np.float64(0.28772821543424665), np.float64(0.28772821543424665), np.float64(0.3383500570684794), np.float64(0.35930443480313207), np.float64(0.33716873623651655), np.float64(0.35952048013809745), np.float64(0.3212552340542143), np.float64(0.28102562047214197), np.float64(0.267476691837168), np.float64(0.267476691837168), np.float64(0.267476691837168), np.float64(0.267476691837168), np.float64(0.29004896911102146), np.float64(0.29004896911102146), np.float64(0.2577943890935241), np.float64(0.2577943890935241), np.float64(0.2900584709765759), np.float64(0.2900584709765759), np.float64(0.31963019443436574), np.float64(0.31963019443436574), np.float64(0.2699619832086779), np.float64(0.2923339741242852), np.float64(0.2923339741242852), np.float64(0.3157731421213968), np.float64(0.3402075577023309), np.float64(0.36282163157983177), np.float64(0.37211440807054863), np.float64(0.37642030863914777), np.float64(0.3372672764824297), np.float64(0.3422706553930682), np.float64(0.3422706553930682), np.float64(0.3583913845992459), np.float64(0.3606705933070456), np.float64(0.3775253000855019), np.float64(0.38946552334620715), np.float64(0.38946552334620715), np.float64(0.40547990277789214), np.float64(0.4153783932132349), np.float64(0.4153783932132349), np.float64(0.4153783932132349), np.float64(0.427246990342133), np.float64(0.4008539571795163), np.float64(0.38978005771982865), np.float64(0.40363132538335544), np.float64(0.41690420257495153), np.float64(0.41690420257495153), np.float64(0.40544167744263915), np.float64(0.41691496905630127), np.float64(0.41691496905630127), np.float64(0.4239439174293931), np.float64(0.4198215399584286), np.float64(0.41273884031907354), np.float64(0.4038746659955275), np.float64(0.4074745024548586), np.float64(0.4092225480025316), np.float64(0.388256842156835), np.float64(0.37776846883996856), np.float64(0.3642030907688864), np.float64(0.37334582911626385), np.float64(0.3840781855902992), np.float64(0.3912081212781285), np.float64(0.3802782260433872), np.float64(0.36562497736498917), np.float64(0.3618725596273333), np.float64(0.3632425365119285), np.float64(0.37328328869955346), np.float64(0.3738413438760242), np.float64(0.38004862929093014), np.float64(0.38562498217881963), np.float64(0.38818387518447917), np.float64(0.38818387518447917), np.float64(0.3836123386649544), np.float64(0.3872957452840805), np.float64(0.39422344255637587), np.float64(0.40087525484545405), np.float64(0.40909094281147973), np.float64(0.4088850747750444), np.float64(0.41672670276245005), np.float64(0.41945550794803027), np.float64(0.4266915846744342), np.float64(0.42537378850069624), np.float64(0.42023307930290926), np.float64(0.42668183970038803), np.float64(0.43073912909467726), np.float64(0.43642555371480707), np.float64(0.4377475978282626), np.float64(0.4424539769816775), np.float64(0.4463895973026386), np.float64(0.44266377668998735), np.float64(0.4305284113027536), np.float64(0.4179069143575673), np.float64(0.4024587069306415), np.float64(0.40696011288886125), np.float64(0.4031670531837915), np.float64(0.3988797289827239), np.float64(0.4053505375031767), np.float64(0.3924010357490073), np.float64(0.39298864896083135), np.float64(0.39935568104137503), np.float64(0.3981500734618068), np.float64(0.40429189982928904), np.float64(0.40429189982928904), np.float64(0.404342022394519), np.float64(0.40600632210065435), np.float64(0.4110353024713239), np.float64(0.40279628943541057), np.float64(0.40597697238067615), np.float64(0.4085084830556935), np.float64(0.4085084830556935), np.float64(0.40861987506815783), np.float64(0.4058585774889141), np.float64(0.3981555306862431), np.float64(0.3902216601090119), np.float64(0.3951912205975721), np.float64(0.3902556290635041), np.float64(0.3905838397664859), np.float64(0.39602003113440976), np.float64(0.401063823860465), np.float64(0.40531864344658136), np.float64(0.39372612825916997), np.float64(0.3933675120889411), np.float64(0.39815660730107966), np.float64(0.3989184099973072), np.float64(0.40383081532709847), np.float64(0.4032978420752827), np.float64(0.40760914965962175), np.float64(0.4046916509174598), np.float64(0.4089653459862071), np.float64(0.4063811179526264), np.float64(0.4109090968139524), np.float64(0.4142734965798994), np.float64(0.4185985987813347), np.float64(0.42226311430129565), np.float64(0.4154846440161919), np.float64(0.40752702372960686), np.float64(0.4087681978057673), np.float64(0.4094831283117167), np.float64(0.4098788801702706), np.float64(0.4136534852899556), np.float64(0.41538759512924683), np.float64(0.41940802935678134), np.float64(0.41517744101475046), np.float64(0.41813005566312184), np.float64(0.42043516244978235), np.float64(0.42455321801901635), np.float64(0.4235709905309943), np.float64(0.42541677382479864), np.float64(0.4294567523318631), np.float64(0.4251216517253976), np.float64(0.4251216517253976), np.float64(0.42514742629877816), np.float64(0.4221333430098953), np.float64(0.42393183066022855), np.float64(0.42352534797936964), np.float64(0.41448404713165343), np.float64(0.4158017549977268), np.float64(0.416722738276468), np.float64(0.4080692854754554), np.float64(0.4094660309572277), np.float64(0.40808925803508417), np.float64(0.4019254271607151), np.float64(0.39731632790929766), np.float64(0.39541020211023004), np.float64(0.38885459598929717), np.float64(0.389859048318859), np.float64(0.3922457371916413), np.float64(0.38787800492332897), np.float64(0.38892372864513725), np.float64(0.3890490655170459), np.float64(0.39170802520356757), np.float64(0.3928676460372107), np.float64(0.39069129386970597), np.float64(0.39040756009113853), np.float64(0.3900759072833449), np.float64(0.393689830918305), np.float64(0.393689830918305), np.float64(0.3971767659511392), np.float64(0.3971767659511392), np.float64(0.3971767659511392), np.float64(0.39755278495446383), np.float64(0.40090353979771115), np.float64(0.40435833375329516), np.float64(0.4054301393691499), np.float64(0.4084782895890654), np.float64(0.4092946488152961), np.float64(0.4094796602336397), np.float64(0.40953018068698666), np.float64(0.40672453563119493), np.float64(0.4007207879532273), np.float64(0.39871407269875303), np.float64(0.40154004304782065), np.float64(0.4048184639299838), np.float64(0.4039761298349891), np.float64(0.4046229439320496), np.float64(0.4073771222618361), np.float64(0.40875073101920495), np.float64(0.40919512261536367), np.float64(0.41170499297919777), np.float64(0.41447269546315896), np.float64(0.41309883295477995), np.float64(0.4160795873576246), np.float64(0.4191140597952485), np.float64(0.4124067295929047), np.float64(0.41282244999406376), np.float64(0.41578613257629904), np.float64(0.4101158237581164), np.float64(0.41286347293911074), np.float64(0.40844303716622854), np.float64(0.40624568589706767), np.float64(0.4092107756485406), np.float64(0.40372561834623083), np.float64(0.4055024431468076), np.float64(0.40806124192360077), np.float64(0.4085840854406338), np.float64(0.4024028177105308), np.float64(0.40518394238907945), np.float64(0.40656354974225495), np.float64(0.4017685340173634), np.float64(0.40224316989672865), np.float64(0.4050798046598206), np.float64(0.39987809503670946), np.float64(0.40165743347290384), np.float64(0.4035157432267903), np.float64(0.40090970089377415), np.float64(0.40318766049649507), np.float64(0.401785209222599), np.float64(0.39632380779215737), np.float64(0.39907204619441067), np.float64(0.39322402656795735), np.float64(0.3932051172938517), np.float64(0.39528541175596915), np.float64(0.3979614065135328), np.float64(0.4002304163480802), np.float64(0.40213952613982407), np.float64(0.4044019979305715), np.float64(0.40066752589576055), np.float64(0.40066752589576055), np.float64(0.4004743727989778), np.float64(0.4006882063666999), np.float64(0.39754268408075033), np.float64(0.3984458271512594), np.float64(0.4008582847459689), np.float64(0.4026594727420167), np.float64(0.4042862033263876), np.float64(0.40629292603527817), np.float64(0.4083123203147677), np.float64(0.4107207866330446), np.float64(0.412956018453752), np.float64(0.4130717403764159), np.float64(0.4142207431515476), np.float64(0.4099036622582959), np.float64(0.40617367768816676), np.float64(0.40755938080738874), np.float64(0.40902669934069724)]</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 3, 4, 5, 6, 6, 7, 8, 9, 10, 10, 11, 12, 13, 14, 15, 16, 17, 18, 18, 19, 20, 21, 22, 23, 24, 24, 24, 25, 26, 27, 28, 28, 29, 30, 31, 31, 31, 31, 32, 32, 33, 33, 33, 34, 34, 34, 34, 34, 34, 34, 34, 35, 36, 37, 37, 38, 38, 39, 39, 40, 40, 41, 41, 41, 42, 42, 42, 42, 42, 42, 42, 42, 43, 43, 43, 43, 43, 44, 44, 44, 45, 46, 46, 46, 46, 46, 46, 47, 47, 47, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 48, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 49, 50, 50, 50, 50, 50, 50, 50, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 51, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 52, 53, 53, 54, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 55, 56, 56, 56, 56, 56, 56, 56, 56, 56, 56, 56, 56, 56, 56, 56, 56, 56, 56]</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>mixII</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>35</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.6344781627115841</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.6004366222468586</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, np.float64(0.31764821135040205), np.float64(0.31764821135040205), np.float64(0.31764821135040205), np.float64(0.31764821135040205), np.float64(-0.11780706116489695), np.float64(-0.11780706116489695), np.float64(0.2544700559740481), np.float64(0.2544700559740481), np.float64(0.3611202941030417), np.float64(0.3611202941030417), np.float64(0.47108732618039645), np.float64(0.47108732618039645), np.float64(0.558270076575617), np.float64(0.5867558366793879), np.float64(0.6353934196975404), np.float64(0.6431801570018716), np.float64(0.6496161061086851), np.float64(0.597840893149527), np.float64(0.597840893149527), np.float64(0.6229731105055123), np.float64(0.6229731105055123), np.float64(0.5656562126627953), np.float64(0.5656562126627953), np.float64(0.5594078793057755), np.float64(0.5594078793057755), np.float64(0.5594078793057755), np.float64(0.5594078793057755), np.float64(0.5792624756332612), np.float64(0.5904661256303692), np.float64(0.5793977924969882), np.float64(0.5918938179839132), np.float64(0.6133729599820236), np.float64(0.5721319310780759), np.float64(0.5721319310780759), np.float64(0.5397217263590415), np.float64(0.5397217263590415), np.float64(0.5237466079159875), np.float64(0.5313753707700763), np.float64(0.547468042621236), np.float64(0.5651920668511927), np.float64(0.5681158659298325), np.float64(0.5739610562681514), np.float64(0.5888954991434746), np.float64(0.5956978057806759), np.float64(0.6090944778637176), np.float64(0.6025482270571593), np.float64(0.6148538052693294), np.float64(0.6255960238462204), np.float64(0.636594058040927), np.float64(0.6216627417652054), np.float64(0.6174443866426125), np.float64(0.609058682625021), np.float64(0.6174927900558217), np.float64(0.6182695520080288), np.float64(0.6216523953914395), np.float64(0.6216523953914395), np.float64(0.6296035642121448), np.float64(0.6296035642121448), np.float64(0.6345728167774319), np.float64(0.6381424641116203), np.float64(0.631056462403497), np.float64(0.6264248680518857), np.float64(0.6332195707779271), np.float64(0.6376020972751523), np.float64(0.6189306971251409), np.float64(0.6196101491019468), np.float64(0.6196101491019468), np.float64(0.6196101491019468), np.float64(0.6196101491019468), np.float64(0.6180133599328739), np.float64(0.6248605411076679), np.float64(0.6191118735160005), np.float64(0.6246001003291353), np.float64(0.6248381312896171), np.float64(0.621483649600782), np.float64(0.621483649600782), np.float64(0.6280634056881323), np.float64(0.6301898685018704), np.float64(0.6364903713079059), np.float64(0.6254859513378088), np.float64(0.6309639742499143), np.float64(0.6289854363470578), np.float64(0.6341486140162577), np.float64(0.6341486140162577), np.float64(0.6341486140162577), np.float64(0.6318334052810102), np.float64(0.6203445550436422), np.float64(0.6184978748439225), np.float64(0.6140198635021817), np.float64(0.6023103624593367), np.float64(0.6081225922123685), np.float64(0.6074968409351506), np.float64(0.6056196455194877), np.float64(0.5977166618494498), np.float64(0.5977166618494496), np.float64(0.6008546143073774), np.float64(0.605467145098402), np.float64(0.6068872357883685), np.float64(0.6097825709650407), np.float64(0.6140539012923895), np.float64(0.6190646527704784), np.float64(0.622193223227853), np.float64(0.619887274196004), np.float64(0.6245626317580465), np.float64(0.628725914698607), np.float64(0.6238260838351846), np.float64(0.6282938637599178), np.float64(0.6270286045937573), np.float64(0.6270337576076856), np.float64(0.6304835549851515), np.float64(0.63032901459361), np.float64(0.6324469190019518), np.float64(0.6229098171303539), np.float64(0.6246490751632029), np.float64(0.626550522073316), np.float64(0.6296561036873618), np.float64(0.6315784677719071), np.float64(0.632827069665269), np.float64(0.6316892635718108), np.float64(0.6348594984801629), np.float64(0.6332399794194483), np.float64(0.6369770458937359), np.float64(0.6335775722654038), np.float64(0.6316861771809608), np.float64(0.6344191165607728), np.float64(0.6357391505809485), np.float64(0.6387018134978003), np.float64(0.6414152940112617), np.float64(0.6414152940112617), np.float64(0.6359063995503018), np.float64(0.6384885505097964), np.float64(0.6360876105633598), np.float64(0.6307284418983272), np.float64(0.6296605364627716), np.float64(0.6279886420271765), np.float64(0.6303116327313779), np.float64(0.6250648027467378), np.float64(0.6208120849499476), np.float64(0.6169383242749101), np.float64(0.6199771287048946), np.float64(0.6121872396790105), np.float64(0.614254049280577), np.float64(0.607041639868825), np.float64(0.6073040844874185), np.float64(0.6100016876831925), np.float64(0.612825737582908), np.float64(0.6046180339248174), np.float64(0.6013189753908512), np.float64(0.6045012665677004), np.float64(0.6076634292333716), np.float64(0.6051905385059212), np.float64(0.6009727186189736), np.float64(0.6039610816217849), np.float64(0.6046465721317684), np.float64(0.6069701661629106), np.float64(0.6073705769178438), np.float64(0.6074503952604129), np.float64(0.6098048209847559), np.float64(0.6126124092926433), np.float64(0.6130660895061043), np.float64(0.6159066016223782), np.float64(0.617384426521344), np.float64(0.6199727955364799), np.float64(0.622696121988097), np.float64(0.6246176132067305), np.float64(0.6202436452495024), np.float64(0.6220351230233858), np.float64(0.6206668486532763), np.float64(0.6216894376829519), np.float64(0.6232038863423448), np.float64(0.6174487252625154), np.float64(0.6171501678424103), np.float64(0.6197215557577646), np.float64(0.6205413962811278), np.float64(0.6220951133343805), np.float64(0.6243996190627583), np.float64(0.6228196898842434), np.float64(0.6234393852318079), np.float64(0.6170414999399483), np.float64(0.618799875383658), np.float64(0.621180474273888), np.float64(0.6205154053849173), np.float64(0.6209647659917468), np.float64(0.6214785831046904), np.float64(0.6238228280419623), np.float64(0.6244426334590114), np.float64(0.6257300441589806), np.float64(0.6280219611027159), np.float64(0.6301520473196031), np.float64(0.6290844301243201), np.float64(0.6289413440140134), np.float64(0.6266179083907307), np.float64(0.6245759340260787), np.float64(0.6209921069665332), np.float64(0.6227739562804574), np.float64(0.6239826738024893), np.float64(0.6220111304700148), np.float64(0.6203009743286488), np.float64(0.6223474807586511), np.float64(0.6192939470730172), np.float64(0.6213129333195142), np.float64(0.6221641606316203), np.float64(0.6192783830125312), np.float64(0.6160823957346361), np.float64(0.6162688766918406), np.float64(0.6170963127666126), np.float64(0.61856740818096), np.float64(0.6194679325891355), np.float64(0.6214964685164186), np.float64(0.6214964685164186), np.float64(0.6224471025842824), np.float64(0.6244758859505569), np.float64(0.6230625634731072), np.float64(0.6240814432795246), np.float64(0.6243770152959996), np.float64(0.6263328893507286), np.float64(0.6248034157419611), np.float64(0.6254898458825056), np.float64(0.6246366559157194), np.float64(0.6249225323838612), np.float64(0.625978195840467), np.float64(0.6243932619362929), np.float64(0.6262560870491645), np.float64(0.6281059134751114), np.float64(0.6275964184652204), np.float64(0.6281737918204006), np.float64(0.6286375396733092), np.float64(0.6291069760588945), np.float64(0.6308656527234533), np.float64(0.6288191195782343), np.float64(0.6288536420969584), np.float64(0.6301401868892356), np.float64(0.6300391138193051), np.float64(0.6318034318520416), np.float64(0.628708844142748), np.float64(0.6259003814187952), np.float64(0.6271039798610283), np.float64(0.6280849909014872), np.float64(0.6298237637271188), np.float64(0.6293617580424835), np.float64(0.6289088704578545), np.float64(0.6300341089416565), np.float64(0.6312659021446598), np.float64(0.6326719038753569), np.float64(0.6333786064216338), np.float64(0.6344338120558087), np.float64(0.6359492803632106), np.float64(0.6370549278386269), np.float64(0.6336884376265552), np.float64(0.635282526118062), np.float64(0.6353968349858021), np.float64(0.6350335144865832), np.float64(0.6320330045107855), np.float64(0.633640526540963), np.float64(0.6348968065899918), np.float64(0.6364341072918545), np.float64(0.6342301118067494), np.float64(0.6331247924169432), np.float64(0.6344364298235626), np.float64(0.6359984354297931), np.float64(0.6373268930284478), np.float64(0.6340214800263321), np.float64(0.6354946444664128), np.float64(0.6367987902450108), np.float64(0.6345639703856365), np.float64(0.6340497111037819), np.float64(0.6355633012740587), np.float64(0.6366978114749299), np.float64(0.6381397420322771), np.float64(0.6382960413969502), np.float64(0.6354205757322426), np.float64(0.6369025461466085), np.float64(0.6365845216154268), np.float64(0.6353862386652515), np.float64(0.6354871707928195), np.float64(0.6340098368613234), np.float64(0.6343376448457416), np.float64(0.6354184822842591), np.float64(0.6334103409031314), np.float64(0.6339902484564494), np.float64(0.6353858417615517), np.float64(0.6330591855683981), np.float64(0.6330297116394223), np.float64(0.6327523054850591), np.float64(0.6339234512468827), np.float64(0.6337503711372643), np.float64(0.635010020502602), np.float64(0.6362016716449813), np.float64(0.6355669880999563), np.float64(0.6331171892998865)]</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 9, 10, 11, 12, 12, 13, 13, 14, 14, 15, 15, 16, 16, 16, 16, 16, 16, 16, 17, 17, 18, 18, 19, 19, 20, 21, 22, 22, 22, 22, 22, 22, 22, 23, 23, 24, 24, 24, 24, 24, 24, 24, 24, 24, 24, 24, 24, 24, 24, 24, 24, 24, 24, 24, 24, 25, 25, 26, 26, 26, 26, 26, 26, 26, 26, 26, 27, 28, 29, 29, 29, 29, 29, 29, 29, 30, 30, 30, 30, 30, 30, 30, 30, 31, 32, 32, 32, 32, 32, 32, 32, 32, 32, 32, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 33, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 34, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35, 35]</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>